<commit_message>
Auto commit - 08011727
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$8</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-01  )</t>
   </si>
@@ -215,6 +215,126 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>1D148114080101</t>
+  </si>
+  <si>
+    <t>D148</t>
+  </si>
+  <si>
+    <t>新莊福營店</t>
+  </si>
+  <si>
+    <t>新北市新莊區</t>
+  </si>
+  <si>
+    <t>2025-08-01 11:09:15</t>
+  </si>
+  <si>
+    <t>星期五</t>
+  </si>
+  <si>
+    <t>HL24</t>
+  </si>
+  <si>
+    <t>HL-SC主機</t>
+  </si>
+  <si>
+    <t>滑鼠故障無作用</t>
+  </si>
+  <si>
+    <t>門市反應sc滑鼠左鍵卡鍵時常點了無反應貨卡頓....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D148</t>
+  </si>
+  <si>
+    <t>湯家瑋</t>
+  </si>
+  <si>
+    <t>2025-08-01 11:10:03</t>
+  </si>
+  <si>
+    <t>2025-08-01 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 12:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-04 15:10:00</t>
+  </si>
+  <si>
+    <t>更換滑鼠</t>
+  </si>
+  <si>
+    <t>服務</t>
+  </si>
+  <si>
+    <t>三重三文店</t>
+  </si>
+  <si>
+    <t>THILF04586</t>
+  </si>
+  <si>
+    <t>2025-08-01 14:02:17</t>
+  </si>
+  <si>
+    <t>2025-08-01 13:40:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 14:01:00</t>
+  </si>
+  <si>
+    <t>PMQ3</t>
+  </si>
+  <si>
+    <t>北縣天龍店</t>
+  </si>
+  <si>
+    <t>THILF03840</t>
+  </si>
+  <si>
+    <t>2025-08-01 14:22:44</t>
+  </si>
+  <si>
+    <t>2025-08-01 14:07:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 14:22:00</t>
+  </si>
+  <si>
+    <t>三重仁義店</t>
+  </si>
+  <si>
+    <t>THILF04241</t>
+  </si>
+  <si>
+    <t>2025-08-01 15:06:47</t>
+  </si>
+  <si>
+    <t>2025-08-01 14:45:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 15:06:00</t>
+  </si>
+  <si>
+    <t>D346</t>
+  </si>
+  <si>
+    <t>三重維德店</t>
+  </si>
+  <si>
+    <t>THILF0D346</t>
+  </si>
+  <si>
+    <t>2025-08-01 15:48:50</t>
+  </si>
+  <si>
+    <t>2025-08-01 15:25:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 15:48:00</t>
   </si>
 </sst>
 </file>
@@ -294,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -307,6 +427,9 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
@@ -318,6 +441,12 @@
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,10 +748,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK3"/>
+  <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,7 +813,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="5"/>
+      <c r="P1" s="6"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
@@ -697,7 +826,7 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
-      <c r="AC1" s="5"/>
+      <c r="AC1" s="6"/>
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
@@ -821,99 +950,504 @@
       </c>
     </row>
     <row r="3" spans="1:37">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>2025073935</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>4804</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="7">
         <v>5903</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="T3" s="6">
+      <c r="T3" s="7">
         <v>1</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Y3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="Z3" s="6">
+      <c r="Z3" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6" t="s">
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC3" s="7" t="s">
+      <c r="AC3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6" t="s">
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2025080035</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="3">
+        <v>2403</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T4" s="3">
+        <v>1</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2025080098</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7">
+        <v>4586</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T5" s="7">
+        <v>1</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2025080101</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>3840</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T6" s="3">
+        <v>1</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC6" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2025080112</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7">
+        <v>4241</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T7" s="7">
+        <v>1</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2025080131</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T8" s="3">
+        <v>1</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08051556
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$24</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="190">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-04  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="227">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-05  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -563,6 +563,53 @@
     <t>已將錢櫃線接至主機端，請門市人員觀察狀況</t>
   </si>
   <si>
+    <t>14101114080401</t>
+  </si>
+  <si>
+    <t>三重溪華店</t>
+  </si>
+  <si>
+    <t>2025-08-04 10:19:10</t>
+  </si>
+  <si>
+    <t>星期一</t>
+  </si>
+  <si>
+    <t>HLF6</t>
+  </si>
+  <si>
+    <t>HL-多卡機QP3000E</t>
+  </si>
+  <si>
+    <t>F603</t>
+  </si>
+  <si>
+    <t>無法連線</t>
+  </si>
+  <si>
+    <t>門市反應tm1多卡機(QP3000E)畫面卡在異常英文字畫面，門市已有重新拔插後方線路仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04101</t>
+  </si>
+  <si>
+    <t>2025-08-04 10:20:22</t>
+  </si>
+  <si>
+    <t>2025-08-05 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-05 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-05 14:20:00</t>
+  </si>
+  <si>
+    <t>更換多卡機
+換下8183000568
+換上8183001839</t>
+  </si>
+  <si>
     <t>2025-08-04 10:38:40</t>
   </si>
   <si>
@@ -590,9 +637,6 @@
     <t>2025-08-04 14:41:21</t>
   </si>
   <si>
-    <t>星期一</t>
-  </si>
-  <si>
     <t>HL23</t>
   </si>
   <si>
@@ -612,6 +656,76 @@
   </si>
   <si>
     <t>2025-08-05 18:43:00</t>
+  </si>
+  <si>
+    <t>14917114080401</t>
+  </si>
+  <si>
+    <t>板橋翠華店</t>
+  </si>
+  <si>
+    <t>新北市板橋區</t>
+  </si>
+  <si>
+    <t>2025-08-04 15:42:05</t>
+  </si>
+  <si>
+    <t>門市TM1熱感發票機((BSC10II))時常發生交班後第一筆交易發票完全未印出，且昨日還有發生清帳後未出Z帳條情況，確認機台未有卡紙，但此情況已造成門市作業不便，要求工程師到店查看.......還請台芝協助</t>
+  </si>
+  <si>
+    <t>THILF04917</t>
+  </si>
+  <si>
+    <t>狄澤洋</t>
+  </si>
+  <si>
+    <t>2025-08-04 15:47:51</t>
+  </si>
+  <si>
+    <t>2025-08-05 11:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-05 12:13:00</t>
+  </si>
+  <si>
+    <t>2025-08-05 19:47:00</t>
+  </si>
+  <si>
+    <t>錢箱線路換接至TCX800
+測試正常</t>
+  </si>
+  <si>
+    <t>14917114080402</t>
+  </si>
+  <si>
+    <t>2025-08-04 16:14:24</t>
+  </si>
+  <si>
+    <t>2025/8/4 (週一) 下午 04:11 總公司小晶mail:TM2(TCX800)因該門市回報中班開機的第一筆結帳未出發票情況，請到店將二台【錢箱控制線接主機位置】後觀察是否還有此情況。...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-04 16:15:19</t>
+  </si>
+  <si>
+    <t>2025-08-05 12:14:00</t>
+  </si>
+  <si>
+    <t>2025-08-05 20:15:00</t>
+  </si>
+  <si>
+    <t>2025-08-05 10:41:34</t>
+  </si>
+  <si>
+    <t>2025-08-05 10:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-05 10:41:00</t>
+  </si>
+  <si>
+    <t>2025-08-05 12:46:24</t>
+  </si>
+  <si>
+    <t>2025-08-05 12:10:00</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1139,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK19"/>
+  <dimension ref="A1:AK24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2412,38 +2526,58 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3">
-        <v>2025080425</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>151</v>
+        <v>2025080422</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="3">
+        <v>4101</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>181</v>
+      </c>
       <c r="Q16" s="3" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="R16" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T16" s="3">
         <v>1</v>
@@ -2452,15 +2586,17 @@
         <v>53</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="X16" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y16" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="Z16" s="3">
         <v>0.5</v>
       </c>
@@ -2469,11 +2605,9 @@
         <v>58</v>
       </c>
       <c r="AC16" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD16" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
@@ -2492,7 +2626,7 @@
         <v>78</v>
       </c>
       <c r="C17" s="7">
-        <v>2025080426</v>
+        <v>2025080425</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -2529,10 +2663,10 @@
         <v>53</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="W17" s="7" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="X17" s="7" t="s">
         <v>160</v>
@@ -2569,15 +2703,15 @@
         <v>78</v>
       </c>
       <c r="C18" s="3">
-        <v>2025080447</v>
+        <v>2025080426</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3">
-        <v>4154</v>
+      <c r="F18" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>153</v>
@@ -2591,7 +2725,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="3" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>51</v>
@@ -2606,13 +2740,13 @@
         <v>53</v>
       </c>
       <c r="V18" s="3" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3">
@@ -2643,58 +2777,38 @@
         <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C19" s="7">
-        <v>2025080482</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>2025080447</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="7">
-        <v>4155</v>
+        <v>4154</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="N19" s="7">
-        <v>2305</v>
-      </c>
-      <c r="O19" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="P19" s="8" t="s">
-        <v>186</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="9"/>
       <c r="Q19" s="7" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T19" s="7">
         <v>1</v>
@@ -2703,28 +2817,28 @@
         <v>53</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="W19" s="7" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="X19" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y19" s="7" t="s">
-        <v>189</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="Y19" s="7"/>
       <c r="Z19" s="7">
-        <v>1.6</v>
+        <v>0.5</v>
       </c>
       <c r="AA19" s="7"/>
       <c r="AB19" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC19" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="AD19" s="7"/>
+      <c r="AC19" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AE19" s="7"/>
       <c r="AF19" s="7"/>
       <c r="AG19" s="7"/>
@@ -2732,6 +2846,451 @@
       <c r="AI19" s="7"/>
       <c r="AJ19" s="7"/>
       <c r="AK19" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2025080482</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="3">
+        <v>4155</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="N20" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T20" s="3">
+        <v>1</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC20" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2025080521</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="7">
+        <v>4917</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T21" s="7">
+        <v>1</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y21" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z21" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC21" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD21" s="7"/>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
+      <c r="AK21" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2025080527</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="3">
+        <v>4917</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="N22" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T22" s="3">
+        <v>1</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y22" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC22" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2025080594</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7">
+        <v>4101</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T23" s="7">
+        <v>1</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7"/>
+      <c r="AK23" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2025080636</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3">
+        <v>4917</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T24" s="3">
+        <v>1</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08061651
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$25</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="241">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-06  )</t>
   </si>
@@ -726,6 +726,51 @@
   </si>
   <si>
     <t>2025-08-05 12:10:00</t>
+  </si>
+  <si>
+    <t>12014114080501</t>
+  </si>
+  <si>
+    <t>三重果菜市場</t>
+  </si>
+  <si>
+    <t>2025-08-05 14:04:16</t>
+  </si>
+  <si>
+    <t>星期二</t>
+  </si>
+  <si>
+    <t>HL25</t>
+  </si>
+  <si>
+    <t>HL-SC螢幕</t>
+  </si>
+  <si>
+    <t>螢幕畫面閃爍頻繁或無畫面</t>
+  </si>
+  <si>
+    <t>門市反應SC螢幕(LCD)黑屏顯示無訊號，PING1有通可VNC，門市已嘗試將後方線路重新拔插仍異常，門市告知非與監視器共用螢幕....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF02014</t>
+  </si>
+  <si>
+    <t>2025-08-05 14:06:46</t>
+  </si>
+  <si>
+    <t>2025-08-06 09:40:00</t>
+  </si>
+  <si>
+    <t>2025-08-06 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-06 18:06:00</t>
+  </si>
+  <si>
+    <t>螢幕測試正常，SC主機的VGA 孔位損壞，需更換主機，現場的螢幕切換器也損壞無法切換，已告知店員報修，目前將SC和螢幕直接對接使用
+更換SC主機
+換下8114003252
+換上8114004371</t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1184,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK24"/>
+  <dimension ref="A1:AK25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC21" sqref="AC21"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3245,7 +3290,7 @@
       <c r="M24" s="4"/>
       <c r="N24" s="3"/>
       <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
+      <c r="P24" s="10"/>
       <c r="Q24" s="3" t="s">
         <v>209</v>
       </c>
@@ -3278,7 +3323,7 @@
       <c r="AB24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC24" s="4" t="s">
+      <c r="AC24" s="10" t="s">
         <v>84</v>
       </c>
       <c r="AD24" s="3" t="s">
@@ -3291,6 +3336,103 @@
       <c r="AI24" s="3"/>
       <c r="AJ24" s="3"/>
       <c r="AK24" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2025080650</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="7">
+        <v>2014</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="N25" s="7">
+        <v>2501</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="P25" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T25" s="7">
+        <v>1</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V25" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="Z25" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC25" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD25" s="7"/>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7"/>
+      <c r="AJ25" s="7"/>
+      <c r="AK25" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08071742
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$35</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="241">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-06  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="317">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-07  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -771,6 +771,241 @@
 更換SC主機
 換下8114003252
 換上8114004371</t>
+  </si>
+  <si>
+    <t>14101114080601</t>
+  </si>
+  <si>
+    <t>2025-08-06 15:21:10</t>
+  </si>
+  <si>
+    <t>星期三</t>
+  </si>
+  <si>
+    <t>門市反應TM1多卡機(QP3000E)無法使用，VNC版更後操作悠遊卡機重開顯示悠遊卡通訊逾時!、操作一卡通開機顯示0801錯誤訊息:...、操作iCash愛金卡手動開機授權顯示代碼:20C...，門市告知8/5工程師有到店更換過設備，今日再度無法使用..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-06 15:23:55</t>
+  </si>
+  <si>
+    <t>2025-08-07 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 09:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 19:23:00</t>
+  </si>
+  <si>
+    <t>更換變壓器
+目前測試皆為正常，重新開機測試也正常</t>
+  </si>
+  <si>
+    <t>E4046114080701</t>
+  </si>
+  <si>
+    <t>板橋福康店</t>
+  </si>
+  <si>
+    <t>2025-08-07 07:48:19</t>
+  </si>
+  <si>
+    <t>凌晨</t>
+  </si>
+  <si>
+    <t>F604</t>
+  </si>
+  <si>
+    <t>無電源反應</t>
+  </si>
+  <si>
+    <t>門市反應tm2多卡機(QP3000E)無畫面無電源反應，門市重插後方線路仍異常....須請台芝到店協助(多卡機螢幕沒有畫面(靠近電話這台))</t>
+  </si>
+  <si>
+    <t>THILF04046</t>
+  </si>
+  <si>
+    <t>2025-08-07 09:06:39</t>
+  </si>
+  <si>
+    <t>2025-08-07 15:16:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 15:42:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 13:06:00</t>
+  </si>
+  <si>
+    <t>更換QP3000
+換上：8183003279
+換下：8183001981</t>
+  </si>
+  <si>
+    <t>13890114080701</t>
+  </si>
+  <si>
+    <t>三重美堤店</t>
+  </si>
+  <si>
+    <t>2025-08-07 09:12:52</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)抽屜打不開，抽屜外觀白/鑰匙孔右邊/鑰匙孔編號719，已將發票機關機紙捲重裝仍異常，門市告知疑似線路被老鼠咬斷...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03890</t>
+  </si>
+  <si>
+    <t>2025-08-07 09:15:05</t>
+  </si>
+  <si>
+    <t>2025-08-07 10:54:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 11:24:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 13:15:00</t>
+  </si>
+  <si>
+    <t>更換錢箱線</t>
+  </si>
+  <si>
+    <t>15384114080701</t>
+  </si>
+  <si>
+    <t>板橋民生站</t>
+  </si>
+  <si>
+    <t>2025-08-07 10:17:04</t>
+  </si>
+  <si>
+    <t>HL60</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET印票機L90</t>
+  </si>
+  <si>
+    <t>門市反應印票機L90 paper燈號亮紅燈，但列印測試票券正常，關機紙捲重裝後紅燈仍恆亮，門市反應因票券機時常有狀況不能列印，需求請工程師到店檢查設備...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05384</t>
+  </si>
+  <si>
+    <t>2025-08-07 10:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 14:23:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 15:10:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 14:20:00</t>
+  </si>
+  <si>
+    <t>原店內印票機測試正常，更換設備供門市測試
+更換印票機
+換上：8139002712
+換下：8139003247</t>
+  </si>
+  <si>
+    <t>15352114080701</t>
+  </si>
+  <si>
+    <t>三重重陽店</t>
+  </si>
+  <si>
+    <t>2025-08-07 10:09:31</t>
+  </si>
+  <si>
+    <t>HLM3</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET 標籤印表機</t>
+  </si>
+  <si>
+    <t>M302</t>
+  </si>
+  <si>
+    <t>印字不清</t>
+  </si>
+  <si>
+    <t>MMK標籤印表機-消費者操作MMK列印EC寄件單，印出後寄件人取件人欄位都為空白，經測試其他門市列印此寄件單並無異常，請門市協助執行測試也是一樣寄件人取件人欄位都為空白
+與店長確認此狀況近幾天才開始發生</t>
+  </si>
+  <si>
+    <t>THILF05352</t>
+  </si>
+  <si>
+    <t>2025-08-07 10:30:24</t>
+  </si>
+  <si>
+    <t>2025-08-07 13:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 13:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 14:30:00</t>
+  </si>
+  <si>
+    <t>重新下載文字檔案測試，寄件人和取件人列印都有出現</t>
+  </si>
+  <si>
+    <t>北縣莊玲店</t>
+  </si>
+  <si>
+    <t>THILF03052</t>
+  </si>
+  <si>
+    <t>2025-08-07 12:10:17</t>
+  </si>
+  <si>
+    <t>2025-08-07 11:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 12:10:00</t>
+  </si>
+  <si>
+    <t>新莊祐信店</t>
+  </si>
+  <si>
+    <t>THILF04025</t>
+  </si>
+  <si>
+    <t>2025-08-07 13:15:49</t>
+  </si>
+  <si>
+    <t>2025-08-07 13:00:00</t>
+  </si>
+  <si>
+    <t>新莊中泉店</t>
+  </si>
+  <si>
+    <t>THILF04163</t>
+  </si>
+  <si>
+    <t>2025-08-07 13:42:43</t>
+  </si>
+  <si>
+    <t>2025-08-07 13:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 15:16:46</t>
+  </si>
+  <si>
+    <t>EDC</t>
+  </si>
+  <si>
+    <t>2025-08-07 15:47:09</t>
+  </si>
+  <si>
+    <t>2025-08-07 15:24:00</t>
+  </si>
+  <si>
+    <t>2025-08-07 15:45:00</t>
   </si>
 </sst>
 </file>
@@ -1184,10 +1419,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK25"/>
+  <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3385,7 +3620,7 @@
       <c r="O25" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="P25" s="8" t="s">
+      <c r="P25" s="9" t="s">
         <v>234</v>
       </c>
       <c r="Q25" s="7" t="s">
@@ -3422,7 +3657,7 @@
       <c r="AB25" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC25" s="8" t="s">
+      <c r="AC25" s="9" t="s">
         <v>240</v>
       </c>
       <c r="AD25" s="7"/>
@@ -3433,6 +3668,876 @@
       <c r="AI25" s="7"/>
       <c r="AJ25" s="7"/>
       <c r="AK25" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2025080821</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="3">
+        <v>4101</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T26" s="3">
+        <v>1</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC26" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="7">
+        <v>2025080889</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="7">
+        <v>4046</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y27" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z27" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC27" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD27" s="7"/>
+      <c r="AE27" s="7"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="7"/>
+      <c r="AK27" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2025080892</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="3">
+        <v>3890</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="N28" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P28" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T28" s="3">
+        <v>1</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y28" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC28" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37">
+      <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2025080946</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="7">
+        <v>5384</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="N29" s="7">
+        <v>6003</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T29" s="7">
+        <v>1</v>
+      </c>
+      <c r="U29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="Y29" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="Z29" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC29" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="AD29" s="7"/>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="7"/>
+      <c r="AH29" s="7"/>
+      <c r="AI29" s="7"/>
+      <c r="AJ29" s="7"/>
+      <c r="AK29" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2025080953</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="3">
+        <v>5352</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="P30" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T30" s="3">
+        <v>1</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V30" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y30" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC30" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37">
+      <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="7">
+        <v>2025081004</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7">
+        <v>3052</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="R31" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T31" s="7">
+        <v>1</v>
+      </c>
+      <c r="U31" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V31" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="W31" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="X31" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC31" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
+      <c r="AJ31" s="7"/>
+      <c r="AK31" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2025081012</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>4025</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T32" s="3">
+        <v>1</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC32" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="7">
+        <v>2025081016</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7">
+        <v>4163</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T33" s="7">
+        <v>1</v>
+      </c>
+      <c r="U33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC33" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7"/>
+      <c r="AK33" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2025081053</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3">
+        <v>5384</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T34" s="3">
+        <v>1</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC34" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK34" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37">
+      <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2025081062</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7">
+        <v>4046</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="R35" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T35" s="7">
+        <v>1</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC35" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
+      <c r="AJ35" s="7"/>
+      <c r="AK35" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08081714
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$43</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="317">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-07  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="369">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-08  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -969,6 +969,38 @@
     <t>2025-08-07 12:10:00</t>
   </si>
   <si>
+    <t>13741114080702</t>
+  </si>
+  <si>
+    <t>三重重新三</t>
+  </si>
+  <si>
+    <t>2025-08-07 13:07:51</t>
+  </si>
+  <si>
+    <t>tm2 ccd掃描器(HC76-TR)-門市反應TM2清帳後會跳出:COMPORT偵測異常，請按[清除]後，退到登入頁面，按下[版本更新]，自動重啟系統，或撥打0800客服報修11111，都需再版更後才會正常，門市告知這幾天發生頻繁，hipos與開發確認，顯示COMPORT偵測異常，請按[清除]後判斷為掃描槍問題。頻繁發生建議轉派台芝到店檢查CCD相關設備及線路。...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03741</t>
+  </si>
+  <si>
+    <t>2025-08-07 13:10:07</t>
+  </si>
+  <si>
+    <t>2025-08-08 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 10:12:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 17:10:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119011532
+換上8119011671</t>
+  </si>
+  <si>
     <t>新莊祐信店</t>
   </si>
   <si>
@@ -1006,6 +1038,137 @@
   </si>
   <si>
     <t>2025-08-07 15:45:00</t>
+  </si>
+  <si>
+    <t>14101114080701</t>
+  </si>
+  <si>
+    <t>2025-08-07 16:34:04</t>
+  </si>
+  <si>
+    <t>門市反應今日工程師有到店協助，但TM1多卡機(QP3000E)仍無法使用，查詢餘額顯示悠遊卡通訊逾時!，於TM2測試則正常，TM1已協助點選版更&gt;悠遊卡機重開仍顯示悠遊卡通訊逾時!...請台芝到店協助
+08/05 案14101114080401，台芝到店更換多卡機
+08/07 案14101114080601，台芝到店更換變壓器，並回覆目前測試皆為正常，重新開機測試也正常</t>
+  </si>
+  <si>
+    <t>2025-08-07 16:39:26</t>
+  </si>
+  <si>
+    <t>2025-08-08 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 12:40:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 20:39:00</t>
+  </si>
+  <si>
+    <t>更換多卡機
+換下8183001839
+換上8183003229
+將TM1和TM2交換對接做卡機測試，比且等待店家交班及清帳後再次測試確認，目前都可以進行讀卡的動作，請店家在進行觀察</t>
+  </si>
+  <si>
+    <t>14856114080701</t>
+  </si>
+  <si>
+    <t>新莊小胖店</t>
+  </si>
+  <si>
+    <t>2025-08-07 20:44:30</t>
+  </si>
+  <si>
+    <t>夜間</t>
+  </si>
+  <si>
+    <t>空白列印/印一半/未列印</t>
+  </si>
+  <si>
+    <t>門市告知TM1熱感發票機(BSC10II)結帳兩筆都列印空白發票，已有將發票機關機重開更換新紙捲，門市告知紙捲裝正確，請門市點選點餐紙仍列印空白...還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04856</t>
+  </si>
+  <si>
+    <t>2025-08-07 20:53:59</t>
+  </si>
+  <si>
+    <t>2025-08-08 08:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 08:45:00</t>
+  </si>
+  <si>
+    <t>2025-08-11 00:54:00</t>
+  </si>
+  <si>
+    <t>取消叫修</t>
+  </si>
+  <si>
+    <t>客戶取消</t>
+  </si>
+  <si>
+    <t>D022</t>
+  </si>
+  <si>
+    <t>三重溪尾店</t>
+  </si>
+  <si>
+    <t>THILF0D022</t>
+  </si>
+  <si>
+    <t>2025-08-08 14:50:45</t>
+  </si>
+  <si>
+    <t>2025-08-08 14:00:00</t>
+  </si>
+  <si>
+    <t>D057</t>
+  </si>
+  <si>
+    <t>北縣溪尾二店</t>
+  </si>
+  <si>
+    <t>THILF0D057</t>
+  </si>
+  <si>
+    <t>2025-08-08 14:52:21</t>
+  </si>
+  <si>
+    <t>2025-08-08 14:51:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 14:58:53</t>
+  </si>
+  <si>
+    <t>三重美溪店</t>
+  </si>
+  <si>
+    <t>THILF03772</t>
+  </si>
+  <si>
+    <t>2025-08-08 15:48:24</t>
+  </si>
+  <si>
+    <t>2025-08-08 15:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 15:46:00</t>
+  </si>
+  <si>
+    <t>三重義天店</t>
+  </si>
+  <si>
+    <t>THILF02222</t>
+  </si>
+  <si>
+    <t>2025-08-08 17:05:15</t>
+  </si>
+  <si>
+    <t>2025-08-08 16:39:00</t>
+  </si>
+  <si>
+    <t>2025-08-08 17:04:00</t>
   </si>
 </sst>
 </file>
@@ -1419,10 +1582,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK35"/>
+  <dimension ref="A1:AK43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4238,38 +4401,58 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C32" s="3">
-        <v>2025081012</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+        <v>2025081011</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F32" s="3">
-        <v>4025</v>
+        <v>3741</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P32" s="10" t="s">
+        <v>307</v>
+      </c>
       <c r="Q32" s="3" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="R32" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T32" s="3">
         <v>1</v>
@@ -4278,28 +4461,28 @@
         <v>53</v>
       </c>
       <c r="V32" s="3" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="W32" s="3" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="X32" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="Y32" s="3"/>
+        <v>311</v>
+      </c>
+      <c r="Y32" s="3" t="s">
+        <v>312</v>
+      </c>
       <c r="Z32" s="3">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="AA32" s="3"/>
       <c r="AB32" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC32" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD32" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
@@ -4318,15 +4501,15 @@
         <v>78</v>
       </c>
       <c r="C33" s="7">
-        <v>2025081016</v>
+        <v>2025081012</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7">
-        <v>4163</v>
+        <v>4025</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>64</v>
@@ -4340,7 +4523,7 @@
       <c r="O33" s="8"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="7" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>51</v>
@@ -4355,13 +4538,13 @@
         <v>53</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="W33" s="7" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="X33" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Y33" s="7"/>
       <c r="Z33" s="7">
@@ -4395,18 +4578,18 @@
         <v>78</v>
       </c>
       <c r="C34" s="3">
-        <v>2025081053</v>
+        <v>2025081016</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3">
-        <v>5384</v>
+        <v>4163</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>206</v>
+        <v>64</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -4417,13 +4600,13 @@
       <c r="O34" s="4"/>
       <c r="P34" s="10"/>
       <c r="Q34" s="3" t="s">
-        <v>279</v>
+        <v>319</v>
       </c>
       <c r="R34" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>210</v>
+        <v>72</v>
       </c>
       <c r="T34" s="3">
         <v>1</v>
@@ -4432,34 +4615,34 @@
         <v>53</v>
       </c>
       <c r="V34" s="3" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>281</v>
+        <v>321</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="Y34" s="3"/>
       <c r="Z34" s="3">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="AA34" s="3"/>
       <c r="AB34" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC34" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="AD34" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="AD34" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AE34" s="3"/>
       <c r="AF34" s="3"/>
       <c r="AG34" s="3"/>
       <c r="AH34" s="3"/>
       <c r="AI34" s="3"/>
-      <c r="AJ34" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ34" s="3"/>
       <c r="AK34" s="3" t="s">
         <v>60</v>
       </c>
@@ -4472,15 +4655,15 @@
         <v>78</v>
       </c>
       <c r="C35" s="7">
-        <v>2025081062</v>
+        <v>2025081053</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7">
-        <v>4046</v>
+        <v>5384</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>206</v>
@@ -4492,9 +4675,9 @@
       <c r="M35" s="8"/>
       <c r="N35" s="7"/>
       <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
+      <c r="P35" s="9"/>
       <c r="Q35" s="7" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>51</v>
@@ -4509,35 +4692,691 @@
         <v>53</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="W35" s="7" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
       <c r="X35" s="7" t="s">
-        <v>316</v>
+        <v>282</v>
       </c>
       <c r="Y35" s="7"/>
       <c r="Z35" s="7">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="AA35" s="7"/>
       <c r="AB35" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC35" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD35" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC35" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="AD35" s="7"/>
       <c r="AE35" s="7"/>
       <c r="AF35" s="7"/>
       <c r="AG35" s="7"/>
       <c r="AH35" s="7"/>
       <c r="AI35" s="7"/>
-      <c r="AJ35" s="7"/>
+      <c r="AJ35" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AK35" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2025081062</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <v>4046</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T36" s="3">
+        <v>1</v>
+      </c>
+      <c r="U36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V36" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="W36" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="X36" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC36" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+      <c r="AG36" s="3"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3"/>
+      <c r="AK36" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37">
+      <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2025081073</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="7">
+        <v>4101</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="M37" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="O37" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="P37" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q37" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="R37" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T37" s="7">
+        <v>1</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="X37" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="Y37" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="Z37" s="7">
+        <v>2.2</v>
+      </c>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC37" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="AD37" s="7"/>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7"/>
+      <c r="AK37" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2025081108</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="3">
+        <v>4856</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="P38" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T38" s="3">
+        <v>1</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V38" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="Y38" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="Z38" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="AC38" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="3"/>
+      <c r="AG38" s="3"/>
+      <c r="AH38" s="3"/>
+      <c r="AI38" s="3"/>
+      <c r="AJ38" s="3"/>
+      <c r="AK38" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="7">
+        <v>2025081193</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="R39" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T39" s="7">
+        <v>1</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V39" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="W39" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="X39" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC39" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD39" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE39" s="7"/>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
+      <c r="AJ39" s="7"/>
+      <c r="AK39" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2025081194</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T40" s="3">
+        <v>1</v>
+      </c>
+      <c r="U40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V40" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="X40" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC40" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="3"/>
+      <c r="AG40" s="3"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="3"/>
+      <c r="AJ40" s="3"/>
+      <c r="AK40" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37">
+      <c r="A41" s="7">
+        <v>39</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="7">
+        <v>2025081196</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="R41" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T41" s="7">
+        <v>1</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V41" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="W41" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="X41" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA41" s="7"/>
+      <c r="AB41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC41" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD41" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE41" s="7"/>
+      <c r="AF41" s="7"/>
+      <c r="AG41" s="7"/>
+      <c r="AH41" s="7"/>
+      <c r="AI41" s="7"/>
+      <c r="AJ41" s="7"/>
+      <c r="AK41" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2025081215</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3">
+        <v>3772</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T42" s="3">
+        <v>1</v>
+      </c>
+      <c r="U42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V42" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="W42" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="X42" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC42" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE42" s="3"/>
+      <c r="AF42" s="3"/>
+      <c r="AG42" s="3"/>
+      <c r="AH42" s="3"/>
+      <c r="AI42" s="3"/>
+      <c r="AJ42" s="3"/>
+      <c r="AK42" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37">
+      <c r="A43" s="7">
+        <v>41</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="7">
+        <v>2025081220</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7">
+        <v>2222</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="R43" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T43" s="7">
+        <v>1</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V43" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="W43" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="X43" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y43" s="7"/>
+      <c r="Z43" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC43" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD43" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE43" s="7"/>
+      <c r="AF43" s="7"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7"/>
+      <c r="AJ43" s="7"/>
+      <c r="AK43" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08121105
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$47</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="369">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-08  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="408">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-12  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1138,6 +1138,42 @@
     <t>2025-08-08 14:51:00</t>
   </si>
   <si>
+    <t>14541114080802</t>
+  </si>
+  <si>
+    <t>淡水海天店</t>
+  </si>
+  <si>
+    <t>新北市淡水區</t>
+  </si>
+  <si>
+    <t>2025-08-08 14:46:22</t>
+  </si>
+  <si>
+    <t>客顯示器畫面不正常</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)客顯畫面全黑，確認右下角燈號藍燈，客服查看畫面正常，已協助重啟TM仍異常...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04541</t>
+  </si>
+  <si>
+    <t>2025-08-08 14:52:49</t>
+  </si>
+  <si>
+    <t>2025-08-11 15:27:00</t>
+  </si>
+  <si>
+    <t>2025-08-11 15:57:00</t>
+  </si>
+  <si>
+    <t>2025-08-11 18:52:00</t>
+  </si>
+  <si>
+    <t>重新插拔客顯USB，重開機後正常</t>
+  </si>
+  <si>
     <t>2025-08-08 14:58:53</t>
   </si>
   <si>
@@ -1169,6 +1205,90 @@
   </si>
   <si>
     <t>2025-08-08 17:04:00</t>
+  </si>
+  <si>
+    <t>14528114081101</t>
+  </si>
+  <si>
+    <t>急修件</t>
+  </si>
+  <si>
+    <t>八里鐵塔店</t>
+  </si>
+  <si>
+    <t>新北市八里區</t>
+  </si>
+  <si>
+    <t>2025-08-11 09:29:12</t>
+  </si>
+  <si>
+    <t>檔案損毀(更換硬碟)</t>
+  </si>
+  <si>
+    <t>08/11 09:49 啟動緊急叫修:門市反應使用HI SHOP當前系統異常，請通知門市人員或重新操作，VNC重啟HISHOP仍無法開啟程式，登入最高權限&gt;執行GetNewHiShop仍異常，開訂貨3.0顯示TM_ORDER\'應用程式中發生伺服器錯誤異常。總公司功評告知:SC主機ADATA SU800\\\\.\\PHYSICALDRIVE0  256055869440 已重試磁碟 0 (PDO 名稱: \\Device\\00000034) 邏輯區塊位址 0x1556e0 上的 IO 操作。第一顆硬碟異常，請派工更換不備份還原。...請台芝到店協助 
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認帳務做到08/10，與通訊圭連確認有收到08/10的銷售
+08/01  09:33  已通知總公司功評協助確認...廖</t>
+  </si>
+  <si>
+    <t>THILF04528</t>
+  </si>
+  <si>
+    <t>2025-08-11 09:52:50</t>
+  </si>
+  <si>
+    <t>2025-08-11 10:40:00</t>
+  </si>
+  <si>
+    <t>2025-08-11 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-11 15:52:00</t>
+  </si>
+  <si>
+    <t>更換第一顆硬碟不備份還原完成</t>
+  </si>
+  <si>
+    <t>2025-08-11 16:00:24</t>
+  </si>
+  <si>
+    <t>2025-08-11 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-11 15:59:00</t>
+  </si>
+  <si>
+    <t>12267114081101</t>
+  </si>
+  <si>
+    <t>北縣金陽店</t>
+  </si>
+  <si>
+    <t>新北市金山區</t>
+  </si>
+  <si>
+    <t>2025-08-11 15:55:53</t>
+  </si>
+  <si>
+    <t>08/11 16:01總公司明翰來信啟動緊急叫修:總公司通訊健誌副理來信:目前門市的銷售引擎已經在8/11早上就停止運作，請安排到店更換SC的第二顆硬碟。請協助派工2267北縣金陽店，2025/8/11 (週一) 下午 03:52總公司明翰來信:到店更換SC第二顆硬碟不備份還原。請啟動緊急叫修，謝謝。...請台芝到店協助 
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認帳務做到08/11，與通訊圭連確認有收到08/11的銷售但缺少tm1、2電子存根聯</t>
+  </si>
+  <si>
+    <t>THILF02267</t>
+  </si>
+  <si>
+    <t>2025-08-11 16:03:56</t>
+  </si>
+  <si>
+    <t>2025-08-11 18:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-11 20:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 09:03:00</t>
+  </si>
+  <si>
+    <t>更換第二顆硬碟不備份還原完成</t>
   </si>
 </sst>
 </file>
@@ -1582,10 +1702,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK43"/>
+  <dimension ref="A1:AK47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5154,32 +5274,52 @@
         <v>39</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C41" s="7">
-        <v>2025081196</v>
-      </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7" t="s">
-        <v>348</v>
+        <v>2025081195</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="7">
+        <v>4541</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="9"/>
+        <v>360</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M41" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N41" s="7">
+        <v>2302</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="P41" s="9" t="s">
+        <v>363</v>
+      </c>
       <c r="Q41" s="7" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="R41" s="7" t="s">
         <v>51</v>
@@ -5194,28 +5334,28 @@
         <v>53</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="W41" s="7" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="X41" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="Y41" s="7"/>
+        <v>367</v>
+      </c>
+      <c r="Y41" s="7" t="s">
+        <v>368</v>
+      </c>
       <c r="Z41" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA41" s="7"/>
       <c r="AB41" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC41" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD41" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="AD41" s="7"/>
       <c r="AE41" s="7"/>
       <c r="AF41" s="7"/>
       <c r="AG41" s="7"/>
@@ -5234,15 +5374,15 @@
         <v>78</v>
       </c>
       <c r="C42" s="3">
-        <v>2025081215</v>
+        <v>2025081196</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="3">
-        <v>3772</v>
+      <c r="F42" s="3" t="s">
+        <v>348</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>42</v>
@@ -5256,7 +5396,7 @@
       <c r="O42" s="4"/>
       <c r="P42" s="10"/>
       <c r="Q42" s="3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="R42" s="3" t="s">
         <v>51</v>
@@ -5271,17 +5411,17 @@
         <v>53</v>
       </c>
       <c r="V42" s="3" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="W42" s="3" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="X42" s="3" t="s">
-        <v>363</v>
+        <v>283</v>
       </c>
       <c r="Y42" s="3"/>
       <c r="Z42" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA42" s="3"/>
       <c r="AB42" s="3" t="s">
@@ -5311,15 +5451,15 @@
         <v>78</v>
       </c>
       <c r="C43" s="7">
-        <v>2025081220</v>
+        <v>2025081215</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7">
-        <v>2222</v>
+        <v>3772</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>42</v>
@@ -5331,9 +5471,9 @@
       <c r="M43" s="8"/>
       <c r="N43" s="7"/>
       <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
+      <c r="P43" s="9"/>
       <c r="Q43" s="7" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="R43" s="7" t="s">
         <v>51</v>
@@ -5348,13 +5488,13 @@
         <v>53</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="W43" s="7" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="X43" s="7" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="Y43" s="7"/>
       <c r="Z43" s="7">
@@ -5364,7 +5504,7 @@
       <c r="AB43" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC43" s="8" t="s">
+      <c r="AC43" s="9" t="s">
         <v>84</v>
       </c>
       <c r="AD43" s="7" t="s">
@@ -5377,6 +5517,354 @@
       <c r="AI43" s="7"/>
       <c r="AJ43" s="7"/>
       <c r="AK43" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2025081220</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3">
+        <v>2222</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T44" s="3">
+        <v>1</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V44" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="W44" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="X44" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC44" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE44" s="3"/>
+      <c r="AF44" s="3"/>
+      <c r="AG44" s="3"/>
+      <c r="AH44" s="3"/>
+      <c r="AI44" s="3"/>
+      <c r="AJ44" s="3"/>
+      <c r="AK44" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37">
+      <c r="A45" s="7">
+        <v>43</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2025081296</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="F45" s="7">
+        <v>4528</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M45" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N45" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O45" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="P45" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q45" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="R45" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T45" s="7">
+        <v>1</v>
+      </c>
+      <c r="U45" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V45" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="W45" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="X45" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="Y45" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="Z45" s="7">
+        <v>3.8</v>
+      </c>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC45" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AD45" s="7"/>
+      <c r="AE45" s="7"/>
+      <c r="AF45" s="7"/>
+      <c r="AG45" s="7"/>
+      <c r="AH45" s="7"/>
+      <c r="AI45" s="7"/>
+      <c r="AJ45" s="7"/>
+      <c r="AK45" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2025081374</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3">
+        <v>4541</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T46" s="3">
+        <v>1</v>
+      </c>
+      <c r="U46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V46" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="W46" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="X46" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC46" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE46" s="3"/>
+      <c r="AF46" s="3"/>
+      <c r="AG46" s="3"/>
+      <c r="AH46" s="3"/>
+      <c r="AI46" s="3"/>
+      <c r="AJ46" s="3"/>
+      <c r="AK46" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37">
+      <c r="A47" s="7">
+        <v>45</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="7">
+        <v>2025081377</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="F47" s="7">
+        <v>2267</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N47" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O47" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="P47" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q47" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T47" s="7">
+        <v>1</v>
+      </c>
+      <c r="U47" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V47" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="W47" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="X47" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="Y47" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="Z47" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC47" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="AD47" s="7"/>
+      <c r="AE47" s="7"/>
+      <c r="AF47" s="7"/>
+      <c r="AG47" s="7"/>
+      <c r="AH47" s="7"/>
+      <c r="AI47" s="7"/>
+      <c r="AJ47" s="7"/>
+      <c r="AK47" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08121410
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$53</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="449">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-12  )</t>
   </si>
@@ -1248,6 +1248,93 @@
     <t>更換第一顆硬碟不備份還原完成</t>
   </si>
   <si>
+    <t>13416114081101</t>
+  </si>
+  <si>
+    <t>板橋國慶店</t>
+  </si>
+  <si>
+    <t>2025-08-11 10:00:23</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)抽屜常常打不開，有打開的聲響但未彈出，門市已將發票機重開仍無改善，抽屜外觀白/鑰匙孔中間/鑰匙孔無編號...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03416</t>
+  </si>
+  <si>
+    <t>2025-08-11 10:13:03</t>
+  </si>
+  <si>
+    <t>2025-08-12 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 12:55:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 14:13:00</t>
+  </si>
+  <si>
+    <t>更換錢箱
+換上：81Z1004477
+換下：81Z1001049</t>
+  </si>
+  <si>
+    <t>13362114081101</t>
+  </si>
+  <si>
+    <t>北縣重武店</t>
+  </si>
+  <si>
+    <t>2025-08-11 13:48:17</t>
+  </si>
+  <si>
+    <t>門市反應TM1-CCD掃描器(HC56II-TR)刷讀所有條碼都感應不良，有亮燈有嗶聲但無入TM，已嘗試執行掃描器校正仍無改善..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03362</t>
+  </si>
+  <si>
+    <t>2025-08-11 13:49:35</t>
+  </si>
+  <si>
+    <t>2025-08-12 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 12:36:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 17:49:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119007651
+換上8119011857</t>
+  </si>
+  <si>
+    <t>13362114081102</t>
+  </si>
+  <si>
+    <t>2025-08-11 13:49:47</t>
+  </si>
+  <si>
+    <t>門市反應TM2-CCD掃描器(HC56II-TR)刷讀所有條碼都感應不良，有亮燈有嗶聲但無入TM，已嘗試執行掃描器校正仍無改善..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-11 13:50:15</t>
+  </si>
+  <si>
+    <t>2025-08-12 12:33:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 17:50:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119008618
+換上8119010761</t>
+  </si>
+  <si>
     <t>2025-08-11 16:00:24</t>
   </si>
   <si>
@@ -1289,6 +1376,48 @@
   </si>
   <si>
     <t>更換第二顆硬碟不備份還原完成</t>
+  </si>
+  <si>
+    <t>15352114081101</t>
+  </si>
+  <si>
+    <t>2025-08-11 17:31:21</t>
+  </si>
+  <si>
+    <t>門市反應tm2近期交班大夜後的第一筆交易容易發生未出發票異狀，當下設備燈號正常，門市已有將發票機重裝紙捲重開機過但此狀況仍會發生，發票機為二代（BSC10II），經hipos查看:Eventlog無異常，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。</t>
+  </si>
+  <si>
+    <t>2025-08-11 17:32:17</t>
+  </si>
+  <si>
+    <t>2025-08-12 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 13:48:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 21:32:00</t>
+  </si>
+  <si>
+    <t>現場將錢櫃線轉接至TM主機上，比且請騰雲安裝驅動完成，請門市人員在進行觀察</t>
+  </si>
+  <si>
+    <t>2025-08-12 12:54:44</t>
+  </si>
+  <si>
+    <t>板橋玉川店</t>
+  </si>
+  <si>
+    <t>THILF03977</t>
+  </si>
+  <si>
+    <t>2025-08-12 13:24:09</t>
+  </si>
+  <si>
+    <t>2025-08-12 13:05:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 13:20:00</t>
   </si>
 </sst>
 </file>
@@ -1702,10 +1831,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK47"/>
+  <dimension ref="A1:AK53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5699,38 +5828,58 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C46" s="3">
-        <v>2025081374</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+        <v>2025081304</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F46" s="3">
-        <v>4541</v>
+        <v>3416</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>359</v>
+        <v>395</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="10"/>
+        <v>206</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="N46" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P46" s="10" t="s">
+        <v>397</v>
+      </c>
       <c r="Q46" s="3" t="s">
-        <v>364</v>
+        <v>398</v>
       </c>
       <c r="R46" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="T46" s="3">
         <v>1</v>
@@ -5739,28 +5888,28 @@
         <v>53</v>
       </c>
       <c r="V46" s="3" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="W46" s="3" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="X46" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="Y46" s="3"/>
+        <v>401</v>
+      </c>
+      <c r="Y46" s="3" t="s">
+        <v>402</v>
+      </c>
       <c r="Z46" s="3">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="AA46" s="3"/>
       <c r="AB46" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC46" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD46" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>403</v>
+      </c>
+      <c r="AD46" s="3"/>
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
       <c r="AG46" s="3"/>
@@ -5779,25 +5928,25 @@
         <v>38</v>
       </c>
       <c r="C47" s="7">
-        <v>2025081377</v>
+        <v>2025081343</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>382</v>
+        <v>40</v>
       </c>
       <c r="F47" s="7">
-        <v>2267</v>
+        <v>3362</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>399</v>
+        <v>42</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="J47" s="7" t="s">
         <v>176</v>
@@ -5806,22 +5955,22 @@
         <v>104</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N47" s="7">
-        <v>2405</v>
+        <v>120</v>
+      </c>
+      <c r="N47" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="O47" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="P47" s="8" t="s">
-        <v>401</v>
+        <v>122</v>
+      </c>
+      <c r="P47" s="9" t="s">
+        <v>407</v>
       </c>
       <c r="Q47" s="7" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="R47" s="7" t="s">
         <v>51</v>
@@ -5836,26 +5985,26 @@
         <v>53</v>
       </c>
       <c r="V47" s="7" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="W47" s="7" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="X47" s="7" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="Y47" s="7" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="Z47" s="7">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="AA47" s="7"/>
       <c r="AB47" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC47" s="8" t="s">
-        <v>407</v>
+      <c r="AC47" s="9" t="s">
+        <v>413</v>
       </c>
       <c r="AD47" s="7"/>
       <c r="AE47" s="7"/>
@@ -5865,6 +6014,528 @@
       <c r="AI47" s="7"/>
       <c r="AJ47" s="7"/>
       <c r="AK47" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="3">
+        <v>2025081344</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="3">
+        <v>3362</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P48" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T48" s="3">
+        <v>1</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="X48" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="Y48" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="Z48" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC48" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="AD48" s="3"/>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="3"/>
+      <c r="AG48" s="3"/>
+      <c r="AH48" s="3"/>
+      <c r="AI48" s="3"/>
+      <c r="AJ48" s="3"/>
+      <c r="AK48" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37">
+      <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="7">
+        <v>2025081374</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7">
+        <v>4541</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="R49" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S49" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T49" s="7">
+        <v>1</v>
+      </c>
+      <c r="U49" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V49" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="W49" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="X49" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="Y49" s="7"/>
+      <c r="Z49" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA49" s="7"/>
+      <c r="AB49" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC49" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD49" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE49" s="7"/>
+      <c r="AF49" s="7"/>
+      <c r="AG49" s="7"/>
+      <c r="AH49" s="7"/>
+      <c r="AI49" s="7"/>
+      <c r="AJ49" s="7"/>
+      <c r="AK49" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:37">
+      <c r="A50" s="3">
+        <v>48</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="3">
+        <v>2025081377</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F50" s="3">
+        <v>2267</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N50" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="P50" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q50" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="R50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T50" s="3">
+        <v>1</v>
+      </c>
+      <c r="U50" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V50" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="X50" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="Y50" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="Z50" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC50" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="AD50" s="3"/>
+      <c r="AE50" s="3"/>
+      <c r="AF50" s="3"/>
+      <c r="AG50" s="3"/>
+      <c r="AH50" s="3"/>
+      <c r="AI50" s="3"/>
+      <c r="AJ50" s="3"/>
+      <c r="AK50" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37">
+      <c r="A51" s="7">
+        <v>49</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="7">
+        <v>2025081415</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" s="7">
+        <v>5352</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L51" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M51" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="N51" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O51" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="P51" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q51" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="R51" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T51" s="7">
+        <v>1</v>
+      </c>
+      <c r="U51" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V51" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="W51" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="X51" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="Y51" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="Z51" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA51" s="7"/>
+      <c r="AB51" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC51" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="AD51" s="7"/>
+      <c r="AE51" s="7"/>
+      <c r="AF51" s="7"/>
+      <c r="AG51" s="7"/>
+      <c r="AH51" s="7"/>
+      <c r="AI51" s="7"/>
+      <c r="AJ51" s="7"/>
+      <c r="AK51" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="3">
+        <v>2025081464</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3">
+        <v>3416</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T52" s="3">
+        <v>1</v>
+      </c>
+      <c r="U52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V52" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="X52" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC52" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE52" s="3"/>
+      <c r="AF52" s="3"/>
+      <c r="AG52" s="3"/>
+      <c r="AH52" s="3"/>
+      <c r="AI52" s="3"/>
+      <c r="AJ52" s="3"/>
+      <c r="AK52" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37">
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="7">
+        <v>2025081467</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7">
+        <v>3977</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="R53" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T53" s="7">
+        <v>1</v>
+      </c>
+      <c r="U53" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V53" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="W53" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="X53" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="Y53" s="7"/>
+      <c r="Z53" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA53" s="7"/>
+      <c r="AB53" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC53" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD53" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE53" s="7"/>
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="7"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="7"/>
+      <c r="AK53" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08121738
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$57</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="472">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-12  )</t>
   </si>
@@ -1418,6 +1418,75 @@
   </si>
   <si>
     <t>2025-08-12 13:20:00</t>
+  </si>
+  <si>
+    <t>D620</t>
+  </si>
+  <si>
+    <t>北縣三愛三店</t>
+  </si>
+  <si>
+    <t>THILF0D620</t>
+  </si>
+  <si>
+    <t>2025-08-12 14:19:46</t>
+  </si>
+  <si>
+    <t>2025-08-12 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 14:19:00</t>
+  </si>
+  <si>
+    <t>三重進安店</t>
+  </si>
+  <si>
+    <t>THILF03796</t>
+  </si>
+  <si>
+    <t>2025-08-12 14:48:58</t>
+  </si>
+  <si>
+    <t>2025-08-12 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 14:47:00</t>
+  </si>
+  <si>
+    <t>三重碧華公園</t>
+  </si>
+  <si>
+    <t>THILF03811</t>
+  </si>
+  <si>
+    <t>2025-08-12 15:29:11</t>
+  </si>
+  <si>
+    <t>2025-08-12 15:15:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 15:30:00</t>
+  </si>
+  <si>
+    <t>PMQ3+TVV</t>
+  </si>
+  <si>
+    <t>D350</t>
+  </si>
+  <si>
+    <t>三重徐匯店</t>
+  </si>
+  <si>
+    <t>THILF0D350</t>
+  </si>
+  <si>
+    <t>2025-08-12 16:23:19</t>
+  </si>
+  <si>
+    <t>2025-08-12 16:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 16:22:00</t>
   </si>
 </sst>
 </file>
@@ -1831,10 +1900,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK53"/>
+  <dimension ref="A1:AK57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6490,7 +6559,7 @@
       <c r="M53" s="8"/>
       <c r="N53" s="7"/>
       <c r="O53" s="8"/>
-      <c r="P53" s="8"/>
+      <c r="P53" s="9"/>
       <c r="Q53" s="7" t="s">
         <v>445</v>
       </c>
@@ -6523,7 +6592,7 @@
       <c r="AB53" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC53" s="8" t="s">
+      <c r="AC53" s="9" t="s">
         <v>84</v>
       </c>
       <c r="AD53" s="7" t="s">
@@ -6536,6 +6605,314 @@
       <c r="AI53" s="7"/>
       <c r="AJ53" s="7"/>
       <c r="AK53" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2025081485</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="R54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S54" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T54" s="3">
+        <v>1</v>
+      </c>
+      <c r="U54" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V54" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="W54" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="X54" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="Y54" s="3"/>
+      <c r="Z54" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA54" s="3"/>
+      <c r="AB54" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC54" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE54" s="3"/>
+      <c r="AF54" s="3"/>
+      <c r="AG54" s="3"/>
+      <c r="AH54" s="3"/>
+      <c r="AI54" s="3"/>
+      <c r="AJ54" s="3"/>
+      <c r="AK54" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37">
+      <c r="A55" s="7">
+        <v>53</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="7">
+        <v>2025081493</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7">
+        <v>3796</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="R55" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T55" s="7">
+        <v>1</v>
+      </c>
+      <c r="U55" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V55" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="W55" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="X55" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="Y55" s="7"/>
+      <c r="Z55" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA55" s="7"/>
+      <c r="AB55" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC55" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD55" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE55" s="7"/>
+      <c r="AF55" s="7"/>
+      <c r="AG55" s="7"/>
+      <c r="AH55" s="7"/>
+      <c r="AI55" s="7"/>
+      <c r="AJ55" s="7"/>
+      <c r="AK55" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" s="3">
+        <v>2025081505</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3">
+        <v>3811</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="R56" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S56" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T56" s="3">
+        <v>1</v>
+      </c>
+      <c r="U56" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V56" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="W56" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="X56" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA56" s="3"/>
+      <c r="AB56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC56" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="AD56" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="3"/>
+      <c r="AH56" s="3"/>
+      <c r="AI56" s="3"/>
+      <c r="AJ56" s="3"/>
+      <c r="AK56" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37">
+      <c r="A57" s="7">
+        <v>55</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="7">
+        <v>2025081518</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="R57" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T57" s="7">
+        <v>1</v>
+      </c>
+      <c r="U57" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V57" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="W57" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="X57" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA57" s="7"/>
+      <c r="AB57" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC57" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD57" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE57" s="7"/>
+      <c r="AF57" s="7"/>
+      <c r="AG57" s="7"/>
+      <c r="AH57" s="7"/>
+      <c r="AI57" s="7"/>
+      <c r="AJ57" s="7"/>
+      <c r="AK57" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08131316
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$57</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$62</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="472">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-12  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="506">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-13  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1438,6 +1438,48 @@
     <t>2025-08-12 14:19:00</t>
   </si>
   <si>
+    <t>14259114081201</t>
+  </si>
+  <si>
+    <t>八里水灣店</t>
+  </si>
+  <si>
+    <t>2025-08-12 14:41:14</t>
+  </si>
+  <si>
+    <t>HLN4</t>
+  </si>
+  <si>
+    <t>HL-PepLink負載平衡器</t>
+  </si>
+  <si>
+    <t>N405</t>
+  </si>
+  <si>
+    <t>4G 無法連線</t>
+  </si>
+  <si>
+    <t>2025/8/12 (週二) 下午 02:36 總公司文豪MAIL:8/12 11:00雙北中華大障礙，其中2家A163士林社子店、4259八里水灣店無法切換4G備援，請協助派工檢測（請更新Firmware 8.4.1s031 build 5461）。...須請台芝到店協助(BALANCE20X)</t>
+  </si>
+  <si>
+    <t>THILF04259</t>
+  </si>
+  <si>
+    <t>2025-08-12 14:44:29</t>
+  </si>
+  <si>
+    <t>2025-08-13 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 12:14:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 18:44:00</t>
+  </si>
+  <si>
+    <t>至現場更新到Firmware8.4，比且中斷中華電信數據機測試4G的使用，可正常使用連線</t>
+  </si>
+  <si>
     <t>三重進安店</t>
   </si>
   <si>
@@ -1487,6 +1529,66 @@
   </si>
   <si>
     <t>2025-08-12 16:22:00</t>
+  </si>
+  <si>
+    <t>板橋民治店</t>
+  </si>
+  <si>
+    <t>THILF03965</t>
+  </si>
+  <si>
+    <t>2025-08-13 11:54:52</t>
+  </si>
+  <si>
+    <t>2025-08-13 11:35:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 11:55:00</t>
+  </si>
+  <si>
+    <t>PMQ3 螢幕線路重置</t>
+  </si>
+  <si>
+    <t>板橋仁化店</t>
+  </si>
+  <si>
+    <t>THILF03962</t>
+  </si>
+  <si>
+    <t>2025-08-13 12:15:48</t>
+  </si>
+  <si>
+    <t>2025-08-13 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 12:15:00</t>
+  </si>
+  <si>
+    <t>北縣莊民店</t>
+  </si>
+  <si>
+    <t>THILF03652</t>
+  </si>
+  <si>
+    <t>2025-08-13 13:09:35</t>
+  </si>
+  <si>
+    <t>2025-08-13 12:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 12:50:00</t>
+  </si>
+  <si>
+    <t>新莊中港店</t>
+  </si>
+  <si>
+    <t>THILF05057</t>
+  </si>
+  <si>
+    <t>2025-08-13 13:13:08</t>
+  </si>
+  <si>
+    <t>2025-08-13 13:10:00</t>
   </si>
 </sst>
 </file>
@@ -1900,10 +2002,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK57"/>
+  <dimension ref="A1:AK62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="AC59" sqref="AC59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6690,32 +6792,52 @@
         <v>53</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C55" s="7">
-        <v>2025081493</v>
-      </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
+        <v>2025081491</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F55" s="7">
-        <v>3796</v>
+        <v>4259</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="8"/>
-      <c r="P55" s="9"/>
+        <v>384</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L55" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="M55" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="N55" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="O55" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="P55" s="9" t="s">
+        <v>462</v>
+      </c>
       <c r="Q55" s="7" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="R55" s="7" t="s">
         <v>51</v>
@@ -6730,28 +6852,28 @@
         <v>53</v>
       </c>
       <c r="V55" s="7" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="W55" s="7" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="X55" s="7" t="s">
-        <v>459</v>
-      </c>
-      <c r="Y55" s="7"/>
+        <v>466</v>
+      </c>
+      <c r="Y55" s="7" t="s">
+        <v>467</v>
+      </c>
       <c r="Z55" s="7">
-        <v>0.3</v>
+        <v>1.2</v>
       </c>
       <c r="AA55" s="7"/>
       <c r="AB55" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC55" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD55" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>468</v>
+      </c>
+      <c r="AD55" s="7"/>
       <c r="AE55" s="7"/>
       <c r="AF55" s="7"/>
       <c r="AG55" s="7"/>
@@ -6770,15 +6892,15 @@
         <v>78</v>
       </c>
       <c r="C56" s="3">
-        <v>2025081505</v>
+        <v>2025081493</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3">
-        <v>3811</v>
+        <v>3796</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>42</v>
@@ -6792,7 +6914,7 @@
       <c r="O56" s="4"/>
       <c r="P56" s="10"/>
       <c r="Q56" s="3" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="R56" s="3" t="s">
         <v>51</v>
@@ -6807,13 +6929,13 @@
         <v>53</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="W56" s="3" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="X56" s="3" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="Y56" s="3"/>
       <c r="Z56" s="3">
@@ -6824,7 +6946,7 @@
         <v>58</v>
       </c>
       <c r="AC56" s="10" t="s">
-        <v>465</v>
+        <v>84</v>
       </c>
       <c r="AD56" s="3" t="s">
         <v>60</v>
@@ -6847,15 +6969,15 @@
         <v>78</v>
       </c>
       <c r="C57" s="7">
-        <v>2025081518</v>
+        <v>2025081505</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
-      <c r="F57" s="7" t="s">
-        <v>466</v>
+      <c r="F57" s="7">
+        <v>3811</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>42</v>
@@ -6867,9 +6989,9 @@
       <c r="M57" s="8"/>
       <c r="N57" s="7"/>
       <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
+      <c r="P57" s="9"/>
       <c r="Q57" s="7" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="R57" s="7" t="s">
         <v>51</v>
@@ -6884,24 +7006,24 @@
         <v>53</v>
       </c>
       <c r="V57" s="7" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="W57" s="7" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="X57" s="7" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="Y57" s="7"/>
       <c r="Z57" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA57" s="7"/>
       <c r="AB57" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC57" s="8" t="s">
-        <v>84</v>
+      <c r="AC57" s="9" t="s">
+        <v>479</v>
       </c>
       <c r="AD57" s="7" t="s">
         <v>60</v>
@@ -6913,6 +7035,391 @@
       <c r="AI57" s="7"/>
       <c r="AJ57" s="7"/>
       <c r="AK57" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:37">
+      <c r="A58" s="3">
+        <v>56</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="3">
+        <v>2025081518</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S58" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T58" s="3">
+        <v>1</v>
+      </c>
+      <c r="U58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V58" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="W58" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="X58" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="Y58" s="3"/>
+      <c r="Z58" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA58" s="3"/>
+      <c r="AB58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC58" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE58" s="3"/>
+      <c r="AF58" s="3"/>
+      <c r="AG58" s="3"/>
+      <c r="AH58" s="3"/>
+      <c r="AI58" s="3"/>
+      <c r="AJ58" s="3"/>
+      <c r="AK58" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:37">
+      <c r="A59" s="7">
+        <v>57</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="7">
+        <v>2025081584</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7">
+        <v>3965</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="8"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="9"/>
+      <c r="Q59" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="R59" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S59" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T59" s="7">
+        <v>1</v>
+      </c>
+      <c r="U59" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V59" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="W59" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="X59" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="Y59" s="7"/>
+      <c r="Z59" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA59" s="7"/>
+      <c r="AB59" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC59" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="AD59" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE59" s="7"/>
+      <c r="AF59" s="7"/>
+      <c r="AG59" s="7"/>
+      <c r="AH59" s="7"/>
+      <c r="AI59" s="7"/>
+      <c r="AJ59" s="7"/>
+      <c r="AK59" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37">
+      <c r="A60" s="3">
+        <v>58</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" s="3">
+        <v>2025081585</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3">
+        <v>3962</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="R60" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S60" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T60" s="3">
+        <v>1</v>
+      </c>
+      <c r="U60" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V60" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="W60" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="X60" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y60" s="3"/>
+      <c r="Z60" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA60" s="3"/>
+      <c r="AB60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC60" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD60" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE60" s="3"/>
+      <c r="AF60" s="3"/>
+      <c r="AG60" s="3"/>
+      <c r="AH60" s="3"/>
+      <c r="AI60" s="3"/>
+      <c r="AJ60" s="3"/>
+      <c r="AK60" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:37">
+      <c r="A61" s="7">
+        <v>59</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="7">
+        <v>2025081589</v>
+      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7">
+        <v>3652</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="9"/>
+      <c r="Q61" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="R61" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S61" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T61" s="7">
+        <v>1</v>
+      </c>
+      <c r="U61" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V61" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="W61" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="X61" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="Y61" s="7"/>
+      <c r="Z61" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA61" s="7"/>
+      <c r="AB61" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC61" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD61" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE61" s="7"/>
+      <c r="AF61" s="7"/>
+      <c r="AG61" s="7"/>
+      <c r="AH61" s="7"/>
+      <c r="AI61" s="7"/>
+      <c r="AJ61" s="7"/>
+      <c r="AK61" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:37">
+      <c r="A62" s="3">
+        <v>60</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="3">
+        <v>2025081592</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3">
+        <v>5057</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="R62" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S62" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T62" s="3">
+        <v>1</v>
+      </c>
+      <c r="U62" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V62" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="W62" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="X62" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y62" s="3"/>
+      <c r="Z62" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA62" s="3"/>
+      <c r="AB62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC62" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD62" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE62" s="3"/>
+      <c r="AF62" s="3"/>
+      <c r="AG62" s="3"/>
+      <c r="AH62" s="3"/>
+      <c r="AI62" s="3"/>
+      <c r="AJ62" s="3"/>
+      <c r="AK62" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08131715
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$68</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="536">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-13  )</t>
   </si>
@@ -1589,6 +1589,96 @@
   </si>
   <si>
     <t>2025-08-13 13:10:00</t>
+  </si>
+  <si>
+    <t>北縣莊榮店</t>
+  </si>
+  <si>
+    <t>THILF03785</t>
+  </si>
+  <si>
+    <t>2025-08-13 13:44:29</t>
+  </si>
+  <si>
+    <t>2025-08-13 13:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 13:40:00</t>
+  </si>
+  <si>
+    <t>蘆洲永平店</t>
+  </si>
+  <si>
+    <t>新北市蘆洲區</t>
+  </si>
+  <si>
+    <t>THILF04923</t>
+  </si>
+  <si>
+    <t>2025-08-13 14:49:50</t>
+  </si>
+  <si>
+    <t>2025-08-13 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 14:47:00</t>
+  </si>
+  <si>
+    <t>新莊豐年店</t>
+  </si>
+  <si>
+    <t>THILF02743</t>
+  </si>
+  <si>
+    <t>2025-08-13 14:54:01</t>
+  </si>
+  <si>
+    <t>2025-08-13 14:50:00</t>
+  </si>
+  <si>
+    <t>蘆洲光榮店</t>
+  </si>
+  <si>
+    <t>THILF03892</t>
+  </si>
+  <si>
+    <t>2025-08-13 15:22:32</t>
+  </si>
+  <si>
+    <t>2025-08-13 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 15:21:00</t>
+  </si>
+  <si>
+    <t>蘆洲長樂店</t>
+  </si>
+  <si>
+    <t>THILF04125</t>
+  </si>
+  <si>
+    <t>2025-08-13 15:52:14</t>
+  </si>
+  <si>
+    <t>2025-08-13 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 15:51:00</t>
+  </si>
+  <si>
+    <t>蘆洲洲正店</t>
+  </si>
+  <si>
+    <t>THILF04609</t>
+  </si>
+  <si>
+    <t>2025-08-13 16:20:52</t>
+  </si>
+  <si>
+    <t>2025-08-13 16:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-13 16:20:00</t>
   </si>
 </sst>
 </file>
@@ -2002,10 +2092,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK62"/>
+  <dimension ref="A1:AK68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC59" sqref="AC59"/>
+      <selection activeCell="AC65" sqref="AC65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7374,7 +7464,7 @@
       <c r="M62" s="4"/>
       <c r="N62" s="3"/>
       <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
+      <c r="P62" s="10"/>
       <c r="Q62" s="3" t="s">
         <v>503</v>
       </c>
@@ -7407,7 +7497,7 @@
       <c r="AB62" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC62" s="4" t="s">
+      <c r="AC62" s="10" t="s">
         <v>84</v>
       </c>
       <c r="AD62" s="3" t="s">
@@ -7420,6 +7510,468 @@
       <c r="AI62" s="3"/>
       <c r="AJ62" s="3"/>
       <c r="AK62" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37">
+      <c r="A63" s="7">
+        <v>61</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="7">
+        <v>2025081597</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7">
+        <v>3785</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="9"/>
+      <c r="Q63" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="R63" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S63" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T63" s="7">
+        <v>1</v>
+      </c>
+      <c r="U63" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V63" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="W63" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="X63" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="Y63" s="7"/>
+      <c r="Z63" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA63" s="7"/>
+      <c r="AB63" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC63" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD63" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE63" s="7"/>
+      <c r="AF63" s="7"/>
+      <c r="AG63" s="7"/>
+      <c r="AH63" s="7"/>
+      <c r="AI63" s="7"/>
+      <c r="AJ63" s="7"/>
+      <c r="AK63" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37">
+      <c r="A64" s="3">
+        <v>62</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="3">
+        <v>2025081663</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3">
+        <v>4923</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="10"/>
+      <c r="Q64" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="R64" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S64" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T64" s="3">
+        <v>1</v>
+      </c>
+      <c r="U64" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V64" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="W64" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="X64" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="Y64" s="3"/>
+      <c r="Z64" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA64" s="3"/>
+      <c r="AB64" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC64" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD64" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE64" s="3"/>
+      <c r="AF64" s="3"/>
+      <c r="AG64" s="3"/>
+      <c r="AH64" s="3"/>
+      <c r="AI64" s="3"/>
+      <c r="AJ64" s="3"/>
+      <c r="AK64" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:37">
+      <c r="A65" s="7">
+        <v>63</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2025081664</v>
+      </c>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7">
+        <v>2743</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="R65" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S65" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T65" s="7">
+        <v>1</v>
+      </c>
+      <c r="U65" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V65" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="W65" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="X65" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC65" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD65" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="7"/>
+      <c r="AG65" s="7"/>
+      <c r="AH65" s="7"/>
+      <c r="AI65" s="7"/>
+      <c r="AJ65" s="7"/>
+      <c r="AK65" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:37">
+      <c r="A66" s="3">
+        <v>64</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="3">
+        <v>2025081670</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3">
+        <v>3892</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T66" s="3">
+        <v>1</v>
+      </c>
+      <c r="U66" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V66" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="W66" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="X66" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="Y66" s="3"/>
+      <c r="Z66" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA66" s="3"/>
+      <c r="AB66" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC66" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="AD66" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE66" s="3"/>
+      <c r="AF66" s="3"/>
+      <c r="AG66" s="3"/>
+      <c r="AH66" s="3"/>
+      <c r="AI66" s="3"/>
+      <c r="AJ66" s="3"/>
+      <c r="AK66" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:37">
+      <c r="A67" s="7">
+        <v>65</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="7">
+        <v>2025081677</v>
+      </c>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7">
+        <v>4125</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="8"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="8"/>
+      <c r="P67" s="9"/>
+      <c r="Q67" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="R67" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S67" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T67" s="7">
+        <v>1</v>
+      </c>
+      <c r="U67" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V67" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="W67" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="X67" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="Y67" s="7"/>
+      <c r="Z67" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA67" s="7"/>
+      <c r="AB67" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC67" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD67" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE67" s="7"/>
+      <c r="AF67" s="7"/>
+      <c r="AG67" s="7"/>
+      <c r="AH67" s="7"/>
+      <c r="AI67" s="7"/>
+      <c r="AJ67" s="7"/>
+      <c r="AK67" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:37">
+      <c r="A68" s="3">
+        <v>66</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" s="3">
+        <v>2025081687</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3">
+        <v>4609</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4"/>
+      <c r="Q68" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T68" s="3">
+        <v>1</v>
+      </c>
+      <c r="U68" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V68" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="W68" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="X68" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA68" s="3"/>
+      <c r="AB68" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC68" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD68" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE68" s="3"/>
+      <c r="AF68" s="3"/>
+      <c r="AG68" s="3"/>
+      <c r="AH68" s="3"/>
+      <c r="AI68" s="3"/>
+      <c r="AJ68" s="3"/>
+      <c r="AK68" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08141600
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$75</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="536">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-13  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="590">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-14  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1531,6 +1531,39 @@
     <t>2025-08-12 16:22:00</t>
   </si>
   <si>
+    <t>12042114081301</t>
+  </si>
+  <si>
+    <t>三重中央北店</t>
+  </si>
+  <si>
+    <t>2025-08-13 11:14:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm1 CCD掃瞄器(HC76-TR):門市反應TM1不論清帳或交班後都會跳出COMPORT偵測異常，點選清除後，出現：COMPORT偵測異常，請按[清除]後，退到登入頁面，按下[版本更新]，自動重啟系統，或撥打0800客服報修11111，因頻繁發生門市告知已造成困擾。經HIPOS查詢:與開發確認，出現回主畫面出現COMPORT偵測異常，請按[清除]後，退到登入頁面，按下[版本更新]為系統與CCD之間連線問題，如頻繁發生建議轉派台芝到店檢查相關設備及線路。..請台芝到店協助
+</t>
+  </si>
+  <si>
+    <t>THILF02042</t>
+  </si>
+  <si>
+    <t>2025-08-13 11:16:45</t>
+  </si>
+  <si>
+    <t>2025-08-14 13:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-14 14:31:00</t>
+  </si>
+  <si>
+    <t>2025-08-14 15:16:00</t>
+  </si>
+  <si>
+    <t>更換主機
+換下8185000630
+換上8185002963</t>
+  </si>
+  <si>
     <t>板橋民治店</t>
   </si>
   <si>
@@ -1606,6 +1639,42 @@
     <t>2025-08-13 13:40:00</t>
   </si>
   <si>
+    <t>1D111114081301</t>
+  </si>
+  <si>
+    <t>D111</t>
+  </si>
+  <si>
+    <t>北縣府中店</t>
+  </si>
+  <si>
+    <t>2025-08-13 14:12:40</t>
+  </si>
+  <si>
+    <t>觸控不良(游標偏移)</t>
+  </si>
+  <si>
+    <t>門市TM1(TCX800)觸控亂跳，已協助遠端重啟後仍異常，因亂跳嚴重無法協助觸控校正，請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D111</t>
+  </si>
+  <si>
+    <t>2025-08-13 14:13:56</t>
+  </si>
+  <si>
+    <t>2025-08-14 13:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-14 15:05:00</t>
+  </si>
+  <si>
+    <t>2025-08-14 18:13:00</t>
+  </si>
+  <si>
+    <t>線路重接，軟體校正後測試正常</t>
+  </si>
+  <si>
     <t>蘆洲永平店</t>
   </si>
   <si>
@@ -1679,6 +1748,110 @@
   </si>
   <si>
     <t>2025-08-13 16:20:00</t>
+  </si>
+  <si>
+    <t>1D111114081302</t>
+  </si>
+  <si>
+    <t>2025-08-13 17:15:18</t>
+  </si>
+  <si>
+    <t>門市反應印票機(L90)ERROR燈號亮紅燈，門市嘗試關機關不了，後方線路雜亂也無法協助拔插電源線，需請台芝入店協助</t>
+  </si>
+  <si>
+    <t>2025-08-13 17:17:01</t>
+  </si>
+  <si>
+    <t>2025-08-14 21:17:00</t>
+  </si>
+  <si>
+    <t>印票機測試正常
+因案：1D111114081301
+POS機觸控異常導致出票程序無法操作</t>
+  </si>
+  <si>
+    <t>14194114081301</t>
+  </si>
+  <si>
+    <t>新莊鼎苑店</t>
+  </si>
+  <si>
+    <t>2025-08-13 20:18:21</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)抽屜打不開，門市已嘗試將發票機重啟並重新安裝卷紙仍異常，抽屜外觀米白/鑰匙孔中間/無編號，需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04194</t>
+  </si>
+  <si>
+    <t>2025-08-13 20:20:03</t>
+  </si>
+  <si>
+    <t>2025-08-14 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-14 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 00:20:00</t>
+  </si>
+  <si>
+    <t>更換錢箱
+換上81Z1004478
+換下81Z1000878</t>
+  </si>
+  <si>
+    <t>14194114081302</t>
+  </si>
+  <si>
+    <t>2025-08-13 20:26:36</t>
+  </si>
+  <si>
+    <t>門市告知TM1掃槍(HC56II-TR)經常無法刷讀，已嘗試執行掃槍校正到第3條碼就沒反應，需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-13 20:30:59</t>
+  </si>
+  <si>
+    <t>2025-08-14 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 00:31:00</t>
+  </si>
+  <si>
+    <t>更換手持
+換上8119011532
+換下8119008007</t>
+  </si>
+  <si>
+    <t>2025-08-14 11:27:47</t>
+  </si>
+  <si>
+    <t>2025-08-14 11:20:00</t>
+  </si>
+  <si>
+    <t>E4194114081401</t>
+  </si>
+  <si>
+    <t>2025-08-14 12:20:07</t>
+  </si>
+  <si>
+    <t>門市反應TM2 CCD(HC56II-TR)前端膠條破損導致感應不良...須請台芝到店協助(機台2掃描器破損，請工程師到店檢查)</t>
+  </si>
+  <si>
+    <t>2025-08-14 12:34:56</t>
+  </si>
+  <si>
+    <t>2025-08-14 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 16:34:00</t>
+  </si>
+  <si>
+    <t>更換手持
+換上8119012879
+換下8119008008</t>
   </si>
 </sst>
 </file>
@@ -2092,10 +2265,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK68"/>
+  <dimension ref="A1:AK75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC65" sqref="AC65"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7210,38 +7383,58 @@
         <v>57</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C59" s="7">
-        <v>2025081584</v>
-      </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
+        <v>2025081576</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F59" s="7">
-        <v>3965</v>
+        <v>2042</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="8"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="8"/>
-      <c r="P59" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L59" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M59" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="N59" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O59" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="P59" s="9" t="s">
+        <v>489</v>
+      </c>
       <c r="Q59" s="7" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="R59" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S59" s="7" t="s">
-        <v>210</v>
+        <v>52</v>
       </c>
       <c r="T59" s="7">
         <v>1</v>
@@ -7250,28 +7443,28 @@
         <v>53</v>
       </c>
       <c r="V59" s="7" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="W59" s="7" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="X59" s="7" t="s">
-        <v>490</v>
-      </c>
-      <c r="Y59" s="7"/>
+        <v>493</v>
+      </c>
+      <c r="Y59" s="7" t="s">
+        <v>494</v>
+      </c>
       <c r="Z59" s="7">
-        <v>0.3</v>
+        <v>1.2</v>
       </c>
       <c r="AA59" s="7"/>
       <c r="AB59" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC59" s="9" t="s">
-        <v>491</v>
-      </c>
-      <c r="AD59" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>495</v>
+      </c>
+      <c r="AD59" s="7"/>
       <c r="AE59" s="7"/>
       <c r="AF59" s="7"/>
       <c r="AG59" s="7"/>
@@ -7290,15 +7483,15 @@
         <v>78</v>
       </c>
       <c r="C60" s="3">
-        <v>2025081585</v>
+        <v>2025081584</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3">
-        <v>3962</v>
+        <v>3965</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>206</v>
@@ -7312,7 +7505,7 @@
       <c r="O60" s="4"/>
       <c r="P60" s="10"/>
       <c r="Q60" s="3" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="R60" s="3" t="s">
         <v>51</v>
@@ -7327,13 +7520,13 @@
         <v>53</v>
       </c>
       <c r="V60" s="3" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="W60" s="3" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="X60" s="3" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="Y60" s="3"/>
       <c r="Z60" s="3">
@@ -7344,7 +7537,7 @@
         <v>58</v>
       </c>
       <c r="AC60" s="10" t="s">
-        <v>84</v>
+        <v>501</v>
       </c>
       <c r="AD60" s="3" t="s">
         <v>60</v>
@@ -7367,18 +7560,18 @@
         <v>78</v>
       </c>
       <c r="C61" s="7">
-        <v>2025081589</v>
+        <v>2025081585</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7">
-        <v>3652</v>
+        <v>3962</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
@@ -7389,13 +7582,13 @@
       <c r="O61" s="8"/>
       <c r="P61" s="9"/>
       <c r="Q61" s="7" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="R61" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S61" s="7" t="s">
-        <v>72</v>
+        <v>210</v>
       </c>
       <c r="T61" s="7">
         <v>1</v>
@@ -7404,13 +7597,13 @@
         <v>53</v>
       </c>
       <c r="V61" s="7" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="W61" s="7" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="X61" s="7" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="Y61" s="7"/>
       <c r="Z61" s="7">
@@ -7444,15 +7637,15 @@
         <v>78</v>
       </c>
       <c r="C62" s="3">
-        <v>2025081592</v>
+        <v>2025081589</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3">
-        <v>5057</v>
+        <v>3652</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>64</v>
@@ -7466,7 +7659,7 @@
       <c r="O62" s="4"/>
       <c r="P62" s="10"/>
       <c r="Q62" s="3" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="R62" s="3" t="s">
         <v>51</v>
@@ -7481,13 +7674,13 @@
         <v>53</v>
       </c>
       <c r="V62" s="3" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="W62" s="3" t="s">
-        <v>501</v>
+        <v>510</v>
       </c>
       <c r="X62" s="3" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="Y62" s="3"/>
       <c r="Z62" s="3">
@@ -7521,15 +7714,15 @@
         <v>78</v>
       </c>
       <c r="C63" s="7">
-        <v>2025081597</v>
+        <v>2025081592</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7">
-        <v>3785</v>
+        <v>5057</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>64</v>
@@ -7543,7 +7736,7 @@
       <c r="O63" s="8"/>
       <c r="P63" s="9"/>
       <c r="Q63" s="7" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="R63" s="7" t="s">
         <v>51</v>
@@ -7558,13 +7751,13 @@
         <v>53</v>
       </c>
       <c r="V63" s="7" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="W63" s="7" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="X63" s="7" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="Y63" s="7"/>
       <c r="Z63" s="7">
@@ -7598,18 +7791,18 @@
         <v>78</v>
       </c>
       <c r="C64" s="3">
-        <v>2025081663</v>
+        <v>2025081597</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3">
-        <v>4923</v>
+        <v>3785</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
@@ -7620,13 +7813,13 @@
       <c r="O64" s="4"/>
       <c r="P64" s="10"/>
       <c r="Q64" s="3" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="R64" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T64" s="3">
         <v>1</v>
@@ -7635,13 +7828,13 @@
         <v>53</v>
       </c>
       <c r="V64" s="3" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="W64" s="3" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="X64" s="3" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="Y64" s="3"/>
       <c r="Z64" s="3">
@@ -7672,38 +7865,58 @@
         <v>63</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C65" s="7">
-        <v>2025081664</v>
-      </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7">
-        <v>2743</v>
+        <v>2025081606</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>522</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="7"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="7"/>
-      <c r="O65" s="8"/>
-      <c r="P65" s="9"/>
+        <v>206</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="J65" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="K65" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L65" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M65" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N65" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O65" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="P65" s="9" t="s">
+        <v>526</v>
+      </c>
       <c r="Q65" s="7" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
       <c r="R65" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S65" s="7" t="s">
-        <v>72</v>
+        <v>210</v>
       </c>
       <c r="T65" s="7">
         <v>1</v>
@@ -7712,28 +7925,28 @@
         <v>53</v>
       </c>
       <c r="V65" s="7" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
       <c r="W65" s="7" t="s">
-        <v>515</v>
+        <v>529</v>
       </c>
       <c r="X65" s="7" t="s">
-        <v>520</v>
-      </c>
-      <c r="Y65" s="7"/>
+        <v>530</v>
+      </c>
+      <c r="Y65" s="7" t="s">
+        <v>531</v>
+      </c>
       <c r="Z65" s="7">
-        <v>0.3</v>
+        <v>1.6</v>
       </c>
       <c r="AA65" s="7"/>
       <c r="AB65" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC65" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD65" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>532</v>
+      </c>
+      <c r="AD65" s="7"/>
       <c r="AE65" s="7"/>
       <c r="AF65" s="7"/>
       <c r="AG65" s="7"/>
@@ -7752,18 +7965,18 @@
         <v>78</v>
       </c>
       <c r="C66" s="3">
-        <v>2025081670</v>
+        <v>2025081663</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3">
-        <v>3892</v>
+        <v>4923</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>512</v>
+        <v>534</v>
       </c>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
@@ -7774,7 +7987,7 @@
       <c r="O66" s="4"/>
       <c r="P66" s="10"/>
       <c r="Q66" s="3" t="s">
-        <v>522</v>
+        <v>535</v>
       </c>
       <c r="R66" s="3" t="s">
         <v>51</v>
@@ -7789,24 +8002,24 @@
         <v>53</v>
       </c>
       <c r="V66" s="3" t="s">
-        <v>523</v>
+        <v>536</v>
       </c>
       <c r="W66" s="3" t="s">
-        <v>524</v>
+        <v>537</v>
       </c>
       <c r="X66" s="3" t="s">
-        <v>525</v>
+        <v>538</v>
       </c>
       <c r="Y66" s="3"/>
       <c r="Z66" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA66" s="3"/>
       <c r="AB66" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC66" s="10" t="s">
-        <v>479</v>
+        <v>84</v>
       </c>
       <c r="AD66" s="3" t="s">
         <v>60</v>
@@ -7829,18 +8042,18 @@
         <v>78</v>
       </c>
       <c r="C67" s="7">
-        <v>2025081677</v>
+        <v>2025081664</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7">
-        <v>4125</v>
+        <v>2743</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>526</v>
+        <v>539</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
@@ -7851,13 +8064,13 @@
       <c r="O67" s="8"/>
       <c r="P67" s="9"/>
       <c r="Q67" s="7" t="s">
-        <v>527</v>
+        <v>540</v>
       </c>
       <c r="R67" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S67" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T67" s="7">
         <v>1</v>
@@ -7866,17 +8079,17 @@
         <v>53</v>
       </c>
       <c r="V67" s="7" t="s">
-        <v>528</v>
+        <v>541</v>
       </c>
       <c r="W67" s="7" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="X67" s="7" t="s">
-        <v>530</v>
+        <v>542</v>
       </c>
       <c r="Y67" s="7"/>
       <c r="Z67" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA67" s="7"/>
       <c r="AB67" s="7" t="s">
@@ -7906,18 +8119,18 @@
         <v>78</v>
       </c>
       <c r="C68" s="3">
-        <v>2025081687</v>
+        <v>2025081670</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3">
-        <v>4609</v>
+        <v>3892</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>531</v>
+        <v>543</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>512</v>
+        <v>534</v>
       </c>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
@@ -7926,9 +8139,9 @@
       <c r="M68" s="4"/>
       <c r="N68" s="3"/>
       <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
+      <c r="P68" s="10"/>
       <c r="Q68" s="3" t="s">
-        <v>532</v>
+        <v>544</v>
       </c>
       <c r="R68" s="3" t="s">
         <v>51</v>
@@ -7943,24 +8156,24 @@
         <v>53</v>
       </c>
       <c r="V68" s="3" t="s">
-        <v>533</v>
+        <v>545</v>
       </c>
       <c r="W68" s="3" t="s">
-        <v>534</v>
+        <v>546</v>
       </c>
       <c r="X68" s="3" t="s">
-        <v>535</v>
+        <v>547</v>
       </c>
       <c r="Y68" s="3"/>
       <c r="Z68" s="3">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="AA68" s="3"/>
       <c r="AB68" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC68" s="4" t="s">
-        <v>84</v>
+      <c r="AC68" s="10" t="s">
+        <v>479</v>
       </c>
       <c r="AD68" s="3" t="s">
         <v>60</v>
@@ -7972,6 +8185,625 @@
       <c r="AI68" s="3"/>
       <c r="AJ68" s="3"/>
       <c r="AK68" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:37">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" s="7">
+        <v>2025081677</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7">
+        <v>4125</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="8"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="8"/>
+      <c r="P69" s="9"/>
+      <c r="Q69" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="R69" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S69" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T69" s="7">
+        <v>1</v>
+      </c>
+      <c r="U69" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V69" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="W69" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="X69" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="Y69" s="7"/>
+      <c r="Z69" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA69" s="7"/>
+      <c r="AB69" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC69" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD69" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE69" s="7"/>
+      <c r="AF69" s="7"/>
+      <c r="AG69" s="7"/>
+      <c r="AH69" s="7"/>
+      <c r="AI69" s="7"/>
+      <c r="AJ69" s="7"/>
+      <c r="AK69" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:37">
+      <c r="A70" s="3">
+        <v>68</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" s="3">
+        <v>2025081687</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3">
+        <v>4609</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="R70" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S70" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T70" s="3">
+        <v>1</v>
+      </c>
+      <c r="U70" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V70" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="W70" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="X70" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="Y70" s="3"/>
+      <c r="Z70" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA70" s="3"/>
+      <c r="AB70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC70" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD70" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE70" s="3"/>
+      <c r="AF70" s="3"/>
+      <c r="AG70" s="3"/>
+      <c r="AH70" s="3"/>
+      <c r="AI70" s="3"/>
+      <c r="AJ70" s="3"/>
+      <c r="AK70" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:37">
+      <c r="A71" s="7">
+        <v>69</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="7">
+        <v>2025081702</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="J71" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="K71" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L71" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="M71" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="N71" s="7">
+        <v>6003</v>
+      </c>
+      <c r="O71" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P71" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="Q71" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="R71" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S71" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T71" s="7">
+        <v>1</v>
+      </c>
+      <c r="U71" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V71" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="W71" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="X71" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="Y71" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="Z71" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="AA71" s="7"/>
+      <c r="AB71" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC71" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="AD71" s="7"/>
+      <c r="AE71" s="7"/>
+      <c r="AF71" s="7"/>
+      <c r="AG71" s="7"/>
+      <c r="AH71" s="7"/>
+      <c r="AI71" s="7"/>
+      <c r="AJ71" s="7"/>
+      <c r="AK71" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:37">
+      <c r="A72" s="3">
+        <v>70</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" s="3">
+        <v>2025081705</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F72" s="3">
+        <v>4194</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M72" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="N72" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O72" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P72" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="Q72" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="R72" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S72" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T72" s="3">
+        <v>1</v>
+      </c>
+      <c r="U72" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V72" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="W72" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="X72" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="Y72" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="Z72" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA72" s="3"/>
+      <c r="AB72" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC72" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="AD72" s="3"/>
+      <c r="AE72" s="3"/>
+      <c r="AF72" s="3"/>
+      <c r="AG72" s="3"/>
+      <c r="AH72" s="3"/>
+      <c r="AI72" s="3"/>
+      <c r="AJ72" s="3"/>
+      <c r="AK72" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:37">
+      <c r="A73" s="7">
+        <v>71</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" s="7">
+        <v>2025081706</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F73" s="7">
+        <v>4194</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="J73" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="K73" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="L73" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M73" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="N73" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O73" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="P73" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="Q73" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="R73" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S73" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T73" s="7">
+        <v>1</v>
+      </c>
+      <c r="U73" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V73" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="W73" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="X73" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="Y73" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="Z73" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA73" s="7"/>
+      <c r="AB73" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC73" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="AD73" s="7"/>
+      <c r="AE73" s="7"/>
+      <c r="AF73" s="7"/>
+      <c r="AG73" s="7"/>
+      <c r="AH73" s="7"/>
+      <c r="AI73" s="7"/>
+      <c r="AJ73" s="7"/>
+      <c r="AK73" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:37">
+      <c r="A74" s="3">
+        <v>72</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" s="3">
+        <v>2025081741</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3">
+        <v>4194</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="R74" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S74" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T74" s="3">
+        <v>1</v>
+      </c>
+      <c r="U74" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V74" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="W74" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="X74" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="Y74" s="3"/>
+      <c r="Z74" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA74" s="3"/>
+      <c r="AB74" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC74" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD74" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE74" s="3"/>
+      <c r="AF74" s="3"/>
+      <c r="AG74" s="3"/>
+      <c r="AH74" s="3"/>
+      <c r="AI74" s="3"/>
+      <c r="AJ74" s="3"/>
+      <c r="AK74" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:37">
+      <c r="A75" s="7">
+        <v>73</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" s="7">
+        <v>2025081760</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F75" s="7">
+        <v>4194</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K75" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M75" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="N75" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O75" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="P75" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="Q75" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="R75" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S75" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T75" s="7">
+        <v>1</v>
+      </c>
+      <c r="U75" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V75" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="W75" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="X75" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="Y75" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="Z75" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC75" s="8" t="s">
+        <v>589</v>
+      </c>
+      <c r="AD75" s="7"/>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="7"/>
+      <c r="AG75" s="7"/>
+      <c r="AH75" s="7"/>
+      <c r="AI75" s="7"/>
+      <c r="AJ75" s="7"/>
+      <c r="AK75" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08151615
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$85</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="590">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-14  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="651">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-15  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1852,6 +1852,192 @@
     <t>更換手持
 換上8119012879
 換下8119008008</t>
+  </si>
+  <si>
+    <t>E3772114081501</t>
+  </si>
+  <si>
+    <t>2025-08-15 06:41:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應LIFEET 熱感機T70II印出的小白單模糊，中間靠右有明顯空白線條，已請門市嘗試重裝紙捲、重啟熱感機電源，清潔出票口仍異常....需請台芝到店協助(印字不清)  
+</t>
+  </si>
+  <si>
+    <t>2025-08-15 09:08:49</t>
+  </si>
+  <si>
+    <t>2025-08-15 13:59:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 14:29:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 13:08:00</t>
+  </si>
+  <si>
+    <t>清除熱感頭異物，列印後都可正常使用</t>
+  </si>
+  <si>
+    <t>D191</t>
+  </si>
+  <si>
+    <t>三重興德店</t>
+  </si>
+  <si>
+    <t>THILF0D191</t>
+  </si>
+  <si>
+    <t>2025-08-15 10:15:33</t>
+  </si>
+  <si>
+    <t>2025-08-15 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 10:00:00</t>
+  </si>
+  <si>
+    <t>三重初戀店</t>
+  </si>
+  <si>
+    <t>THILF04977</t>
+  </si>
+  <si>
+    <t>2025-08-15 10:38:06</t>
+  </si>
+  <si>
+    <t>2025-08-15 10:10:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 10:30:00</t>
+  </si>
+  <si>
+    <t>D087</t>
+  </si>
+  <si>
+    <t>三重中興北</t>
+  </si>
+  <si>
+    <t>THILF0D087</t>
+  </si>
+  <si>
+    <t>2025-08-15 11:01:58</t>
+  </si>
+  <si>
+    <t>2025-08-15 10:40:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 11:01:00</t>
+  </si>
+  <si>
+    <t>D138</t>
+  </si>
+  <si>
+    <t>三重中興北二</t>
+  </si>
+  <si>
+    <t>THILF0D138</t>
+  </si>
+  <si>
+    <t>2025-08-15 11:32:44</t>
+  </si>
+  <si>
+    <t>2025-08-15 11:10:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 11:32:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 13:25:58</t>
+  </si>
+  <si>
+    <t>2025-08-15 11:30:00</t>
+  </si>
+  <si>
+    <t>TVV</t>
+  </si>
+  <si>
+    <t>北縣重富店</t>
+  </si>
+  <si>
+    <t>THILF03601</t>
+  </si>
+  <si>
+    <t>2025-08-15 13:29:18</t>
+  </si>
+  <si>
+    <t>2025-08-15 13:10:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 13:30:00</t>
+  </si>
+  <si>
+    <t>三重頂崁店</t>
+  </si>
+  <si>
+    <t>THILF04698</t>
+  </si>
+  <si>
+    <t>2025-08-15 13:56:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 13:40:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 14:00:00</t>
+  </si>
+  <si>
+    <t>E4098114081501</t>
+  </si>
+  <si>
+    <t>三重仁美店</t>
+  </si>
+  <si>
+    <t>2025-08-15 13:39:59</t>
+  </si>
+  <si>
+    <t>門市反應tm2 ccd掃描器(HC56II-TR)刷讀所有條碼都無反應有亮燈有逼聲，已請門市操作掃描器校正但第六段條碼都刷不到....須請台芝到店協助 (掃描器無法使用)</t>
+  </si>
+  <si>
+    <t>THILF04098</t>
+  </si>
+  <si>
+    <t>2025-08-15 14:22:22</t>
+  </si>
+  <si>
+    <t>2025-08-15 15:04:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 15:34:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 18:22:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119008721
+換上8119012881</t>
+  </si>
+  <si>
+    <t>14098114081501</t>
+  </si>
+  <si>
+    <t>2025-08-15 14:48:59</t>
+  </si>
+  <si>
+    <t>2025/08/15 14:45總公司郁仁來電啟動緊急叫修：反應tm2 ccd掃描器(HC56II-TR)刷讀所有條碼都無反應有亮燈有逼聲，已請門市操作掃描器校正但第六段條碼都刷不到....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-15 14:50:09</t>
+  </si>
+  <si>
+    <t>2025-08-15 15:06:00</t>
+  </si>
+  <si>
+    <t>2025-08-15 15:36:00</t>
+  </si>
+  <si>
+    <t>2025-08-16 07:50:00</t>
   </si>
 </sst>
 </file>
@@ -2265,10 +2451,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK75"/>
+  <dimension ref="A1:AK85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8756,7 +8942,7 @@
       <c r="O75" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="P75" s="8" t="s">
+      <c r="P75" s="9" t="s">
         <v>585</v>
       </c>
       <c r="Q75" s="7" t="s">
@@ -8793,7 +8979,7 @@
       <c r="AB75" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC75" s="8" t="s">
+      <c r="AC75" s="9" t="s">
         <v>589</v>
       </c>
       <c r="AD75" s="7"/>
@@ -8804,6 +8990,836 @@
       <c r="AI75" s="7"/>
       <c r="AJ75" s="7"/>
       <c r="AK75" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:37">
+      <c r="A76" s="3">
+        <v>74</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76" s="3">
+        <v>2025081829</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F76" s="3">
+        <v>3772</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M76" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N76" s="3">
+        <v>5902</v>
+      </c>
+      <c r="O76" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="Q76" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="R76" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S76" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T76" s="3">
+        <v>1</v>
+      </c>
+      <c r="U76" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V76" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="W76" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="X76" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="Y76" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="Z76" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA76" s="3"/>
+      <c r="AB76" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC76" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="AD76" s="3"/>
+      <c r="AE76" s="3"/>
+      <c r="AF76" s="3"/>
+      <c r="AG76" s="3"/>
+      <c r="AH76" s="3"/>
+      <c r="AI76" s="3"/>
+      <c r="AJ76" s="3"/>
+      <c r="AK76" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:37">
+      <c r="A77" s="7">
+        <v>75</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77" s="7">
+        <v>2025081853</v>
+      </c>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="8"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="8"/>
+      <c r="P77" s="9"/>
+      <c r="Q77" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="R77" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S77" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T77" s="7">
+        <v>1</v>
+      </c>
+      <c r="U77" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V77" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="W77" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="X77" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="Y77" s="7"/>
+      <c r="Z77" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA77" s="7"/>
+      <c r="AB77" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC77" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD77" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE77" s="7"/>
+      <c r="AF77" s="7"/>
+      <c r="AG77" s="7"/>
+      <c r="AH77" s="7"/>
+      <c r="AI77" s="7"/>
+      <c r="AJ77" s="7"/>
+      <c r="AK77" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:37">
+      <c r="A78" s="3">
+        <v>76</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C78" s="3">
+        <v>2025081858</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3">
+        <v>4977</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="10"/>
+      <c r="Q78" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S78" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T78" s="3">
+        <v>1</v>
+      </c>
+      <c r="U78" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V78" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="W78" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="X78" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="Y78" s="3"/>
+      <c r="Z78" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA78" s="3"/>
+      <c r="AB78" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC78" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD78" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE78" s="3"/>
+      <c r="AF78" s="3"/>
+      <c r="AG78" s="3"/>
+      <c r="AH78" s="3"/>
+      <c r="AI78" s="3"/>
+      <c r="AJ78" s="3"/>
+      <c r="AK78" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:37">
+      <c r="A79" s="7">
+        <v>77</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" s="7">
+        <v>2025081863</v>
+      </c>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="8"/>
+      <c r="N79" s="7"/>
+      <c r="O79" s="8"/>
+      <c r="P79" s="9"/>
+      <c r="Q79" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="R79" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S79" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T79" s="7">
+        <v>1</v>
+      </c>
+      <c r="U79" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V79" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="W79" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="X79" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="Y79" s="7"/>
+      <c r="Z79" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA79" s="7"/>
+      <c r="AB79" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC79" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD79" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE79" s="7"/>
+      <c r="AF79" s="7"/>
+      <c r="AG79" s="7"/>
+      <c r="AH79" s="7"/>
+      <c r="AI79" s="7"/>
+      <c r="AJ79" s="7"/>
+      <c r="AK79" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:37">
+      <c r="A80" s="3">
+        <v>78</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" s="3">
+        <v>2025081871</v>
+      </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="10"/>
+      <c r="Q80" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="R80" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S80" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T80" s="3">
+        <v>1</v>
+      </c>
+      <c r="U80" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V80" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="W80" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="X80" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y80" s="3"/>
+      <c r="Z80" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA80" s="3"/>
+      <c r="AB80" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC80" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD80" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE80" s="3"/>
+      <c r="AF80" s="3"/>
+      <c r="AG80" s="3"/>
+      <c r="AH80" s="3"/>
+      <c r="AI80" s="3"/>
+      <c r="AJ80" s="3"/>
+      <c r="AK80" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:37">
+      <c r="A81" s="7">
+        <v>79</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C81" s="7">
+        <v>2025081894</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="R81" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S81" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T81" s="7">
+        <v>1</v>
+      </c>
+      <c r="U81" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V81" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="W81" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="X81" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC81" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="AD81" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="7"/>
+      <c r="AG81" s="7"/>
+      <c r="AH81" s="7"/>
+      <c r="AI81" s="7"/>
+      <c r="AJ81" s="7"/>
+      <c r="AK81" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:37">
+      <c r="A82" s="3">
+        <v>80</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C82" s="3">
+        <v>2025081895</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3">
+        <v>3601</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="10"/>
+      <c r="Q82" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="R82" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S82" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T82" s="3">
+        <v>1</v>
+      </c>
+      <c r="U82" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V82" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="W82" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="X82" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="Y82" s="3"/>
+      <c r="Z82" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA82" s="3"/>
+      <c r="AB82" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC82" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD82" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE82" s="3"/>
+      <c r="AF82" s="3"/>
+      <c r="AG82" s="3"/>
+      <c r="AH82" s="3"/>
+      <c r="AI82" s="3"/>
+      <c r="AJ82" s="3"/>
+      <c r="AK82" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:37">
+      <c r="A83" s="7">
+        <v>81</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C83" s="7">
+        <v>2025081898</v>
+      </c>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7">
+        <v>4698</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="8"/>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="R83" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S83" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T83" s="7">
+        <v>1</v>
+      </c>
+      <c r="U83" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V83" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="W83" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="X83" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="Y83" s="7"/>
+      <c r="Z83" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA83" s="7"/>
+      <c r="AB83" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC83" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="AD83" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE83" s="7"/>
+      <c r="AF83" s="7"/>
+      <c r="AG83" s="7"/>
+      <c r="AH83" s="7"/>
+      <c r="AI83" s="7"/>
+      <c r="AJ83" s="7"/>
+      <c r="AK83" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:37">
+      <c r="A84" s="3">
+        <v>82</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C84" s="3">
+        <v>2025081905</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F84" s="3">
+        <v>4098</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K84" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L84" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M84" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="N84" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O84" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P84" s="10" t="s">
+        <v>637</v>
+      </c>
+      <c r="Q84" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="R84" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S84" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T84" s="3">
+        <v>1</v>
+      </c>
+      <c r="U84" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V84" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="W84" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="X84" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="Y84" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="Z84" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA84" s="3"/>
+      <c r="AB84" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC84" s="10" t="s">
+        <v>643</v>
+      </c>
+      <c r="AD84" s="3"/>
+      <c r="AE84" s="3"/>
+      <c r="AF84" s="3"/>
+      <c r="AG84" s="3"/>
+      <c r="AH84" s="3"/>
+      <c r="AI84" s="3"/>
+      <c r="AJ84" s="3"/>
+      <c r="AK84" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:37">
+      <c r="A85" s="7">
+        <v>83</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C85" s="7">
+        <v>2025081923</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="F85" s="7">
+        <v>4098</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I85" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="J85" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K85" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L85" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M85" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="N85" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O85" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="P85" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="Q85" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="R85" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S85" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T85" s="7">
+        <v>1</v>
+      </c>
+      <c r="U85" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V85" s="7" t="s">
+        <v>647</v>
+      </c>
+      <c r="W85" s="7" t="s">
+        <v>648</v>
+      </c>
+      <c r="X85" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="Y85" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="Z85" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA85" s="7"/>
+      <c r="AB85" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC85" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="AD85" s="7"/>
+      <c r="AE85" s="7"/>
+      <c r="AF85" s="7"/>
+      <c r="AG85" s="7"/>
+      <c r="AH85" s="7"/>
+      <c r="AI85" s="7"/>
+      <c r="AJ85" s="7"/>
+      <c r="AK85" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08181322
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$85</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$97</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="651">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-15  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="718">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-18  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2038,6 +2038,212 @@
   </si>
   <si>
     <t>2025-08-16 07:50:00</t>
+  </si>
+  <si>
+    <t>13929114081601</t>
+  </si>
+  <si>
+    <t>蘆洲中山一</t>
+  </si>
+  <si>
+    <t>2025-08-16 10:21:51</t>
+  </si>
+  <si>
+    <t>門市反應TM1多卡機(QP3000E)無電源反應無畫面，門市已有重新拔插後方線路仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03929</t>
+  </si>
+  <si>
+    <t>2025-08-16 10:23:16</t>
+  </si>
+  <si>
+    <t>2025-08-18 11:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 12:10:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 13:00:00</t>
+  </si>
+  <si>
+    <t>檢查變壓器插上後，通電正常，可正常使用</t>
+  </si>
+  <si>
+    <t>E2837114081601</t>
+  </si>
+  <si>
+    <t>三重洛陽店</t>
+  </si>
+  <si>
+    <t>2025-08-16 11:28:02</t>
+  </si>
+  <si>
+    <t>門市反應lifeet熱感機t70II無反應，電源燈號正常，已有關機紙捲重裝仍無反應...請台芝到店協助(視窗跳掉 熱感機無法列印)</t>
+  </si>
+  <si>
+    <t>THILF02837</t>
+  </si>
+  <si>
+    <t>2025-08-16 11:53:07</t>
+  </si>
+  <si>
+    <t>2025-08-18 08:40:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 09:10:00</t>
+  </si>
+  <si>
+    <t>E4801114081701</t>
+  </si>
+  <si>
+    <t>五股成州店</t>
+  </si>
+  <si>
+    <t>新北市五股區</t>
+  </si>
+  <si>
+    <t>2025-08-17 08:01:26</t>
+  </si>
+  <si>
+    <t>門市反應票券機L90亮紅燈，上蓋卡住打不開，門市告知擔心硬拆機器會故障...請台芝到店協助(票券機無法正常列印以及開蓋重啟，疑似卡紙。)</t>
+  </si>
+  <si>
+    <t>THILF04801</t>
+  </si>
+  <si>
+    <t>2025-08-17 09:02:27</t>
+  </si>
+  <si>
+    <t>2025-08-18 10:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 10:40:00</t>
+  </si>
+  <si>
+    <t>移除電源線 清潔切刀  重開機正常</t>
+  </si>
+  <si>
+    <t>14025114081701</t>
+  </si>
+  <si>
+    <t>2025-08-17 09:20:04</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)螢幕游標會亂跳觸控異常，重啟TM仍異常，螢幕未貼保護貼、文宣，周邊也無商品，因游標飄移嚴重無法執行觸控校正...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-17 09:26:48</t>
+  </si>
+  <si>
+    <t>2025-08-18 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 12:20:00</t>
+  </si>
+  <si>
+    <t>清潔螢幕 移除保護貼 觸控校正</t>
+  </si>
+  <si>
+    <t>13955114081701</t>
+  </si>
+  <si>
+    <t>板橋海龍店</t>
+  </si>
+  <si>
+    <t>2025-08-17 10:52:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/17 11:12 總公司玫君來電啟動緊急叫修:門市反應sc(SHUTTLE6S)點選開啟hishop跳出當前系統異常，請通知門市人員或者重新操作，客服協助重啟sc後卡重新啟動轉圈圈很久，開機後hishop操作緩慢卡頓且TM轉sc出現無法使用資料庫\'tempsb\'...訊息、訂貨3.0顯示應用程式中發生伺服器錯誤無法使用。致電總公司功評確認並回覆:檢視記錄檔發現CT240BX500SSD1 \\\\.\\PHYSICALDRIVE0  240054312960 已重試磁碟 0 (PDO 名稱: \\Device\\00000034) 邏輯區塊位址 0xf47940 上的 IO 操作。第一顆硬碟有異常更換硬碟不備份還原。...請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)																																
+與門市確認帳務做到08/16，與通訊功評確認有收到08/16的銷售																																
+</t>
+  </si>
+  <si>
+    <t>THILF03955</t>
+  </si>
+  <si>
+    <t>2025-08-17 11:16:01</t>
+  </si>
+  <si>
+    <t>2025-08-17 13:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-17 14:33:00</t>
+  </si>
+  <si>
+    <t>2025-08-17 17:16:00</t>
+  </si>
+  <si>
+    <t>更換SC第一顆硬碟無備份還原
+H20250805
+已通知檢查代收</t>
+  </si>
+  <si>
+    <t>2025-08-17 15:47:36</t>
+  </si>
+  <si>
+    <t>2025-08-17 15:45:00</t>
+  </si>
+  <si>
+    <t>五股凌雲店</t>
+  </si>
+  <si>
+    <t>THILF04819</t>
+  </si>
+  <si>
+    <t>2025-08-18 10:33:37</t>
+  </si>
+  <si>
+    <t>2025-08-18 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 10:53:08</t>
+  </si>
+  <si>
+    <t>2025-08-18 10:55:00</t>
+  </si>
+  <si>
+    <t>北縣西雲店</t>
+  </si>
+  <si>
+    <t>THILF03770</t>
+  </si>
+  <si>
+    <t>2025-08-18 11:12:01</t>
+  </si>
+  <si>
+    <t>2025-08-18 11:10:00</t>
+  </si>
+  <si>
+    <t>北縣五泰店</t>
+  </si>
+  <si>
+    <t>THILF02325</t>
+  </si>
+  <si>
+    <t>2025-08-18 11:26:44</t>
+  </si>
+  <si>
+    <t>2025-08-18 12:40:27</t>
+  </si>
+  <si>
+    <t>2025-08-18 12:40:00</t>
+  </si>
+  <si>
+    <t>北縣蘆旺店</t>
+  </si>
+  <si>
+    <t>THILF02958</t>
+  </si>
+  <si>
+    <t>2025-08-18 13:09:52</t>
+  </si>
+  <si>
+    <t>2025-08-18 12:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 13:10:00</t>
   </si>
 </sst>
 </file>
@@ -2451,10 +2657,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK85"/>
+  <dimension ref="A1:AK97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9772,7 +9978,7 @@
       <c r="O85" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="P85" s="8" t="s">
+      <c r="P85" s="9" t="s">
         <v>646</v>
       </c>
       <c r="Q85" s="7" t="s">
@@ -9809,7 +10015,7 @@
       <c r="AB85" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC85" s="8" t="s">
+      <c r="AC85" s="9" t="s">
         <v>643</v>
       </c>
       <c r="AD85" s="7"/>
@@ -9820,6 +10026,1032 @@
       <c r="AI85" s="7"/>
       <c r="AJ85" s="7"/>
       <c r="AK85" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:37">
+      <c r="A86" s="3">
+        <v>84</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C86" s="3">
+        <v>2025082007</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F86" s="3">
+        <v>3929</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L86" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="N86" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="O86" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="P86" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="Q86" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="R86" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S86" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T86" s="3">
+        <v>1</v>
+      </c>
+      <c r="U86" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V86" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="W86" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="X86" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="Y86" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="Z86" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA86" s="3"/>
+      <c r="AB86" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC86" s="10" t="s">
+        <v>660</v>
+      </c>
+      <c r="AD86" s="3"/>
+      <c r="AE86" s="3"/>
+      <c r="AF86" s="3"/>
+      <c r="AG86" s="3"/>
+      <c r="AH86" s="3"/>
+      <c r="AI86" s="3"/>
+      <c r="AJ86" s="3"/>
+      <c r="AK86" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:37">
+      <c r="A87" s="7">
+        <v>85</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C87" s="7">
+        <v>2025082009</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F87" s="7">
+        <v>2837</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="J87" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="K87" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L87" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M87" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N87" s="7">
+        <v>5903</v>
+      </c>
+      <c r="O87" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P87" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="Q87" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="R87" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S87" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T87" s="7">
+        <v>1</v>
+      </c>
+      <c r="U87" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V87" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="W87" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="X87" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="Y87" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="Z87" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA87" s="7"/>
+      <c r="AB87" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="AC87" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD87" s="7"/>
+      <c r="AE87" s="7"/>
+      <c r="AF87" s="7"/>
+      <c r="AG87" s="7"/>
+      <c r="AH87" s="7"/>
+      <c r="AI87" s="7"/>
+      <c r="AJ87" s="7"/>
+      <c r="AK87" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:37">
+      <c r="A88" s="3">
+        <v>86</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C88" s="3">
+        <v>2025082014</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F88" s="3">
+        <v>4801</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L88" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="M88" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="N88" s="3">
+        <v>6003</v>
+      </c>
+      <c r="O88" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P88" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="Q88" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="R88" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S88" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T88" s="3">
+        <v>1</v>
+      </c>
+      <c r="U88" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V88" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="W88" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="X88" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="Y88" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="Z88" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA88" s="3"/>
+      <c r="AB88" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC88" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="AD88" s="3"/>
+      <c r="AE88" s="3"/>
+      <c r="AF88" s="3"/>
+      <c r="AG88" s="3"/>
+      <c r="AH88" s="3"/>
+      <c r="AI88" s="3"/>
+      <c r="AJ88" s="3"/>
+      <c r="AK88" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:37">
+      <c r="A89" s="7">
+        <v>87</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" s="7">
+        <v>2025082015</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>679</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F89" s="7">
+        <v>4025</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>680</v>
+      </c>
+      <c r="J89" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="K89" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L89" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M89" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N89" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O89" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="P89" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="Q89" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="R89" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S89" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T89" s="7">
+        <v>1</v>
+      </c>
+      <c r="U89" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V89" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="W89" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="X89" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="Y89" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="Z89" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA89" s="7"/>
+      <c r="AB89" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC89" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD89" s="7"/>
+      <c r="AE89" s="7"/>
+      <c r="AF89" s="7"/>
+      <c r="AG89" s="7"/>
+      <c r="AH89" s="7"/>
+      <c r="AI89" s="7"/>
+      <c r="AJ89" s="7"/>
+      <c r="AK89" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:37">
+      <c r="A90" s="3">
+        <v>88</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2025082018</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F90" s="3">
+        <v>3955</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N90" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O90" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="P90" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="Q90" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T90" s="3">
+        <v>1</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V90" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="W90" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="X90" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="Y90" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="Z90" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA90" s="3"/>
+      <c r="AB90" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC90" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="AD90" s="3"/>
+      <c r="AE90" s="3"/>
+      <c r="AF90" s="3"/>
+      <c r="AG90" s="3"/>
+      <c r="AH90" s="3"/>
+      <c r="AI90" s="3"/>
+      <c r="AJ90" s="3"/>
+      <c r="AK90" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:37">
+      <c r="A91" s="7">
+        <v>89</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C91" s="7">
+        <v>2025082021</v>
+      </c>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7">
+        <v>3955</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I91" s="7"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="8"/>
+      <c r="N91" s="7"/>
+      <c r="O91" s="8"/>
+      <c r="P91" s="9"/>
+      <c r="Q91" s="7" t="s">
+        <v>690</v>
+      </c>
+      <c r="R91" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S91" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T91" s="7">
+        <v>1</v>
+      </c>
+      <c r="U91" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V91" s="7" t="s">
+        <v>696</v>
+      </c>
+      <c r="W91" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="X91" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y91" s="7"/>
+      <c r="Z91" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC91" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD91" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
+      <c r="AG91" s="7"/>
+      <c r="AH91" s="7"/>
+      <c r="AI91" s="7"/>
+      <c r="AJ91" s="7"/>
+      <c r="AK91" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:37">
+      <c r="A92" s="3">
+        <v>90</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" s="3">
+        <v>2025082068</v>
+      </c>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3">
+        <v>4819</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="10"/>
+      <c r="Q92" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="R92" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T92" s="3">
+        <v>1</v>
+      </c>
+      <c r="U92" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V92" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="W92" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="X92" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="Y92" s="3"/>
+      <c r="Z92" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA92" s="3"/>
+      <c r="AB92" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC92" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD92" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE92" s="3"/>
+      <c r="AF92" s="3"/>
+      <c r="AG92" s="3"/>
+      <c r="AH92" s="3"/>
+      <c r="AI92" s="3"/>
+      <c r="AJ92" s="3"/>
+      <c r="AK92" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:37">
+      <c r="A93" s="7">
+        <v>91</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C93" s="7">
+        <v>2025082072</v>
+      </c>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7">
+        <v>4801</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="I93" s="7"/>
+      <c r="J93" s="7"/>
+      <c r="K93" s="7"/>
+      <c r="L93" s="7"/>
+      <c r="M93" s="8"/>
+      <c r="N93" s="7"/>
+      <c r="O93" s="8"/>
+      <c r="P93" s="9"/>
+      <c r="Q93" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="R93" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S93" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T93" s="7">
+        <v>1</v>
+      </c>
+      <c r="U93" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V93" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="W93" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="X93" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="Y93" s="7"/>
+      <c r="Z93" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA93" s="7"/>
+      <c r="AB93" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC93" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD93" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE93" s="7"/>
+      <c r="AF93" s="7"/>
+      <c r="AG93" s="7"/>
+      <c r="AH93" s="7"/>
+      <c r="AI93" s="7"/>
+      <c r="AJ93" s="7"/>
+      <c r="AK93" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:37">
+      <c r="A94" s="3">
+        <v>92</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C94" s="3">
+        <v>2025082077</v>
+      </c>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3">
+        <v>3770</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="10"/>
+      <c r="Q94" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="R94" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S94" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T94" s="3">
+        <v>1</v>
+      </c>
+      <c r="U94" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V94" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="W94" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="X94" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="Y94" s="3"/>
+      <c r="Z94" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA94" s="3"/>
+      <c r="AB94" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC94" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="AD94" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE94" s="3"/>
+      <c r="AF94" s="3"/>
+      <c r="AG94" s="3"/>
+      <c r="AH94" s="3"/>
+      <c r="AI94" s="3"/>
+      <c r="AJ94" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK94" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:37">
+      <c r="A95" s="7">
+        <v>93</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C95" s="7">
+        <v>2025082084</v>
+      </c>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7">
+        <v>2325</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="I95" s="7"/>
+      <c r="J95" s="7"/>
+      <c r="K95" s="7"/>
+      <c r="L95" s="7"/>
+      <c r="M95" s="8"/>
+      <c r="N95" s="7"/>
+      <c r="O95" s="8"/>
+      <c r="P95" s="9"/>
+      <c r="Q95" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="R95" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S95" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T95" s="7">
+        <v>1</v>
+      </c>
+      <c r="U95" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V95" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="W95" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="X95" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="Y95" s="7"/>
+      <c r="Z95" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA95" s="7"/>
+      <c r="AB95" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC95" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD95" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE95" s="7"/>
+      <c r="AF95" s="7"/>
+      <c r="AG95" s="7"/>
+      <c r="AH95" s="7"/>
+      <c r="AI95" s="7"/>
+      <c r="AJ95" s="7"/>
+      <c r="AK95" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:37">
+      <c r="A96" s="3">
+        <v>94</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C96" s="3">
+        <v>2025082096</v>
+      </c>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3">
+        <v>3929</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="10"/>
+      <c r="Q96" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="R96" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S96" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T96" s="3">
+        <v>1</v>
+      </c>
+      <c r="U96" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V96" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="W96" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="X96" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="Y96" s="3"/>
+      <c r="Z96" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA96" s="3"/>
+      <c r="AB96" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC96" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD96" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE96" s="3"/>
+      <c r="AF96" s="3"/>
+      <c r="AG96" s="3"/>
+      <c r="AH96" s="3"/>
+      <c r="AI96" s="3"/>
+      <c r="AJ96" s="3"/>
+      <c r="AK96" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:37">
+      <c r="A97" s="7">
+        <v>95</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C97" s="7">
+        <v>2025082102</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7">
+        <v>2958</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="H97" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="8"/>
+      <c r="N97" s="7"/>
+      <c r="O97" s="8"/>
+      <c r="P97" s="8"/>
+      <c r="Q97" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="R97" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S97" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T97" s="7">
+        <v>1</v>
+      </c>
+      <c r="U97" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V97" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="W97" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="X97" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="Y97" s="7"/>
+      <c r="Z97" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA97" s="7"/>
+      <c r="AB97" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC97" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD97" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE97" s="7"/>
+      <c r="AF97" s="7"/>
+      <c r="AG97" s="7"/>
+      <c r="AH97" s="7"/>
+      <c r="AI97" s="7"/>
+      <c r="AJ97" s="7"/>
+      <c r="AK97" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08181639
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$97</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$102</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="744">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-18  )</t>
   </si>
@@ -1930,6 +1930,38 @@
     <t>2025-08-15 11:01:00</t>
   </si>
   <si>
+    <t>14145114081501</t>
+  </si>
+  <si>
+    <t>板橋僑興店</t>
+  </si>
+  <si>
+    <t>2025-08-15 11:28:33</t>
+  </si>
+  <si>
+    <t>門市反應TM2-CCD掃描器(HC56II-TR)刷讀所有條碼都感應不良，有亮燈有嗶聲但無入TM，已嘗試執行掃槍校正仍異常..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04145</t>
+  </si>
+  <si>
+    <t>2025-08-15 11:29:50</t>
+  </si>
+  <si>
+    <t>2025-08-18 13:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 15:29:00</t>
+  </si>
+  <si>
+    <t>更換76掃槍
+換上：8118012880
+換下：8119008469</t>
+  </si>
+  <si>
     <t>D138</t>
   </si>
   <si>
@@ -2244,6 +2276,56 @@
   </si>
   <si>
     <t>2025-08-18 13:10:00</t>
+  </si>
+  <si>
+    <t>三重太璞宮</t>
+  </si>
+  <si>
+    <t>THILF04968</t>
+  </si>
+  <si>
+    <t>2025-08-18 13:44:03</t>
+  </si>
+  <si>
+    <t>2025-08-18 13:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 13:40:00</t>
+  </si>
+  <si>
+    <t>14145114081801</t>
+  </si>
+  <si>
+    <t>2025-08-18 14:03:42</t>
+  </si>
+  <si>
+    <t>台芝進線告知有更換TM1 CCD掃描器 需客服協助派工</t>
+  </si>
+  <si>
+    <t>2025-08-18 14:04:47</t>
+  </si>
+  <si>
+    <t>2025-08-19 18:04:00</t>
+  </si>
+  <si>
+    <t>更換76掃槍
+換上：8119011905
+換下：8119008728</t>
+  </si>
+  <si>
+    <t>2025-08-18 14:34:57</t>
+  </si>
+  <si>
+    <t>2025-08-18 15:37:43</t>
+  </si>
+  <si>
+    <t>2025-08-18 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-18 15:31:00</t>
+  </si>
+  <si>
+    <t>PEP安裝完成</t>
   </si>
 </sst>
 </file>
@@ -2657,10 +2739,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK97"/>
+  <dimension ref="A1:AK102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A97" sqref="A97"/>
+      <selection activeCell="AC99" sqref="AC99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9532,38 +9614,58 @@
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C80" s="3">
-        <v>2025081871</v>
-      </c>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3" t="s">
+        <v>2025081870</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>615</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F80" s="3">
+        <v>4145</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>616</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="4"/>
-      <c r="N80" s="3"/>
-      <c r="O80" s="4"/>
-      <c r="P80" s="10"/>
+        <v>206</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K80" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L80" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M80" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="N80" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O80" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P80" s="10" t="s">
+        <v>618</v>
+      </c>
       <c r="Q80" s="3" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="R80" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S80" s="3" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="T80" s="3">
         <v>1</v>
@@ -9572,28 +9674,28 @@
         <v>53</v>
       </c>
       <c r="V80" s="3" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="W80" s="3" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="X80" s="3" t="s">
-        <v>620</v>
-      </c>
-      <c r="Y80" s="3"/>
+        <v>622</v>
+      </c>
+      <c r="Y80" s="3" t="s">
+        <v>623</v>
+      </c>
       <c r="Z80" s="3">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="AA80" s="3"/>
       <c r="AB80" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC80" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD80" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>624</v>
+      </c>
+      <c r="AD80" s="3"/>
       <c r="AE80" s="3"/>
       <c r="AF80" s="3"/>
       <c r="AG80" s="3"/>
@@ -9612,15 +9714,15 @@
         <v>78</v>
       </c>
       <c r="C81" s="7">
-        <v>2025081894</v>
+        <v>2025081871</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
       <c r="F81" s="7" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="H81" s="7" t="s">
         <v>42</v>
@@ -9634,7 +9736,7 @@
       <c r="O81" s="8"/>
       <c r="P81" s="9"/>
       <c r="Q81" s="7" t="s">
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="R81" s="7" t="s">
         <v>51</v>
@@ -9649,24 +9751,24 @@
         <v>53</v>
       </c>
       <c r="V81" s="7" t="s">
-        <v>621</v>
+        <v>628</v>
       </c>
       <c r="W81" s="7" t="s">
-        <v>619</v>
+        <v>629</v>
       </c>
       <c r="X81" s="7" t="s">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="Y81" s="7"/>
       <c r="Z81" s="7">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="AA81" s="7"/>
       <c r="AB81" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC81" s="9" t="s">
-        <v>623</v>
+        <v>84</v>
       </c>
       <c r="AD81" s="7" t="s">
         <v>60</v>
@@ -9689,15 +9791,15 @@
         <v>78</v>
       </c>
       <c r="C82" s="3">
-        <v>2025081895</v>
+        <v>2025081894</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="3">
-        <v>3601</v>
+      <c r="F82" s="3" t="s">
+        <v>625</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>42</v>
@@ -9711,7 +9813,7 @@
       <c r="O82" s="4"/>
       <c r="P82" s="10"/>
       <c r="Q82" s="3" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="R82" s="3" t="s">
         <v>51</v>
@@ -9726,13 +9828,13 @@
         <v>53</v>
       </c>
       <c r="V82" s="3" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="W82" s="3" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="X82" s="3" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="Y82" s="3"/>
       <c r="Z82" s="3">
@@ -9743,7 +9845,7 @@
         <v>58</v>
       </c>
       <c r="AC82" s="10" t="s">
-        <v>84</v>
+        <v>633</v>
       </c>
       <c r="AD82" s="3" t="s">
         <v>60</v>
@@ -9766,15 +9868,15 @@
         <v>78</v>
       </c>
       <c r="C83" s="7">
-        <v>2025081898</v>
+        <v>2025081895</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7">
-        <v>4698</v>
+        <v>3601</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
       <c r="H83" s="7" t="s">
         <v>42</v>
@@ -9788,7 +9890,7 @@
       <c r="O83" s="8"/>
       <c r="P83" s="9"/>
       <c r="Q83" s="7" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="R83" s="7" t="s">
         <v>51</v>
@@ -9803,13 +9905,13 @@
         <v>53</v>
       </c>
       <c r="V83" s="7" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="W83" s="7" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="X83" s="7" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="Y83" s="7"/>
       <c r="Z83" s="7">
@@ -9820,7 +9922,7 @@
         <v>58</v>
       </c>
       <c r="AC83" s="9" t="s">
-        <v>479</v>
+        <v>84</v>
       </c>
       <c r="AD83" s="7" t="s">
         <v>60</v>
@@ -9840,52 +9942,32 @@
         <v>82</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C84" s="3">
-        <v>2025081905</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>2025081898</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
       <c r="F84" s="3">
-        <v>4098</v>
+        <v>4698</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I84" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="J84" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K84" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="L84" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="M84" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="N84" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="O84" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="P84" s="10" t="s">
-        <v>637</v>
-      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="10"/>
       <c r="Q84" s="3" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="R84" s="3" t="s">
         <v>51</v>
@@ -9900,28 +9982,28 @@
         <v>53</v>
       </c>
       <c r="V84" s="3" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="W84" s="3" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="X84" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="Y84" s="3" t="s">
-        <v>642</v>
-      </c>
+        <v>643</v>
+      </c>
+      <c r="Y84" s="3"/>
       <c r="Z84" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA84" s="3"/>
       <c r="AB84" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC84" s="10" t="s">
-        <v>643</v>
-      </c>
-      <c r="AD84" s="3"/>
+        <v>479</v>
+      </c>
+      <c r="AD84" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AE84" s="3"/>
       <c r="AF84" s="3"/>
       <c r="AG84" s="3"/>
@@ -9940,25 +10022,25 @@
         <v>38</v>
       </c>
       <c r="C85" s="7">
-        <v>2025081923</v>
+        <v>2025081905</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>644</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>382</v>
+        <v>40</v>
       </c>
       <c r="F85" s="7">
         <v>4098</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>635</v>
+        <v>645</v>
       </c>
       <c r="H85" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I85" s="7" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="J85" s="7" t="s">
         <v>66</v>
@@ -9979,10 +10061,10 @@
         <v>122</v>
       </c>
       <c r="P85" s="9" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="Q85" s="7" t="s">
-        <v>638</v>
+        <v>648</v>
       </c>
       <c r="R85" s="7" t="s">
         <v>51</v>
@@ -9997,16 +10079,16 @@
         <v>53</v>
       </c>
       <c r="V85" s="7" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="W85" s="7" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="X85" s="7" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="Y85" s="7" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="Z85" s="7">
         <v>0.5</v>
@@ -10016,7 +10098,7 @@
         <v>58</v>
       </c>
       <c r="AC85" s="9" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="AD85" s="7"/>
       <c r="AE85" s="7"/>
@@ -10037,49 +10119,49 @@
         <v>38</v>
       </c>
       <c r="C86" s="3">
-        <v>2025082007</v>
+        <v>2025081923</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>40</v>
+        <v>382</v>
       </c>
       <c r="F86" s="3">
-        <v>3929</v>
+        <v>4098</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>534</v>
+        <v>42</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="N86" s="3" t="s">
-        <v>254</v>
+        <v>121</v>
       </c>
       <c r="O86" s="4" t="s">
-        <v>255</v>
+        <v>122</v>
       </c>
       <c r="P86" s="10" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="Q86" s="3" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="R86" s="3" t="s">
         <v>51</v>
@@ -10094,26 +10176,26 @@
         <v>53</v>
       </c>
       <c r="V86" s="3" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="W86" s="3" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="X86" s="3" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="Y86" s="3" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="Z86" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA86" s="3"/>
       <c r="AB86" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC86" s="10" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="AD86" s="3"/>
       <c r="AE86" s="3"/>
@@ -10134,7 +10216,7 @@
         <v>38</v>
       </c>
       <c r="C87" s="7">
-        <v>2025082009</v>
+        <v>2025082007</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>661</v>
@@ -10143,13 +10225,13 @@
         <v>40</v>
       </c>
       <c r="F87" s="7">
-        <v>2837</v>
+        <v>3929</v>
       </c>
       <c r="G87" s="7" t="s">
         <v>662</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>42</v>
+        <v>534</v>
       </c>
       <c r="I87" s="7" t="s">
         <v>663</v>
@@ -10161,16 +10243,16 @@
         <v>45</v>
       </c>
       <c r="L87" s="7" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="M87" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N87" s="7">
-        <v>5903</v>
+        <v>178</v>
+      </c>
+      <c r="N87" s="7" t="s">
+        <v>254</v>
       </c>
       <c r="O87" s="8" t="s">
-        <v>48</v>
+        <v>255</v>
       </c>
       <c r="P87" s="9" t="s">
         <v>664</v>
@@ -10200,17 +10282,17 @@
         <v>668</v>
       </c>
       <c r="Y87" s="7" t="s">
-        <v>659</v>
+        <v>669</v>
       </c>
       <c r="Z87" s="7">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA87" s="7"/>
       <c r="AB87" s="7" t="s">
-        <v>346</v>
+        <v>58</v>
       </c>
       <c r="AC87" s="9" t="s">
-        <v>346</v>
+        <v>670</v>
       </c>
       <c r="AD87" s="7"/>
       <c r="AE87" s="7"/>
@@ -10231,55 +10313,55 @@
         <v>38</v>
       </c>
       <c r="C88" s="3">
-        <v>2025082014</v>
+        <v>2025082009</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F88" s="3">
-        <v>4801</v>
+        <v>2837</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>671</v>
+        <v>42</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="K88" s="3" t="s">
         <v>45</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>276</v>
+        <v>46</v>
       </c>
       <c r="M88" s="4" t="s">
-        <v>277</v>
+        <v>47</v>
       </c>
       <c r="N88" s="3">
-        <v>6003</v>
+        <v>5903</v>
       </c>
       <c r="O88" s="4" t="s">
         <v>48</v>
       </c>
       <c r="P88" s="10" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="Q88" s="3" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="R88" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S88" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T88" s="3">
         <v>1</v>
@@ -10288,26 +10370,26 @@
         <v>53</v>
       </c>
       <c r="V88" s="3" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="W88" s="3" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="X88" s="3" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Y88" s="3" t="s">
-        <v>659</v>
+        <v>669</v>
       </c>
       <c r="Z88" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA88" s="3"/>
       <c r="AB88" s="3" t="s">
-        <v>58</v>
+        <v>346</v>
       </c>
       <c r="AC88" s="10" t="s">
-        <v>678</v>
+        <v>346</v>
       </c>
       <c r="AD88" s="3"/>
       <c r="AE88" s="3"/>
@@ -10328,7 +10410,7 @@
         <v>38</v>
       </c>
       <c r="C89" s="7">
-        <v>2025082015</v>
+        <v>2025082014</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>679</v>
@@ -10337,16 +10419,16 @@
         <v>40</v>
       </c>
       <c r="F89" s="7">
-        <v>4025</v>
+        <v>4801</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>314</v>
+        <v>680</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>64</v>
+        <v>681</v>
       </c>
       <c r="I89" s="7" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="J89" s="7" t="s">
         <v>155</v>
@@ -10355,22 +10437,22 @@
         <v>45</v>
       </c>
       <c r="L89" s="7" t="s">
-        <v>197</v>
+        <v>276</v>
       </c>
       <c r="M89" s="8" t="s">
-        <v>198</v>
+        <v>277</v>
       </c>
       <c r="N89" s="7">
-        <v>2307</v>
+        <v>6003</v>
       </c>
       <c r="O89" s="8" t="s">
-        <v>525</v>
+        <v>48</v>
       </c>
       <c r="P89" s="9" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="Q89" s="7" t="s">
-        <v>315</v>
+        <v>684</v>
       </c>
       <c r="R89" s="7" t="s">
         <v>51</v>
@@ -10385,26 +10467,26 @@
         <v>53</v>
       </c>
       <c r="V89" s="7" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="W89" s="7" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="X89" s="7" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="Y89" s="7" t="s">
-        <v>659</v>
+        <v>669</v>
       </c>
       <c r="Z89" s="7">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="AA89" s="7"/>
       <c r="AB89" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC89" s="9" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="AD89" s="7"/>
       <c r="AE89" s="7"/>
@@ -10425,25 +10507,25 @@
         <v>38</v>
       </c>
       <c r="C90" s="3">
-        <v>2025082018</v>
+        <v>2025082015</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>382</v>
+        <v>40</v>
       </c>
       <c r="F90" s="3">
-        <v>3955</v>
+        <v>4025</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>687</v>
+        <v>314</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>206</v>
+        <v>64</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="J90" s="3" t="s">
         <v>155</v>
@@ -10452,28 +10534,28 @@
         <v>45</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="M90" s="4" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
       <c r="N90" s="3">
-        <v>2405</v>
+        <v>2307</v>
       </c>
       <c r="O90" s="4" t="s">
-        <v>386</v>
+        <v>525</v>
       </c>
       <c r="P90" s="10" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="Q90" s="3" t="s">
-        <v>690</v>
+        <v>315</v>
       </c>
       <c r="R90" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S90" s="3" t="s">
-        <v>210</v>
+        <v>72</v>
       </c>
       <c r="T90" s="3">
         <v>1</v>
@@ -10482,19 +10564,19 @@
         <v>53</v>
       </c>
       <c r="V90" s="3" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="W90" s="3" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="X90" s="3" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="Y90" s="3" t="s">
-        <v>694</v>
+        <v>669</v>
       </c>
       <c r="Z90" s="3">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="AA90" s="3"/>
       <c r="AB90" s="3" t="s">
@@ -10519,32 +10601,52 @@
         <v>89</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C91" s="7">
-        <v>2025082021</v>
-      </c>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
+        <v>2025082018</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>696</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>382</v>
+      </c>
       <c r="F91" s="7">
         <v>3955</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>687</v>
+        <v>697</v>
       </c>
       <c r="H91" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="I91" s="7"/>
-      <c r="J91" s="7"/>
-      <c r="K91" s="7"/>
-      <c r="L91" s="7"/>
-      <c r="M91" s="8"/>
-      <c r="N91" s="7"/>
-      <c r="O91" s="8"/>
-      <c r="P91" s="9"/>
+      <c r="I91" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="J91" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="K91" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L91" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M91" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N91" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O91" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="P91" s="9" t="s">
+        <v>699</v>
+      </c>
       <c r="Q91" s="7" t="s">
-        <v>690</v>
+        <v>700</v>
       </c>
       <c r="R91" s="7" t="s">
         <v>51</v>
@@ -10559,28 +10661,28 @@
         <v>53</v>
       </c>
       <c r="V91" s="7" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
       <c r="W91" s="7" t="s">
-        <v>692</v>
+        <v>702</v>
       </c>
       <c r="X91" s="7" t="s">
-        <v>697</v>
-      </c>
-      <c r="Y91" s="7"/>
+        <v>703</v>
+      </c>
+      <c r="Y91" s="7" t="s">
+        <v>704</v>
+      </c>
       <c r="Z91" s="7">
-        <v>1.9</v>
+        <v>0.7</v>
       </c>
       <c r="AA91" s="7"/>
       <c r="AB91" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC91" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD91" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>705</v>
+      </c>
+      <c r="AD91" s="7"/>
       <c r="AE91" s="7"/>
       <c r="AF91" s="7"/>
       <c r="AG91" s="7"/>
@@ -10599,18 +10701,18 @@
         <v>78</v>
       </c>
       <c r="C92" s="3">
-        <v>2025082068</v>
+        <v>2025082021</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3">
-        <v>4819</v>
+        <v>3955</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>671</v>
+        <v>206</v>
       </c>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
@@ -10621,13 +10723,13 @@
       <c r="O92" s="4"/>
       <c r="P92" s="10"/>
       <c r="Q92" s="3" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="R92" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S92" s="3" t="s">
-        <v>72</v>
+        <v>210</v>
       </c>
       <c r="T92" s="3">
         <v>1</v>
@@ -10636,17 +10738,17 @@
         <v>53</v>
       </c>
       <c r="V92" s="3" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
       <c r="W92" s="3" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="X92" s="3" t="s">
-        <v>676</v>
+        <v>707</v>
       </c>
       <c r="Y92" s="3"/>
       <c r="Z92" s="3">
-        <v>0.3</v>
+        <v>1.9</v>
       </c>
       <c r="AA92" s="3"/>
       <c r="AB92" s="3" t="s">
@@ -10676,18 +10778,18 @@
         <v>78</v>
       </c>
       <c r="C93" s="7">
-        <v>2025082072</v>
+        <v>2025082068</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
       <c r="F93" s="7">
-        <v>4801</v>
+        <v>4819</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>670</v>
+        <v>708</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>671</v>
+        <v>681</v>
       </c>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
@@ -10698,7 +10800,7 @@
       <c r="O93" s="8"/>
       <c r="P93" s="9"/>
       <c r="Q93" s="7" t="s">
-        <v>674</v>
+        <v>709</v>
       </c>
       <c r="R93" s="7" t="s">
         <v>51</v>
@@ -10713,13 +10815,13 @@
         <v>53</v>
       </c>
       <c r="V93" s="7" t="s">
-        <v>702</v>
+        <v>710</v>
       </c>
       <c r="W93" s="7" t="s">
-        <v>677</v>
+        <v>711</v>
       </c>
       <c r="X93" s="7" t="s">
-        <v>703</v>
+        <v>686</v>
       </c>
       <c r="Y93" s="7"/>
       <c r="Z93" s="7">
@@ -10753,18 +10855,18 @@
         <v>78</v>
       </c>
       <c r="C94" s="3">
-        <v>2025082077</v>
+        <v>2025082072</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3">
-        <v>3770</v>
+        <v>4801</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>704</v>
+        <v>680</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>671</v>
+        <v>681</v>
       </c>
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
@@ -10775,7 +10877,7 @@
       <c r="O94" s="4"/>
       <c r="P94" s="10"/>
       <c r="Q94" s="3" t="s">
-        <v>705</v>
+        <v>684</v>
       </c>
       <c r="R94" s="3" t="s">
         <v>51</v>
@@ -10790,13 +10892,13 @@
         <v>53</v>
       </c>
       <c r="V94" s="3" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="W94" s="3" t="s">
-        <v>703</v>
+        <v>687</v>
       </c>
       <c r="X94" s="3" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
       <c r="Y94" s="3"/>
       <c r="Z94" s="3">
@@ -10807,7 +10909,7 @@
         <v>58</v>
       </c>
       <c r="AC94" s="10" t="s">
-        <v>479</v>
+        <v>84</v>
       </c>
       <c r="AD94" s="3" t="s">
         <v>60</v>
@@ -10817,9 +10919,7 @@
       <c r="AG94" s="3"/>
       <c r="AH94" s="3"/>
       <c r="AI94" s="3"/>
-      <c r="AJ94" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ94" s="3"/>
       <c r="AK94" s="3" t="s">
         <v>60</v>
       </c>
@@ -10832,18 +10932,18 @@
         <v>78</v>
       </c>
       <c r="C95" s="7">
-        <v>2025082084</v>
+        <v>2025082077</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
       <c r="F95" s="7">
-        <v>2325</v>
+        <v>3770</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>671</v>
+        <v>681</v>
       </c>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
@@ -10854,7 +10954,7 @@
       <c r="O95" s="8"/>
       <c r="P95" s="9"/>
       <c r="Q95" s="7" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="R95" s="7" t="s">
         <v>51</v>
@@ -10869,13 +10969,13 @@
         <v>53</v>
       </c>
       <c r="V95" s="7" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="W95" s="7" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
       <c r="X95" s="7" t="s">
-        <v>683</v>
+        <v>717</v>
       </c>
       <c r="Y95" s="7"/>
       <c r="Z95" s="7">
@@ -10886,7 +10986,7 @@
         <v>58</v>
       </c>
       <c r="AC95" s="9" t="s">
-        <v>84</v>
+        <v>479</v>
       </c>
       <c r="AD95" s="7" t="s">
         <v>60</v>
@@ -10896,7 +10996,9 @@
       <c r="AG95" s="7"/>
       <c r="AH95" s="7"/>
       <c r="AI95" s="7"/>
-      <c r="AJ95" s="7"/>
+      <c r="AJ95" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AK95" s="7" t="s">
         <v>60</v>
       </c>
@@ -10909,18 +11011,18 @@
         <v>78</v>
       </c>
       <c r="C96" s="3">
-        <v>2025082096</v>
+        <v>2025082084</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3">
-        <v>3929</v>
+        <v>2325</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>652</v>
+        <v>718</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>534</v>
+        <v>681</v>
       </c>
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
@@ -10931,13 +11033,13 @@
       <c r="O96" s="4"/>
       <c r="P96" s="10"/>
       <c r="Q96" s="3" t="s">
-        <v>655</v>
+        <v>719</v>
       </c>
       <c r="R96" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S96" s="3" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T96" s="3">
         <v>1</v>
@@ -10946,13 +11048,13 @@
         <v>53</v>
       </c>
       <c r="V96" s="3" t="s">
-        <v>711</v>
+        <v>720</v>
       </c>
       <c r="W96" s="3" t="s">
-        <v>684</v>
+        <v>717</v>
       </c>
       <c r="X96" s="3" t="s">
-        <v>712</v>
+        <v>693</v>
       </c>
       <c r="Y96" s="3"/>
       <c r="Z96" s="3">
@@ -10986,15 +11088,15 @@
         <v>78</v>
       </c>
       <c r="C97" s="7">
-        <v>2025082102</v>
+        <v>2025082096</v>
       </c>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
       <c r="F97" s="7">
-        <v>2958</v>
+        <v>3929</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>713</v>
+        <v>662</v>
       </c>
       <c r="H97" s="7" t="s">
         <v>534</v>
@@ -11006,9 +11108,9 @@
       <c r="M97" s="8"/>
       <c r="N97" s="7"/>
       <c r="O97" s="8"/>
-      <c r="P97" s="8"/>
+      <c r="P97" s="9"/>
       <c r="Q97" s="7" t="s">
-        <v>714</v>
+        <v>665</v>
       </c>
       <c r="R97" s="7" t="s">
         <v>51</v>
@@ -11023,13 +11125,13 @@
         <v>53</v>
       </c>
       <c r="V97" s="7" t="s">
-        <v>715</v>
+        <v>721</v>
       </c>
       <c r="W97" s="7" t="s">
-        <v>716</v>
+        <v>694</v>
       </c>
       <c r="X97" s="7" t="s">
-        <v>717</v>
+        <v>722</v>
       </c>
       <c r="Y97" s="7"/>
       <c r="Z97" s="7">
@@ -11039,7 +11141,7 @@
       <c r="AB97" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC97" s="8" t="s">
+      <c r="AC97" s="9" t="s">
         <v>84</v>
       </c>
       <c r="AD97" s="7" t="s">
@@ -11052,6 +11154,411 @@
       <c r="AI97" s="7"/>
       <c r="AJ97" s="7"/>
       <c r="AK97" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:37">
+      <c r="A98" s="3">
+        <v>96</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C98" s="3">
+        <v>2025082102</v>
+      </c>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3">
+        <v>2958</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="3"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="R98" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S98" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T98" s="3">
+        <v>1</v>
+      </c>
+      <c r="U98" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V98" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="W98" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="X98" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="Y98" s="3"/>
+      <c r="Z98" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA98" s="3"/>
+      <c r="AB98" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC98" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD98" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE98" s="3"/>
+      <c r="AF98" s="3"/>
+      <c r="AG98" s="3"/>
+      <c r="AH98" s="3"/>
+      <c r="AI98" s="3"/>
+      <c r="AJ98" s="3"/>
+      <c r="AK98" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:37">
+      <c r="A99" s="7">
+        <v>97</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C99" s="7">
+        <v>2025082105</v>
+      </c>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7">
+        <v>4968</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I99" s="7"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+      <c r="L99" s="7"/>
+      <c r="M99" s="8"/>
+      <c r="N99" s="7"/>
+      <c r="O99" s="8"/>
+      <c r="P99" s="9"/>
+      <c r="Q99" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="R99" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S99" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T99" s="7">
+        <v>1</v>
+      </c>
+      <c r="U99" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V99" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="W99" s="7" t="s">
+        <v>731</v>
+      </c>
+      <c r="X99" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="Y99" s="7"/>
+      <c r="Z99" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA99" s="7"/>
+      <c r="AB99" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC99" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD99" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE99" s="7"/>
+      <c r="AF99" s="7"/>
+      <c r="AG99" s="7"/>
+      <c r="AH99" s="7"/>
+      <c r="AI99" s="7"/>
+      <c r="AJ99" s="7"/>
+      <c r="AK99" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:37">
+      <c r="A100" s="3">
+        <v>98</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C100" s="3">
+        <v>2025082114</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F100" s="3">
+        <v>4145</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L100" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M100" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="N100" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O100" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P100" s="10" t="s">
+        <v>735</v>
+      </c>
+      <c r="Q100" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="R100" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S100" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T100" s="3">
+        <v>1</v>
+      </c>
+      <c r="U100" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V100" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="W100" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="X100" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y100" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="Z100" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA100" s="3"/>
+      <c r="AB100" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC100" s="10" t="s">
+        <v>738</v>
+      </c>
+      <c r="AD100" s="3"/>
+      <c r="AE100" s="3"/>
+      <c r="AF100" s="3"/>
+      <c r="AG100" s="3"/>
+      <c r="AH100" s="3"/>
+      <c r="AI100" s="3"/>
+      <c r="AJ100" s="3"/>
+      <c r="AK100" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:37">
+      <c r="A101" s="7">
+        <v>99</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C101" s="7">
+        <v>2025082122</v>
+      </c>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7">
+        <v>4145</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I101" s="7"/>
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+      <c r="L101" s="7"/>
+      <c r="M101" s="8"/>
+      <c r="N101" s="7"/>
+      <c r="O101" s="8"/>
+      <c r="P101" s="9"/>
+      <c r="Q101" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="R101" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S101" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T101" s="7">
+        <v>1</v>
+      </c>
+      <c r="U101" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V101" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="W101" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="X101" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y101" s="7"/>
+      <c r="Z101" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA101" s="7"/>
+      <c r="AB101" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC101" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD101" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE101" s="7"/>
+      <c r="AF101" s="7"/>
+      <c r="AG101" s="7"/>
+      <c r="AH101" s="7"/>
+      <c r="AI101" s="7"/>
+      <c r="AJ101" s="7"/>
+      <c r="AK101" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:37">
+      <c r="A102" s="3">
+        <v>100</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C102" s="3">
+        <v>2025082152</v>
+      </c>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3">
+        <v>5384</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="R102" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S102" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T102" s="3">
+        <v>1</v>
+      </c>
+      <c r="U102" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V102" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="W102" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="X102" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="Y102" s="3"/>
+      <c r="Z102" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA102" s="3"/>
+      <c r="AB102" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC102" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="AD102" s="3"/>
+      <c r="AE102" s="3"/>
+      <c r="AF102" s="3"/>
+      <c r="AG102" s="3"/>
+      <c r="AH102" s="3"/>
+      <c r="AI102" s="3"/>
+      <c r="AJ102" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK102" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08201105
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$102</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$107</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="744">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-18  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="780">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-20  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2257,6 +2257,65 @@
     <t>2025-08-18 11:26:44</t>
   </si>
   <si>
+    <t>E4538114081801</t>
+  </si>
+  <si>
+    <t>林口童樂店</t>
+  </si>
+  <si>
+    <t>2025-08-18 11:42:21</t>
+  </si>
+  <si>
+    <t>門市反應sc滑鼠有時候點左鍵一下但在電腦顯示會變兩下導致使用上困難，已重新拔插線路仍異常...須請台芝到店協助(後場電腦，滑鼠左鍵常常點1下變成2下或者沒反應，掃描器的按鍵很長卡著)</t>
+  </si>
+  <si>
+    <t>THILF04538</t>
+  </si>
+  <si>
+    <t>2025-08-18 11:56:59</t>
+  </si>
+  <si>
+    <t>2025-08-19 09:29:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 09:59:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 15:57:00</t>
+  </si>
+  <si>
+    <t>14538114081802</t>
+  </si>
+  <si>
+    <t>2025-08-18 11:57:09</t>
+  </si>
+  <si>
+    <t>HL29</t>
+  </si>
+  <si>
+    <t>HL-CCD掃描器(SC)</t>
+  </si>
+  <si>
+    <t>門市反應SC CCD掃描器(AT20B)按按鍵時常常按鍵會陷進去卡住....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-18 11:58:25</t>
+  </si>
+  <si>
+    <t>2025-08-19 09:28:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 09:58:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 15:58:00</t>
+  </si>
+  <si>
+    <t>更換SC掃描槍
+換下8119012010
+換上8119013107</t>
+  </si>
+  <si>
     <t>2025-08-18 12:40:27</t>
   </si>
   <si>
@@ -2316,16 +2375,73 @@
     <t>2025-08-18 14:34:57</t>
   </si>
   <si>
+    <t>14312114081802</t>
+  </si>
+  <si>
+    <t>2025-08-18 15:27:54</t>
+  </si>
+  <si>
+    <t>門市反應在TM2熱感發票機(BSC10II)大夜時會發生不定時未出發票，當下設備燈號正常，此筆已作廢，後續門市未操作任何排除動作，下一筆交易結帳即都有正常出紙，經HIPOS查看Eventlog無異常，發票檔內有此筆發票，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。08/01門市已反應列印發票或收據下半部空白過長才裁切，08/04台芝到場確認線路及列印皆為正常，請門市在進行觀察...需請台芝到店確認</t>
+  </si>
+  <si>
+    <t>2025-08-18 15:31:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 11:27:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 11:57:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 19:31:00</t>
+  </si>
+  <si>
+    <t>原發票機測試正常無異常，更換備品再測試
+更換發票機
+換下8155004446
+換上8155006317</t>
+  </si>
+  <si>
     <t>2025-08-18 15:37:43</t>
   </si>
   <si>
     <t>2025-08-18 15:00:00</t>
   </si>
   <si>
-    <t>2025-08-18 15:31:00</t>
-  </si>
-  <si>
     <t>PEP安裝完成</t>
+  </si>
+  <si>
+    <t>13929114081801</t>
+  </si>
+  <si>
+    <t>2025-08-18 16:16:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應TM1多卡機(QP3000E)再次無電源反應無畫面，門市已有重新拔插後方線路仍異常(門市於8/16報修相同問題案13929114081601台芝8/18 12:10回覆:檢查變壓器插上後，通電正常，可正常使用 100% )
+</t>
+  </si>
+  <si>
+    <t>2025-08-18 16:19:24</t>
+  </si>
+  <si>
+    <t>2025-08-19 12:27:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 20:19:00</t>
+  </si>
+  <si>
+    <t>更換多卡機
+換下8183000272
+換上8183000007</t>
+  </si>
+  <si>
+    <t>2025-08-19 10:18:52</t>
+  </si>
+  <si>
+    <t>2025-08-19 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-19 10:18:00</t>
   </si>
 </sst>
 </file>
@@ -2739,10 +2855,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK102"/>
+  <dimension ref="A1:AK107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC99" sqref="AC99"/>
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11085,32 +11201,52 @@
         <v>95</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C97" s="7">
-        <v>2025082096</v>
-      </c>
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
+        <v>2025082091</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F97" s="7">
-        <v>3929</v>
+        <v>4538</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>662</v>
+        <v>722</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>534</v>
-      </c>
-      <c r="I97" s="7"/>
-      <c r="J97" s="7"/>
-      <c r="K97" s="7"/>
-      <c r="L97" s="7"/>
-      <c r="M97" s="8"/>
-      <c r="N97" s="7"/>
-      <c r="O97" s="8"/>
-      <c r="P97" s="9"/>
+        <v>153</v>
+      </c>
+      <c r="I97" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="J97" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K97" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L97" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M97" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N97" s="7">
+        <v>2403</v>
+      </c>
+      <c r="O97" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P97" s="9" t="s">
+        <v>724</v>
+      </c>
       <c r="Q97" s="7" t="s">
-        <v>665</v>
+        <v>725</v>
       </c>
       <c r="R97" s="7" t="s">
         <v>51</v>
@@ -11125,28 +11261,28 @@
         <v>53</v>
       </c>
       <c r="V97" s="7" t="s">
-        <v>721</v>
+        <v>726</v>
       </c>
       <c r="W97" s="7" t="s">
-        <v>694</v>
+        <v>727</v>
       </c>
       <c r="X97" s="7" t="s">
-        <v>722</v>
-      </c>
-      <c r="Y97" s="7"/>
+        <v>728</v>
+      </c>
+      <c r="Y97" s="7" t="s">
+        <v>729</v>
+      </c>
       <c r="Z97" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA97" s="7"/>
       <c r="AB97" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC97" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD97" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="AD97" s="7"/>
       <c r="AE97" s="7"/>
       <c r="AF97" s="7"/>
       <c r="AG97" s="7"/>
@@ -11162,32 +11298,52 @@
         <v>96</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C98" s="3">
-        <v>2025082102</v>
-      </c>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
+        <v>2025082092</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F98" s="3">
-        <v>2958</v>
+        <v>4538</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="I98" s="3"/>
-      <c r="J98" s="3"/>
-      <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
-      <c r="M98" s="4"/>
-      <c r="N98" s="3"/>
-      <c r="O98" s="4"/>
-      <c r="P98" s="10"/>
+        <v>153</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L98" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="N98" s="3">
+        <v>2901</v>
+      </c>
+      <c r="O98" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P98" s="10" t="s">
+        <v>734</v>
+      </c>
       <c r="Q98" s="3" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="R98" s="3" t="s">
         <v>51</v>
@@ -11202,28 +11358,28 @@
         <v>53</v>
       </c>
       <c r="V98" s="3" t="s">
-        <v>725</v>
+        <v>735</v>
       </c>
       <c r="W98" s="3" t="s">
-        <v>726</v>
+        <v>736</v>
       </c>
       <c r="X98" s="3" t="s">
-        <v>727</v>
-      </c>
-      <c r="Y98" s="3"/>
+        <v>737</v>
+      </c>
+      <c r="Y98" s="3" t="s">
+        <v>738</v>
+      </c>
       <c r="Z98" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA98" s="3"/>
       <c r="AB98" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC98" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD98" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>739</v>
+      </c>
+      <c r="AD98" s="3"/>
       <c r="AE98" s="3"/>
       <c r="AF98" s="3"/>
       <c r="AG98" s="3"/>
@@ -11242,18 +11398,18 @@
         <v>78</v>
       </c>
       <c r="C99" s="7">
-        <v>2025082105</v>
+        <v>2025082096</v>
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7">
-        <v>4968</v>
+        <v>3929</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>728</v>
+        <v>662</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>42</v>
+        <v>534</v>
       </c>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
@@ -11264,7 +11420,7 @@
       <c r="O99" s="8"/>
       <c r="P99" s="9"/>
       <c r="Q99" s="7" t="s">
-        <v>729</v>
+        <v>665</v>
       </c>
       <c r="R99" s="7" t="s">
         <v>51</v>
@@ -11279,13 +11435,13 @@
         <v>53</v>
       </c>
       <c r="V99" s="7" t="s">
-        <v>730</v>
+        <v>740</v>
       </c>
       <c r="W99" s="7" t="s">
-        <v>731</v>
+        <v>694</v>
       </c>
       <c r="X99" s="7" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="Y99" s="7"/>
       <c r="Z99" s="7">
@@ -11316,58 +11472,38 @@
         <v>98</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C100" s="3">
-        <v>2025082114</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>2025082102</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
       <c r="F100" s="3">
-        <v>4145</v>
+        <v>2958</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>616</v>
+        <v>742</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="I100" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="J100" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="K100" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="L100" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="M100" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="N100" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="O100" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="P100" s="10" t="s">
-        <v>735</v>
-      </c>
+        <v>534</v>
+      </c>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="3"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="10"/>
       <c r="Q100" s="3" t="s">
-        <v>619</v>
+        <v>743</v>
       </c>
       <c r="R100" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S100" s="3" t="s">
-        <v>210</v>
+        <v>52</v>
       </c>
       <c r="T100" s="3">
         <v>1</v>
@@ -11376,28 +11512,28 @@
         <v>53</v>
       </c>
       <c r="V100" s="3" t="s">
-        <v>736</v>
+        <v>744</v>
       </c>
       <c r="W100" s="3" t="s">
-        <v>621</v>
+        <v>745</v>
       </c>
       <c r="X100" s="3" t="s">
-        <v>622</v>
-      </c>
-      <c r="Y100" s="3" t="s">
-        <v>737</v>
-      </c>
+        <v>746</v>
+      </c>
+      <c r="Y100" s="3"/>
       <c r="Z100" s="3">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="AA100" s="3"/>
       <c r="AB100" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC100" s="10" t="s">
-        <v>738</v>
-      </c>
-      <c r="AD100" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="AD100" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AE100" s="3"/>
       <c r="AF100" s="3"/>
       <c r="AG100" s="3"/>
@@ -11416,18 +11552,18 @@
         <v>78</v>
       </c>
       <c r="C101" s="7">
-        <v>2025082122</v>
+        <v>2025082105</v>
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
       <c r="F101" s="7">
-        <v>4145</v>
+        <v>4968</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>616</v>
+        <v>747</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>206</v>
+        <v>42</v>
       </c>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
@@ -11438,13 +11574,13 @@
       <c r="O101" s="8"/>
       <c r="P101" s="9"/>
       <c r="Q101" s="7" t="s">
-        <v>619</v>
+        <v>748</v>
       </c>
       <c r="R101" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S101" s="7" t="s">
-        <v>210</v>
+        <v>52</v>
       </c>
       <c r="T101" s="7">
         <v>1</v>
@@ -11453,17 +11589,17 @@
         <v>53</v>
       </c>
       <c r="V101" s="7" t="s">
-        <v>739</v>
+        <v>749</v>
       </c>
       <c r="W101" s="7" t="s">
-        <v>621</v>
+        <v>750</v>
       </c>
       <c r="X101" s="7" t="s">
-        <v>622</v>
+        <v>751</v>
       </c>
       <c r="Y101" s="7"/>
       <c r="Z101" s="7">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="AA101" s="7"/>
       <c r="AB101" s="7" t="s">
@@ -11490,32 +11626,52 @@
         <v>100</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C102" s="3">
-        <v>2025082152</v>
-      </c>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
+        <v>2025082114</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>752</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F102" s="3">
-        <v>5384</v>
+        <v>4145</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>274</v>
+        <v>616</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="I102" s="3"/>
-      <c r="J102" s="3"/>
-      <c r="K102" s="3"/>
-      <c r="L102" s="3"/>
-      <c r="M102" s="4"/>
-      <c r="N102" s="3"/>
-      <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
+      <c r="I102" s="3" t="s">
+        <v>753</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M102" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="N102" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O102" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P102" s="10" t="s">
+        <v>754</v>
+      </c>
       <c r="Q102" s="3" t="s">
-        <v>279</v>
+        <v>619</v>
       </c>
       <c r="R102" s="3" t="s">
         <v>51</v>
@@ -11530,24 +11686,26 @@
         <v>53</v>
       </c>
       <c r="V102" s="3" t="s">
-        <v>740</v>
+        <v>755</v>
       </c>
       <c r="W102" s="3" t="s">
-        <v>741</v>
+        <v>621</v>
       </c>
       <c r="X102" s="3" t="s">
-        <v>742</v>
-      </c>
-      <c r="Y102" s="3"/>
+        <v>622</v>
+      </c>
+      <c r="Y102" s="3" t="s">
+        <v>756</v>
+      </c>
       <c r="Z102" s="3">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="AA102" s="3"/>
       <c r="AB102" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC102" s="4" t="s">
-        <v>743</v>
+      <c r="AC102" s="10" t="s">
+        <v>757</v>
       </c>
       <c r="AD102" s="3"/>
       <c r="AE102" s="3"/>
@@ -11555,10 +11713,433 @@
       <c r="AG102" s="3"/>
       <c r="AH102" s="3"/>
       <c r="AI102" s="3"/>
-      <c r="AJ102" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ102" s="3"/>
       <c r="AK102" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:37">
+      <c r="A103" s="7">
+        <v>101</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C103" s="7">
+        <v>2025082122</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7">
+        <v>4145</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
+      <c r="M103" s="8"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="8"/>
+      <c r="P103" s="9"/>
+      <c r="Q103" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="R103" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S103" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T103" s="7">
+        <v>1</v>
+      </c>
+      <c r="U103" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V103" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="W103" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="X103" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y103" s="7"/>
+      <c r="Z103" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA103" s="7"/>
+      <c r="AB103" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC103" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD103" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE103" s="7"/>
+      <c r="AF103" s="7"/>
+      <c r="AG103" s="7"/>
+      <c r="AH103" s="7"/>
+      <c r="AI103" s="7"/>
+      <c r="AJ103" s="7"/>
+      <c r="AK103" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:37">
+      <c r="A104" s="3">
+        <v>102</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C104" s="3">
+        <v>2025082147</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F104" s="3">
+        <v>4312</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M104" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N104" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O104" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="P104" s="10" t="s">
+        <v>761</v>
+      </c>
+      <c r="Q104" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="R104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S104" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T104" s="3">
+        <v>1</v>
+      </c>
+      <c r="U104" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V104" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="W104" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="X104" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="Y104" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="Z104" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA104" s="3"/>
+      <c r="AB104" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC104" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="AD104" s="3"/>
+      <c r="AE104" s="3"/>
+      <c r="AF104" s="3"/>
+      <c r="AG104" s="3"/>
+      <c r="AH104" s="3"/>
+      <c r="AI104" s="3"/>
+      <c r="AJ104" s="3"/>
+      <c r="AK104" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:37">
+      <c r="A105" s="7">
+        <v>103</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C105" s="7">
+        <v>2025082152</v>
+      </c>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7">
+        <v>5384</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+      <c r="L105" s="7"/>
+      <c r="M105" s="8"/>
+      <c r="N105" s="7"/>
+      <c r="O105" s="8"/>
+      <c r="P105" s="9"/>
+      <c r="Q105" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="R105" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S105" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T105" s="7">
+        <v>1</v>
+      </c>
+      <c r="U105" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V105" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="W105" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="X105" s="7" t="s">
+        <v>762</v>
+      </c>
+      <c r="Y105" s="7"/>
+      <c r="Z105" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA105" s="7"/>
+      <c r="AB105" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC105" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="AD105" s="7"/>
+      <c r="AE105" s="7"/>
+      <c r="AF105" s="7"/>
+      <c r="AG105" s="7"/>
+      <c r="AH105" s="7"/>
+      <c r="AI105" s="7"/>
+      <c r="AJ105" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK105" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:37">
+      <c r="A106" s="3">
+        <v>104</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="3">
+        <v>2025082178</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F106" s="3">
+        <v>3929</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K106" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L106" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M106" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="N106" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="O106" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="P106" s="10" t="s">
+        <v>772</v>
+      </c>
+      <c r="Q106" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="R106" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S106" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T106" s="3">
+        <v>1</v>
+      </c>
+      <c r="U106" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V106" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="W106" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="X106" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="Y106" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="Z106" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA106" s="3"/>
+      <c r="AB106" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC106" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="AD106" s="3"/>
+      <c r="AE106" s="3"/>
+      <c r="AF106" s="3"/>
+      <c r="AG106" s="3"/>
+      <c r="AH106" s="3"/>
+      <c r="AI106" s="3"/>
+      <c r="AJ106" s="3"/>
+      <c r="AK106" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:37">
+      <c r="A107" s="7">
+        <v>105</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C107" s="7">
+        <v>2025082205</v>
+      </c>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7">
+        <v>4538</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+      <c r="L107" s="7"/>
+      <c r="M107" s="8"/>
+      <c r="N107" s="7"/>
+      <c r="O107" s="8"/>
+      <c r="P107" s="8"/>
+      <c r="Q107" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="R107" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S107" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T107" s="7">
+        <v>1</v>
+      </c>
+      <c r="U107" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V107" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="W107" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="X107" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="Y107" s="7"/>
+      <c r="Z107" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA107" s="7"/>
+      <c r="AB107" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC107" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="AD107" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE107" s="7"/>
+      <c r="AF107" s="7"/>
+      <c r="AG107" s="7"/>
+      <c r="AH107" s="7"/>
+      <c r="AI107" s="7"/>
+      <c r="AJ107" s="7"/>
+      <c r="AK107" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08201710
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$107</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$110</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="806">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-20  )</t>
   </si>
@@ -2442,6 +2442,88 @@
   </si>
   <si>
     <t>2025-08-19 10:18:00</t>
+  </si>
+  <si>
+    <t>E4057114082001</t>
+  </si>
+  <si>
+    <t>林口香澄店</t>
+  </si>
+  <si>
+    <t>2025-08-20 08:20:23</t>
+  </si>
+  <si>
+    <t>切刀卡紙，切紙不正常</t>
+  </si>
+  <si>
+    <t>門市反應LIFEET印票機L90無法自動裁切票券，需用手撕，已有關機紙捲重裝仍異常...請台芝到店協助(票卷機出紙有位移對不準 (目前無需補出卷況))</t>
+  </si>
+  <si>
+    <t>THILF04057</t>
+  </si>
+  <si>
+    <t>2025-08-20 09:08:07</t>
+  </si>
+  <si>
+    <t>2025-08-20 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-20 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-21 13:08:00</t>
+  </si>
+  <si>
+    <t>更新印票機韌體與印票程式</t>
+  </si>
+  <si>
+    <t>15291114082001</t>
+  </si>
+  <si>
+    <t>新莊國家置地</t>
+  </si>
+  <si>
+    <t>2025-08-20 09:32:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/20 09:55 與總公司玫君確認啟動緊急叫修:門市反應tm1.2咖啡快速鍵消失很多，查sc主檔正確，協助執行sc轉tm.版更仍異常，執行newopen&gt;手動主檔轉入時跳出應用程式錯誤。總公司功評回覆:檢視記錄檔並無硬碟異常資訊，但是重新執行檔案接收與更新後仍會出現錯誤，判斷應為SC(SHUTTLE6S)第一顆硬碟異常，請派工到店更換SC第一顆硬碟不備份還原，並攜帶第二顆備用。...請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)																																
+與門市確認帳務做到08/19，與通訊功評確認有收到08/19的銷售																																
+</t>
+  </si>
+  <si>
+    <t>THILF05291</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:00:01</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-20 12:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-20 16:00:00</t>
+  </si>
+  <si>
+    <t>更換第一顆硬碟不備份還原
+並告知吳先生更換硬碟注意事項</t>
+  </si>
+  <si>
+    <t>林口舊街店</t>
+  </si>
+  <si>
+    <t>THILF05364</t>
+  </si>
+  <si>
+    <t>2025-08-20 15:11:22</t>
+  </si>
+  <si>
+    <t>2025-08-20 14:00:00</t>
+  </si>
+  <si>
+    <t>PMQ3+EDC+TVV+PEP裝機完成</t>
   </si>
 </sst>
 </file>
@@ -2855,10 +2937,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK107"/>
+  <dimension ref="A1:AK110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A107" sqref="A107"/>
+      <selection activeCell="AC107" sqref="AC107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12094,7 +12176,7 @@
       <c r="M107" s="8"/>
       <c r="N107" s="7"/>
       <c r="O107" s="8"/>
-      <c r="P107" s="8"/>
+      <c r="P107" s="9"/>
       <c r="Q107" s="7" t="s">
         <v>725</v>
       </c>
@@ -12127,7 +12209,7 @@
       <c r="AB107" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC107" s="8" t="s">
+      <c r="AC107" s="9" t="s">
         <v>479</v>
       </c>
       <c r="AD107" s="7" t="s">
@@ -12140,6 +12222,279 @@
       <c r="AI107" s="7"/>
       <c r="AJ107" s="7"/>
       <c r="AK107" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108" spans="1:37">
+      <c r="A108" s="3">
+        <v>106</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" s="3">
+        <v>2025082307</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F108" s="3">
+        <v>4057</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L108" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="M108" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="N108" s="3">
+        <v>6001</v>
+      </c>
+      <c r="O108" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="P108" s="10" t="s">
+        <v>784</v>
+      </c>
+      <c r="Q108" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="R108" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S108" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T108" s="3">
+        <v>1</v>
+      </c>
+      <c r="U108" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V108" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="W108" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="X108" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="Y108" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="Z108" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA108" s="3"/>
+      <c r="AB108" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC108" s="10" t="s">
+        <v>790</v>
+      </c>
+      <c r="AD108" s="3"/>
+      <c r="AE108" s="3"/>
+      <c r="AF108" s="3"/>
+      <c r="AG108" s="3"/>
+      <c r="AH108" s="3"/>
+      <c r="AI108" s="3"/>
+      <c r="AJ108" s="3"/>
+      <c r="AK108" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:37">
+      <c r="A109" s="7">
+        <v>107</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C109" s="7">
+        <v>2025082318</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>791</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="F109" s="7">
+        <v>5291</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>792</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I109" s="7" t="s">
+        <v>793</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="K109" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L109" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M109" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N109" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O109" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="P109" s="9" t="s">
+        <v>794</v>
+      </c>
+      <c r="Q109" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="R109" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S109" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T109" s="7">
+        <v>1</v>
+      </c>
+      <c r="U109" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V109" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="W109" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="X109" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="Y109" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="Z109" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="AA109" s="7"/>
+      <c r="AB109" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC109" s="9" t="s">
+        <v>800</v>
+      </c>
+      <c r="AD109" s="7"/>
+      <c r="AE109" s="7"/>
+      <c r="AF109" s="7"/>
+      <c r="AG109" s="7"/>
+      <c r="AH109" s="7"/>
+      <c r="AI109" s="7"/>
+      <c r="AJ109" s="7"/>
+      <c r="AK109" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:37">
+      <c r="A110" s="3">
+        <v>108</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C110" s="3">
+        <v>2025082408</v>
+      </c>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3">
+        <v>5364</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="3"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="4"/>
+      <c r="Q110" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="R110" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S110" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T110" s="3">
+        <v>1</v>
+      </c>
+      <c r="U110" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V110" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="W110" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="X110" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="Y110" s="3"/>
+      <c r="Z110" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA110" s="3"/>
+      <c r="AB110" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC110" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="AD110" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE110" s="3"/>
+      <c r="AF110" s="3"/>
+      <c r="AG110" s="3"/>
+      <c r="AH110" s="3"/>
+      <c r="AI110" s="3"/>
+      <c r="AJ110" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK110" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08211330
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$110</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$113</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="806">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-20  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="830">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-21  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2511,6 +2511,31 @@
 並告知吳先生更換硬碟注意事項</t>
   </si>
   <si>
+    <t>13890114082001</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:42:57</t>
+  </si>
+  <si>
+    <t>門市反應tm1(TCX800)常常無法觸控鼠標會一直飄走，vnc查看鼠標閃爍亂跑無法協助操作觸控校正，重啟tm仍異常，確認無張貼文宣及保護貼....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-20 10:57:22</t>
+  </si>
+  <si>
+    <t>2025-08-21 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-21 10:56:00</t>
+  </si>
+  <si>
+    <t>2025-08-21 14:57:00</t>
+  </si>
+  <si>
+    <t>將主機電源插座換孔位比且重新矯正螢幕，目前螢幕可正常使用
+備註：主機電源線有被老鼠啃咬痕跡，已先用絕緣布包起</t>
+  </si>
+  <si>
     <t>林口舊街店</t>
   </si>
   <si>
@@ -2524,6 +2549,54 @@
   </si>
   <si>
     <t>PMQ3+EDC+TVV+PEP裝機完成</t>
+  </si>
+  <si>
+    <t>14144114082101</t>
+  </si>
+  <si>
+    <t>新莊頭前店</t>
+  </si>
+  <si>
+    <t>2025-08-21 10:31:07</t>
+  </si>
+  <si>
+    <t>門市反應MMK熱感機T70II小白單印不出來，確認印表機亮ERROR紅燈，已嘗試重啟設備+重裝紙捲+重啟MMK仍異常....請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04144</t>
+  </si>
+  <si>
+    <t>2025-08-21 10:32:35</t>
+  </si>
+  <si>
+    <t>2025-08-21 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-21 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 14:32:00</t>
+  </si>
+  <si>
+    <t>清潔切刀 感應器</t>
+  </si>
+  <si>
+    <t>三重護山店</t>
+  </si>
+  <si>
+    <t>THILF05245</t>
+  </si>
+  <si>
+    <t>2025-08-21 12:28:58</t>
+  </si>
+  <si>
+    <t>2025-08-21 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-21 12:25:00</t>
+  </si>
+  <si>
+    <t>PMQ3+TVV+PEP安裝完成</t>
   </si>
 </sst>
 </file>
@@ -2937,10 +3010,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK110"/>
+  <dimension ref="A1:AK113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC107" sqref="AC107"/>
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12424,38 +12497,58 @@
         <v>108</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C110" s="3">
-        <v>2025082408</v>
-      </c>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
+        <v>2025082351</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F110" s="3">
-        <v>5364</v>
+        <v>3890</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>801</v>
+        <v>264</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I110" s="3"/>
-      <c r="J110" s="3"/>
-      <c r="K110" s="3"/>
-      <c r="L110" s="3"/>
-      <c r="M110" s="4"/>
-      <c r="N110" s="3"/>
-      <c r="O110" s="4"/>
-      <c r="P110" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L110" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M110" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="N110" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O110" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="P110" s="10" t="s">
+        <v>803</v>
+      </c>
       <c r="Q110" s="3" t="s">
-        <v>802</v>
+        <v>267</v>
       </c>
       <c r="R110" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S110" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T110" s="3">
         <v>1</v>
@@ -12464,37 +12557,290 @@
         <v>53</v>
       </c>
       <c r="V110" s="3" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="W110" s="3" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="X110" s="3" t="s">
-        <v>787</v>
-      </c>
-      <c r="Y110" s="3"/>
+        <v>806</v>
+      </c>
+      <c r="Y110" s="3" t="s">
+        <v>807</v>
+      </c>
       <c r="Z110" s="3">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="AA110" s="3"/>
       <c r="AB110" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC110" s="4" t="s">
-        <v>805</v>
-      </c>
-      <c r="AD110" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC110" s="10" t="s">
+        <v>808</v>
+      </c>
+      <c r="AD110" s="3"/>
       <c r="AE110" s="3"/>
       <c r="AF110" s="3"/>
       <c r="AG110" s="3"/>
       <c r="AH110" s="3"/>
       <c r="AI110" s="3"/>
-      <c r="AJ110" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ110" s="3"/>
       <c r="AK110" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="111" spans="1:37">
+      <c r="A111" s="7">
+        <v>109</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C111" s="7">
+        <v>2025082408</v>
+      </c>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7">
+        <v>5364</v>
+      </c>
+      <c r="G111" s="7" t="s">
+        <v>809</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I111" s="7"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="8"/>
+      <c r="N111" s="7"/>
+      <c r="O111" s="8"/>
+      <c r="P111" s="9"/>
+      <c r="Q111" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="R111" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S111" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T111" s="7">
+        <v>1</v>
+      </c>
+      <c r="U111" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V111" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="W111" s="7" t="s">
+        <v>812</v>
+      </c>
+      <c r="X111" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="Y111" s="7"/>
+      <c r="Z111" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA111" s="7"/>
+      <c r="AB111" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC111" s="9" t="s">
+        <v>813</v>
+      </c>
+      <c r="AD111" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE111" s="7"/>
+      <c r="AF111" s="7"/>
+      <c r="AG111" s="7"/>
+      <c r="AH111" s="7"/>
+      <c r="AI111" s="7"/>
+      <c r="AJ111" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK111" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:37">
+      <c r="A112" s="3">
+        <v>110</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C112" s="3">
+        <v>2025082482</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F112" s="3">
+        <v>4144</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K112" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L112" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M112" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N112" s="3">
+        <v>5903</v>
+      </c>
+      <c r="O112" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P112" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="Q112" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="R112" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S112" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T112" s="3">
+        <v>1</v>
+      </c>
+      <c r="U112" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V112" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="W112" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="X112" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="Y112" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="Z112" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA112" s="3"/>
+      <c r="AB112" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC112" s="10" t="s">
+        <v>823</v>
+      </c>
+      <c r="AD112" s="3"/>
+      <c r="AE112" s="3"/>
+      <c r="AF112" s="3"/>
+      <c r="AG112" s="3"/>
+      <c r="AH112" s="3"/>
+      <c r="AI112" s="3"/>
+      <c r="AJ112" s="3"/>
+      <c r="AK112" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:37">
+      <c r="A113" s="7">
+        <v>111</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C113" s="7">
+        <v>2025082518</v>
+      </c>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7">
+        <v>5245</v>
+      </c>
+      <c r="G113" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I113" s="7"/>
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
+      <c r="L113" s="7"/>
+      <c r="M113" s="8"/>
+      <c r="N113" s="7"/>
+      <c r="O113" s="8"/>
+      <c r="P113" s="8"/>
+      <c r="Q113" s="7" t="s">
+        <v>825</v>
+      </c>
+      <c r="R113" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S113" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T113" s="7">
+        <v>1</v>
+      </c>
+      <c r="U113" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V113" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="W113" s="7" t="s">
+        <v>827</v>
+      </c>
+      <c r="X113" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="Y113" s="7"/>
+      <c r="Z113" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="AA113" s="7"/>
+      <c r="AB113" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC113" s="8" t="s">
+        <v>829</v>
+      </c>
+      <c r="AD113" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE113" s="7"/>
+      <c r="AF113" s="7"/>
+      <c r="AG113" s="7"/>
+      <c r="AH113" s="7"/>
+      <c r="AI113" s="7"/>
+      <c r="AJ113" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK113" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08221324
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$113</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$121</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="830">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-21  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="890">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-22  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2551,6 +2551,30 @@
     <t>PMQ3+EDC+TVV+PEP裝機完成</t>
   </si>
   <si>
+    <t>E3796114082101</t>
+  </si>
+  <si>
+    <t>2025-08-21 06:26:49</t>
+  </si>
+  <si>
+    <t>TM2(TCX800)觸控常常點選無反應要點很多下，已有協助銃控校正後仍異常，請台芝到店協助(觸控遲緩,反應慢,常常按無反應要按好幾次,機台2)</t>
+  </si>
+  <si>
+    <t>2025-08-21 09:50:16</t>
+  </si>
+  <si>
+    <t>2025-08-21 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-21 14:41:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 13:50:00</t>
+  </si>
+  <si>
+    <t>重新矯正螢幕，目前測試正常，請店員觀察</t>
+  </si>
+  <si>
     <t>14144114082101</t>
   </si>
   <si>
@@ -2581,6 +2605,71 @@
     <t>清潔切刀 感應器</t>
   </si>
   <si>
+    <t>14134114082101</t>
+  </si>
+  <si>
+    <t>三重大同南</t>
+  </si>
+  <si>
+    <t>2025-08-21 11:27:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">總公司健誌副理叫修:4134門市SC(SHUTTLE6S)的第二顆硬碟有目錄損毀導致電子發票無法順利產生，已經暫時排除；為了避免後續還會發生，請這幾天安排時間到店更換SC第二顆硬碟，資料不要備份。已與門市確認今日使用訂貨3.0、HISHOP正常...請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)																																
+與門市確認帳務做到08/20，與通訊健誌副理確認有收到08/20的銷售																																
+</t>
+  </si>
+  <si>
+    <t>THILF04134</t>
+  </si>
+  <si>
+    <t>2025-08-21 11:35:51</t>
+  </si>
+  <si>
+    <t>2025-08-21 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-21 16:54:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 15:35:00</t>
+  </si>
+  <si>
+    <t>1D070114082101</t>
+  </si>
+  <si>
+    <t>D070</t>
+  </si>
+  <si>
+    <t>三重重新店</t>
+  </si>
+  <si>
+    <t>2025-08-21 12:12:36</t>
+  </si>
+  <si>
+    <t>門市反應非24h門市，TM2(BSC10II)近期頻繁發生早上11點左右執行TM2清帳，帳條只印出一小截空白，TM無跳出任何訊息，門市發票機為二代(BSC10II)，未操作任何基本排除後續出發票正常。經HIPOS查看Eventlog無異常，收據檔內有此張帳條，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。...需請台芝到店確認</t>
+  </si>
+  <si>
+    <t>THILF0D070</t>
+  </si>
+  <si>
+    <t>2025-08-21 12:14:01</t>
+  </si>
+  <si>
+    <t>2025-08-22 09:45:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 16:14:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換下8155004154
+換上8155006319</t>
+  </si>
+  <si>
     <t>三重護山店</t>
   </si>
   <si>
@@ -2597,6 +2686,103 @@
   </si>
   <si>
     <t>PMQ3+TVV+PEP安裝完成</t>
+  </si>
+  <si>
+    <t>13452114082101</t>
+  </si>
+  <si>
+    <t>蘆洲信義店</t>
+  </si>
+  <si>
+    <t>2025-08-21 13:41:41</t>
+  </si>
+  <si>
+    <t>門市反應LIFE-ET印票機(L90)亮綠燈，但刷讀小白單顯示票券機異常，點選偵測異常，已有關機、重裝紙捲仍異常，請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03452</t>
+  </si>
+  <si>
+    <t>2025-08-21 13:43:46</t>
+  </si>
+  <si>
+    <t>2025-08-22 09:58:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 10:28:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 17:43:00</t>
+  </si>
+  <si>
+    <t>印票機變壓器鬆脫，插上後可正常使用</t>
+  </si>
+  <si>
+    <t>2025-08-21 13:47:10</t>
+  </si>
+  <si>
+    <t>2025-08-21 12:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-21 13:44:00</t>
+  </si>
+  <si>
+    <t>PMQ3+EDC+TVV+PEP安裝完成</t>
+  </si>
+  <si>
+    <t>1D649114082101</t>
+  </si>
+  <si>
+    <t>D649</t>
+  </si>
+  <si>
+    <t>三重運動公園</t>
+  </si>
+  <si>
+    <t>2025-08-21 17:00:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市告知LIFEET熱感機T70II印出來的小白單不完整導致無法刷讀，請門市關機紙捲重裝後仍異常...請台芝到店協助
+</t>
+  </si>
+  <si>
+    <t>THILF0D649</t>
+  </si>
+  <si>
+    <t>2025-08-21 17:10:54</t>
+  </si>
+  <si>
+    <t>2025-08-22 09:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 21:10:00</t>
+  </si>
+  <si>
+    <t>紙張異物卡至熱感頭，清除後正常</t>
+  </si>
+  <si>
+    <t>2025-08-22 10:30:45</t>
+  </si>
+  <si>
+    <t>2025-08-22 10:10:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 10:30:00</t>
+  </si>
+  <si>
+    <t>三重五常店</t>
+  </si>
+  <si>
+    <t>THILF05316</t>
+  </si>
+  <si>
+    <t>2025-08-22 11:22:20</t>
+  </si>
+  <si>
+    <t>2025-08-22 10:35:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 11:25:00</t>
   </si>
 </sst>
 </file>
@@ -3010,10 +3196,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK113"/>
+  <dimension ref="A1:AK121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A113" sqref="A113"/>
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12676,7 +12862,7 @@
         <v>38</v>
       </c>
       <c r="C112" s="3">
-        <v>2025082482</v>
+        <v>2025082463</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>814</v>
@@ -12685,46 +12871,46 @@
         <v>40</v>
       </c>
       <c r="F112" s="3">
-        <v>4144</v>
+        <v>3796</v>
       </c>
       <c r="G112" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I112" s="3" t="s">
         <v>815</v>
-      </c>
-      <c r="H112" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I112" s="3" t="s">
-        <v>816</v>
       </c>
       <c r="J112" s="3" t="s">
         <v>44</v>
       </c>
       <c r="K112" s="3" t="s">
-        <v>45</v>
+        <v>253</v>
       </c>
       <c r="L112" s="3" t="s">
-        <v>46</v>
+        <v>197</v>
       </c>
       <c r="M112" s="4" t="s">
-        <v>47</v>
+        <v>198</v>
       </c>
       <c r="N112" s="3">
-        <v>5903</v>
+        <v>2307</v>
       </c>
       <c r="O112" s="4" t="s">
-        <v>48</v>
+        <v>525</v>
       </c>
       <c r="P112" s="10" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="Q112" s="3" t="s">
-        <v>818</v>
+        <v>470</v>
       </c>
       <c r="R112" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S112" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T112" s="3">
         <v>1</v>
@@ -12733,26 +12919,26 @@
         <v>53</v>
       </c>
       <c r="V112" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="W112" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="X112" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="W112" s="3" t="s">
+      <c r="Y112" s="3" t="s">
         <v>820</v>
       </c>
-      <c r="X112" s="3" t="s">
-        <v>821</v>
-      </c>
-      <c r="Y112" s="3" t="s">
-        <v>822</v>
-      </c>
       <c r="Z112" s="3">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="AA112" s="3"/>
       <c r="AB112" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC112" s="10" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="AD112" s="3"/>
       <c r="AE112" s="3"/>
@@ -12770,38 +12956,58 @@
         <v>111</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C113" s="7">
-        <v>2025082518</v>
-      </c>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
+        <v>2025082482</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F113" s="7">
-        <v>5245</v>
+        <v>4144</v>
       </c>
       <c r="G113" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I113" s="7" t="s">
         <v>824</v>
       </c>
-      <c r="H113" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I113" s="7"/>
-      <c r="J113" s="7"/>
-      <c r="K113" s="7"/>
-      <c r="L113" s="7"/>
-      <c r="M113" s="8"/>
-      <c r="N113" s="7"/>
-      <c r="O113" s="8"/>
-      <c r="P113" s="8"/>
+      <c r="J113" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K113" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L113" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M113" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N113" s="7">
+        <v>5903</v>
+      </c>
+      <c r="O113" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P113" s="9" t="s">
+        <v>825</v>
+      </c>
       <c r="Q113" s="7" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="R113" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S113" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T113" s="7">
         <v>1</v>
@@ -12810,37 +13016,737 @@
         <v>53</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="W113" s="7" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="X113" s="7" t="s">
-        <v>828</v>
-      </c>
-      <c r="Y113" s="7"/>
+        <v>829</v>
+      </c>
+      <c r="Y113" s="7" t="s">
+        <v>830</v>
+      </c>
       <c r="Z113" s="7">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA113" s="7"/>
       <c r="AB113" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC113" s="8" t="s">
-        <v>829</v>
-      </c>
-      <c r="AD113" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC113" s="9" t="s">
+        <v>831</v>
+      </c>
+      <c r="AD113" s="7"/>
       <c r="AE113" s="7"/>
       <c r="AF113" s="7"/>
       <c r="AG113" s="7"/>
       <c r="AH113" s="7"/>
       <c r="AI113" s="7"/>
-      <c r="AJ113" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ113" s="7"/>
       <c r="AK113" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:37">
+      <c r="A114" s="3">
+        <v>112</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C114" s="3">
+        <v>2025082504</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F114" s="3">
+        <v>4134</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L114" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M114" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N114" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O114" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="P114" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="Q114" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="R114" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S114" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T114" s="3">
+        <v>1</v>
+      </c>
+      <c r="U114" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V114" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="W114" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="X114" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="Y114" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="Z114" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="AA114" s="3"/>
+      <c r="AB114" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC114" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="AD114" s="3"/>
+      <c r="AE114" s="3"/>
+      <c r="AF114" s="3"/>
+      <c r="AG114" s="3"/>
+      <c r="AH114" s="3"/>
+      <c r="AI114" s="3"/>
+      <c r="AJ114" s="3"/>
+      <c r="AK114" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:37">
+      <c r="A115" s="7">
+        <v>113</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C115" s="7">
+        <v>2025082515</v>
+      </c>
+      <c r="D115" s="7" t="s">
+        <v>841</v>
+      </c>
+      <c r="E115" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>842</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>843</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I115" s="7" t="s">
+        <v>844</v>
+      </c>
+      <c r="J115" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K115" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L115" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M115" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="N115" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O115" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="P115" s="9" t="s">
+        <v>845</v>
+      </c>
+      <c r="Q115" s="7" t="s">
+        <v>846</v>
+      </c>
+      <c r="R115" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S115" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T115" s="7">
+        <v>1</v>
+      </c>
+      <c r="U115" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V115" s="7" t="s">
+        <v>847</v>
+      </c>
+      <c r="W115" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="X115" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="Y115" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="Z115" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC115" s="9" t="s">
+        <v>851</v>
+      </c>
+      <c r="AD115" s="7"/>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="7"/>
+      <c r="AK115" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:37">
+      <c r="A116" s="3">
+        <v>114</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2025082518</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3">
+        <v>5245</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I116" s="3"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="3"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="10"/>
+      <c r="Q116" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S116" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T116" s="3">
+        <v>1</v>
+      </c>
+      <c r="U116" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="W116" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="X116" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="Y116" s="3"/>
+      <c r="Z116" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA116" s="3"/>
+      <c r="AB116" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC116" s="10" t="s">
+        <v>857</v>
+      </c>
+      <c r="AD116" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE116" s="3"/>
+      <c r="AF116" s="3"/>
+      <c r="AG116" s="3"/>
+      <c r="AH116" s="3"/>
+      <c r="AI116" s="3"/>
+      <c r="AJ116" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK116" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:37">
+      <c r="A117" s="7">
+        <v>115</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C117" s="7">
+        <v>2025082529</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F117" s="7">
+        <v>3452</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I117" s="7" t="s">
+        <v>860</v>
+      </c>
+      <c r="J117" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K117" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L117" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="M117" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="N117" s="7">
+        <v>6003</v>
+      </c>
+      <c r="O117" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P117" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="Q117" s="7" t="s">
+        <v>862</v>
+      </c>
+      <c r="R117" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S117" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T117" s="7">
+        <v>1</v>
+      </c>
+      <c r="U117" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V117" s="7" t="s">
+        <v>863</v>
+      </c>
+      <c r="W117" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="X117" s="7" t="s">
+        <v>865</v>
+      </c>
+      <c r="Y117" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="Z117" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA117" s="7"/>
+      <c r="AB117" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC117" s="9" t="s">
+        <v>867</v>
+      </c>
+      <c r="AD117" s="7"/>
+      <c r="AE117" s="7"/>
+      <c r="AF117" s="7"/>
+      <c r="AG117" s="7"/>
+      <c r="AH117" s="7"/>
+      <c r="AI117" s="7"/>
+      <c r="AJ117" s="7"/>
+      <c r="AK117" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:37">
+      <c r="A118" s="3">
+        <v>116</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2025082531</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3">
+        <v>5352</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I118" s="3"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="10"/>
+      <c r="Q118" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="R118" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S118" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T118" s="3">
+        <v>1</v>
+      </c>
+      <c r="U118" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V118" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="W118" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="X118" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="Y118" s="3"/>
+      <c r="Z118" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AA118" s="3"/>
+      <c r="AB118" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC118" s="10" t="s">
+        <v>871</v>
+      </c>
+      <c r="AD118" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE118" s="3"/>
+      <c r="AF118" s="3"/>
+      <c r="AG118" s="3"/>
+      <c r="AH118" s="3"/>
+      <c r="AI118" s="3"/>
+      <c r="AJ118" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK118" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:37">
+      <c r="A119" s="7">
+        <v>117</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C119" s="7">
+        <v>2025082761</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>872</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>873</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I119" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="J119" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K119" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L119" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M119" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N119" s="7">
+        <v>5902</v>
+      </c>
+      <c r="O119" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="P119" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="Q119" s="7" t="s">
+        <v>877</v>
+      </c>
+      <c r="R119" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S119" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T119" s="7">
+        <v>1</v>
+      </c>
+      <c r="U119" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V119" s="7" t="s">
+        <v>878</v>
+      </c>
+      <c r="W119" s="7" t="s">
+        <v>879</v>
+      </c>
+      <c r="X119" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="Y119" s="7" t="s">
+        <v>880</v>
+      </c>
+      <c r="Z119" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC119" s="9" t="s">
+        <v>881</v>
+      </c>
+      <c r="AD119" s="7"/>
+      <c r="AE119" s="7"/>
+      <c r="AF119" s="7"/>
+      <c r="AG119" s="7"/>
+      <c r="AH119" s="7"/>
+      <c r="AI119" s="7"/>
+      <c r="AJ119" s="7"/>
+      <c r="AK119" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:37">
+      <c r="A120" s="3">
+        <v>118</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2025082794</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3">
+        <v>3452</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I120" s="3"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="3"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="3"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="10"/>
+      <c r="Q120" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S120" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T120" s="3">
+        <v>1</v>
+      </c>
+      <c r="U120" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="W120" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="X120" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="Y120" s="3"/>
+      <c r="Z120" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA120" s="3"/>
+      <c r="AB120" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC120" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD120" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE120" s="3"/>
+      <c r="AF120" s="3"/>
+      <c r="AG120" s="3"/>
+      <c r="AH120" s="3"/>
+      <c r="AI120" s="3"/>
+      <c r="AJ120" s="3"/>
+      <c r="AK120" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="121" spans="1:37">
+      <c r="A121" s="7">
+        <v>119</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C121" s="7">
+        <v>2025082799</v>
+      </c>
+      <c r="D121" s="7"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7">
+        <v>5316</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="H121" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I121" s="7"/>
+      <c r="J121" s="7"/>
+      <c r="K121" s="7"/>
+      <c r="L121" s="7"/>
+      <c r="M121" s="8"/>
+      <c r="N121" s="7"/>
+      <c r="O121" s="8"/>
+      <c r="P121" s="8"/>
+      <c r="Q121" s="7" t="s">
+        <v>886</v>
+      </c>
+      <c r="R121" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S121" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T121" s="7">
+        <v>1</v>
+      </c>
+      <c r="U121" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V121" s="7" t="s">
+        <v>887</v>
+      </c>
+      <c r="W121" s="7" t="s">
+        <v>888</v>
+      </c>
+      <c r="X121" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="Y121" s="7"/>
+      <c r="Z121" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC121" s="8" t="s">
+        <v>857</v>
+      </c>
+      <c r="AD121" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE121" s="7"/>
+      <c r="AF121" s="7"/>
+      <c r="AG121" s="7"/>
+      <c r="AH121" s="7"/>
+      <c r="AI121" s="7"/>
+      <c r="AJ121" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK121" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08221810
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$121</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$123</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="899">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-22  )</t>
   </si>
@@ -2783,6 +2783,33 @@
   </si>
   <si>
     <t>2025-08-22 11:25:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 13:41:49</t>
+  </si>
+  <si>
+    <t>2025-08-22 13:00:00</t>
+  </si>
+  <si>
+    <t>PEP裝機完成</t>
+  </si>
+  <si>
+    <t>淡水魚市二</t>
+  </si>
+  <si>
+    <t>THILF05155</t>
+  </si>
+  <si>
+    <t>2025-08-22 16:42:52</t>
+  </si>
+  <si>
+    <t>2025-08-22 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-22 16:41:00</t>
+  </si>
+  <si>
+    <t>魚市二借機裝機完成</t>
   </si>
 </sst>
 </file>
@@ -3196,10 +3223,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK121"/>
+  <dimension ref="A1:AK123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A121" sqref="A121"/>
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13699,7 +13726,7 @@
       <c r="M121" s="8"/>
       <c r="N121" s="7"/>
       <c r="O121" s="8"/>
-      <c r="P121" s="8"/>
+      <c r="P121" s="9"/>
       <c r="Q121" s="7" t="s">
         <v>886</v>
       </c>
@@ -13732,7 +13759,7 @@
       <c r="AB121" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC121" s="8" t="s">
+      <c r="AC121" s="9" t="s">
         <v>857</v>
       </c>
       <c r="AD121" s="7" t="s">
@@ -13747,6 +13774,160 @@
         <v>60</v>
       </c>
       <c r="AK121" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:37">
+      <c r="A122" s="3">
+        <v>120</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2025082824</v>
+      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3">
+        <v>5291</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I122" s="3"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="3"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="10"/>
+      <c r="Q122" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T122" s="3">
+        <v>1</v>
+      </c>
+      <c r="U122" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V122" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="W122" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="X122" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="Y122" s="3"/>
+      <c r="Z122" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA122" s="3"/>
+      <c r="AB122" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC122" s="10" t="s">
+        <v>892</v>
+      </c>
+      <c r="AD122" s="3"/>
+      <c r="AE122" s="3"/>
+      <c r="AF122" s="3"/>
+      <c r="AG122" s="3"/>
+      <c r="AH122" s="3"/>
+      <c r="AI122" s="3"/>
+      <c r="AJ122" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK122" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:37">
+      <c r="A123" s="7">
+        <v>121</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C123" s="7">
+        <v>2025082866</v>
+      </c>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7">
+        <v>5155</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>893</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="I123" s="7"/>
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+      <c r="L123" s="7"/>
+      <c r="M123" s="8"/>
+      <c r="N123" s="7"/>
+      <c r="O123" s="8"/>
+      <c r="P123" s="8"/>
+      <c r="Q123" s="7" t="s">
+        <v>894</v>
+      </c>
+      <c r="R123" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S123" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T123" s="7">
+        <v>1</v>
+      </c>
+      <c r="U123" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V123" s="7" t="s">
+        <v>895</v>
+      </c>
+      <c r="W123" s="7" t="s">
+        <v>896</v>
+      </c>
+      <c r="X123" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="Y123" s="7"/>
+      <c r="Z123" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC123" s="8" t="s">
+        <v>898</v>
+      </c>
+      <c r="AD123" s="7"/>
+      <c r="AE123" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF123" s="7"/>
+      <c r="AG123" s="7"/>
+      <c r="AH123" s="7"/>
+      <c r="AI123" s="7"/>
+      <c r="AJ123" s="7"/>
+      <c r="AK123" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08251426
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$123</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$135</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="899">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-22  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="969">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-25  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2785,6 +2785,56 @@
     <t>2025-08-22 11:25:00</t>
   </si>
   <si>
+    <t>E4191114082201</t>
+  </si>
+  <si>
+    <t>三重溪美店</t>
+  </si>
+  <si>
+    <t>2025-08-22 12:40:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應TM1 CCD(HC56IITR)刷讀所有條碼都不好刷，需多刷幾次才有反應，已執行掃描校正仍未改善...須請台芝到店協助(兩台掃描器刷商品會無反應的狀況)
+08/22 12:50 請門市執行校正，門市告知13:30再去電確認
+</t>
+  </si>
+  <si>
+    <t>THILF04191</t>
+  </si>
+  <si>
+    <t>2025-08-22 13:31:42</t>
+  </si>
+  <si>
+    <t>2025-08-25 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 17:31:00</t>
+  </si>
+  <si>
+    <t>清潔掃描器 重接排線 掃描校正</t>
+  </si>
+  <si>
+    <t>14191114082201</t>
+  </si>
+  <si>
+    <t>2025-08-22 13:31:55</t>
+  </si>
+  <si>
+    <t>門市反應TM2 CCD(HC56IITR)刷讀所有條碼都不好刷，需多刷幾次才有反應，已執行掃描校正仍未改善...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-22 13:33:53</t>
+  </si>
+  <si>
+    <t>2025-08-25 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 17:33:00</t>
+  </si>
+  <si>
     <t>2025-08-22 13:41:49</t>
   </si>
   <si>
@@ -2794,6 +2844,67 @@
     <t>PEP裝機完成</t>
   </si>
   <si>
+    <t>13416114082201</t>
+  </si>
+  <si>
+    <t>2025-08-22 14:25:31</t>
+  </si>
+  <si>
+    <t>門市反應TM2收銀機(TCX800)(抽屜顏色:白色、鑰匙孔位子(中)、鎖頭編號:5001)抽屜彈開只會彈出一半需要自己用手拉...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-22 14:29:37</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:48:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:55:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 18:29:00</t>
+  </si>
+  <si>
+    <t>更換錢箱
+換上：81Z1004480
+換下：81Z1001050</t>
+  </si>
+  <si>
+    <t>1D349114082202</t>
+  </si>
+  <si>
+    <t>D349</t>
+  </si>
+  <si>
+    <t>板橋成都店</t>
+  </si>
+  <si>
+    <t>2025-08-22 15:43:04</t>
+  </si>
+  <si>
+    <t>門市反應MMK印票機L90 Error亮紅燈，確認紙捲還有，且無卡紙，重新拔插電源仍亮紅燈且偵測異常..........還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D349</t>
+  </si>
+  <si>
+    <t>2025-08-22 15:44:24</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:15:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:35:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 19:44:00</t>
+  </si>
+  <si>
+    <t>更換印票機
+換上：8139003249
+換下：8139001457</t>
+  </si>
+  <si>
     <t>淡水魚市二</t>
   </si>
   <si>
@@ -2810,6 +2921,111 @@
   </si>
   <si>
     <t>魚市二借機裝機完成</t>
+  </si>
+  <si>
+    <t>15082114082201</t>
+  </si>
+  <si>
+    <t>蘆洲水湳店</t>
+  </si>
+  <si>
+    <t>2025-08-22 17:05:24</t>
+  </si>
+  <si>
+    <t>區經理反應門市票券機L90印出的票券都是空白的，電源燈號正常無亮紅燈，區經理告知已有到店協助門市排除，將票券機關機紙捲重裝及票券紙捲裝另一面再次測試列印票券仍都印出空白...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05082</t>
+  </si>
+  <si>
+    <t>2025-08-22 17:08:57</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:13:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:43:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 21:08:00</t>
+  </si>
+  <si>
+    <t>印票機網路線被老鼠咬斷需請店員報修水電</t>
+  </si>
+  <si>
+    <t>淡水魚市店</t>
+  </si>
+  <si>
+    <t>THILF05060</t>
+  </si>
+  <si>
+    <t>2025-08-25 12:13:25</t>
+  </si>
+  <si>
+    <t>2025-08-25 11:15:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 12:15:50</t>
+  </si>
+  <si>
+    <t>2025-08-25 12:10:00</t>
+  </si>
+  <si>
+    <t>借機結束，撤機完成</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:40:01</t>
+  </si>
+  <si>
+    <t>新莊化成店</t>
+  </si>
+  <si>
+    <t>THILF02362</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:46:10</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:46:25</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:46:00</t>
+  </si>
+  <si>
+    <t>新莊頭前公園</t>
+  </si>
+  <si>
+    <t>THILF04228</t>
+  </si>
+  <si>
+    <t>2025-08-25 14:01:20</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 13:50:00</t>
+  </si>
+  <si>
+    <t>新莊幸運店</t>
+  </si>
+  <si>
+    <t>THILF04679</t>
+  </si>
+  <si>
+    <t>2025-08-25 14:13:48</t>
+  </si>
+  <si>
+    <t>2025-08-25 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 14:20:00</t>
   </si>
 </sst>
 </file>
@@ -3223,10 +3439,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK123"/>
+  <dimension ref="A1:AK135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A123" sqref="A123"/>
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13782,32 +13998,52 @@
         <v>120</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C122" s="3">
-        <v>2025082824</v>
-      </c>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
+        <v>2025082822</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F122" s="3">
-        <v>5291</v>
+        <v>4191</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>792</v>
+        <v>891</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I122" s="3"/>
-      <c r="J122" s="3"/>
-      <c r="K122" s="3"/>
-      <c r="L122" s="3"/>
-      <c r="M122" s="4"/>
-      <c r="N122" s="3"/>
-      <c r="O122" s="4"/>
-      <c r="P122" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="J122" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K122" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L122" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M122" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="N122" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O122" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P122" s="10" t="s">
+        <v>893</v>
+      </c>
       <c r="Q122" s="3" t="s">
-        <v>795</v>
+        <v>894</v>
       </c>
       <c r="R122" s="3" t="s">
         <v>51</v>
@@ -13822,24 +14058,26 @@
         <v>53</v>
       </c>
       <c r="V122" s="3" t="s">
-        <v>890</v>
+        <v>895</v>
       </c>
       <c r="W122" s="3" t="s">
-        <v>891</v>
+        <v>896</v>
       </c>
       <c r="X122" s="3" t="s">
-        <v>820</v>
-      </c>
-      <c r="Y122" s="3"/>
+        <v>897</v>
+      </c>
+      <c r="Y122" s="3" t="s">
+        <v>898</v>
+      </c>
       <c r="Z122" s="3">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="AA122" s="3"/>
       <c r="AB122" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC122" s="10" t="s">
-        <v>892</v>
+        <v>899</v>
       </c>
       <c r="AD122" s="3"/>
       <c r="AE122" s="3"/>
@@ -13847,9 +14085,7 @@
       <c r="AG122" s="3"/>
       <c r="AH122" s="3"/>
       <c r="AI122" s="3"/>
-      <c r="AJ122" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ122" s="3"/>
       <c r="AK122" s="3" t="s">
         <v>60</v>
       </c>
@@ -13859,30 +14095,50 @@
         <v>121</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C123" s="7">
-        <v>2025082866</v>
-      </c>
-      <c r="D123" s="7"/>
-      <c r="E123" s="7"/>
+        <v>2025082823</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F123" s="7">
-        <v>5155</v>
+        <v>4191</v>
       </c>
       <c r="G123" s="7" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="I123" s="7"/>
-      <c r="J123" s="7"/>
-      <c r="K123" s="7"/>
-      <c r="L123" s="7"/>
-      <c r="M123" s="8"/>
-      <c r="N123" s="7"/>
-      <c r="O123" s="8"/>
-      <c r="P123" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="I123" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="J123" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K123" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L123" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M123" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="N123" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O123" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="P123" s="9" t="s">
+        <v>902</v>
+      </c>
       <c r="Q123" s="7" t="s">
         <v>894</v>
       </c>
@@ -13890,7 +14146,7 @@
         <v>51</v>
       </c>
       <c r="S123" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T123" s="7">
         <v>1</v>
@@ -13899,35 +14155,1021 @@
         <v>53</v>
       </c>
       <c r="V123" s="7" t="s">
-        <v>895</v>
+        <v>903</v>
       </c>
       <c r="W123" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="X123" s="7" t="s">
         <v>896</v>
       </c>
-      <c r="X123" s="7" t="s">
-        <v>897</v>
-      </c>
-      <c r="Y123" s="7"/>
+      <c r="Y123" s="7" t="s">
+        <v>905</v>
+      </c>
       <c r="Z123" s="7">
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="AA123" s="7"/>
       <c r="AB123" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC123" s="8" t="s">
-        <v>898</v>
+      <c r="AC123" s="9" t="s">
+        <v>899</v>
       </c>
       <c r="AD123" s="7"/>
-      <c r="AE123" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AE123" s="7"/>
       <c r="AF123" s="7"/>
       <c r="AG123" s="7"/>
       <c r="AH123" s="7"/>
       <c r="AI123" s="7"/>
       <c r="AJ123" s="7"/>
       <c r="AK123" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:37">
+      <c r="A124" s="3">
+        <v>122</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C124" s="3">
+        <v>2025082824</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3">
+        <v>5291</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="3"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="10"/>
+      <c r="Q124" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T124" s="3">
+        <v>1</v>
+      </c>
+      <c r="U124" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V124" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="W124" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="X124" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="Y124" s="3"/>
+      <c r="Z124" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA124" s="3"/>
+      <c r="AB124" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC124" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="AD124" s="3"/>
+      <c r="AE124" s="3"/>
+      <c r="AF124" s="3"/>
+      <c r="AG124" s="3"/>
+      <c r="AH124" s="3"/>
+      <c r="AI124" s="3"/>
+      <c r="AJ124" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK124" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="1:37">
+      <c r="A125" s="7">
+        <v>123</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C125" s="7">
+        <v>2025082834</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F125" s="7">
+        <v>3416</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I125" s="7" t="s">
+        <v>910</v>
+      </c>
+      <c r="J125" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K125" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L125" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M125" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N125" s="7">
+        <v>2305</v>
+      </c>
+      <c r="O125" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="P125" s="9" t="s">
+        <v>911</v>
+      </c>
+      <c r="Q125" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="R125" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S125" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T125" s="7">
+        <v>1</v>
+      </c>
+      <c r="U125" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V125" s="7" t="s">
+        <v>912</v>
+      </c>
+      <c r="W125" s="7" t="s">
+        <v>913</v>
+      </c>
+      <c r="X125" s="7" t="s">
+        <v>914</v>
+      </c>
+      <c r="Y125" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="Z125" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="AA125" s="7"/>
+      <c r="AB125" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC125" s="9" t="s">
+        <v>916</v>
+      </c>
+      <c r="AD125" s="7"/>
+      <c r="AE125" s="7"/>
+      <c r="AF125" s="7"/>
+      <c r="AG125" s="7"/>
+      <c r="AH125" s="7"/>
+      <c r="AI125" s="7"/>
+      <c r="AJ125" s="7"/>
+      <c r="AK125" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="126" spans="1:37">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C126" s="3">
+        <v>2025082856</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="J126" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K126" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L126" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="M126" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="N126" s="3">
+        <v>6003</v>
+      </c>
+      <c r="O126" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P126" s="10" t="s">
+        <v>921</v>
+      </c>
+      <c r="Q126" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="R126" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S126" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T126" s="3">
+        <v>1</v>
+      </c>
+      <c r="U126" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V126" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="W126" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="X126" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="Y126" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="Z126" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA126" s="3"/>
+      <c r="AB126" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC126" s="10" t="s">
+        <v>927</v>
+      </c>
+      <c r="AD126" s="3"/>
+      <c r="AE126" s="3"/>
+      <c r="AF126" s="3"/>
+      <c r="AG126" s="3"/>
+      <c r="AH126" s="3"/>
+      <c r="AI126" s="3"/>
+      <c r="AJ126" s="3"/>
+      <c r="AK126" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="1:37">
+      <c r="A127" s="7">
+        <v>125</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C127" s="7">
+        <v>2025082866</v>
+      </c>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7">
+        <v>5155</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>928</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+      <c r="L127" s="7"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="7"/>
+      <c r="O127" s="8"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="7" t="s">
+        <v>929</v>
+      </c>
+      <c r="R127" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S127" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T127" s="7">
+        <v>1</v>
+      </c>
+      <c r="U127" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V127" s="7" t="s">
+        <v>930</v>
+      </c>
+      <c r="W127" s="7" t="s">
+        <v>931</v>
+      </c>
+      <c r="X127" s="7" t="s">
+        <v>932</v>
+      </c>
+      <c r="Y127" s="7"/>
+      <c r="Z127" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="AA127" s="7"/>
+      <c r="AB127" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC127" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="AD127" s="7"/>
+      <c r="AE127" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF127" s="7"/>
+      <c r="AG127" s="7"/>
+      <c r="AH127" s="7"/>
+      <c r="AI127" s="7"/>
+      <c r="AJ127" s="7"/>
+      <c r="AK127" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:37">
+      <c r="A128" s="3">
+        <v>126</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2025082880</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F128" s="3">
+        <v>5082</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>936</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K128" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L128" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="M128" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="N128" s="3">
+        <v>6002</v>
+      </c>
+      <c r="O128" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="P128" s="10" t="s">
+        <v>937</v>
+      </c>
+      <c r="Q128" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="R128" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S128" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T128" s="3">
+        <v>1</v>
+      </c>
+      <c r="U128" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V128" s="3" t="s">
+        <v>939</v>
+      </c>
+      <c r="W128" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="X128" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="Y128" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="Z128" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA128" s="3"/>
+      <c r="AB128" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC128" s="10" t="s">
+        <v>943</v>
+      </c>
+      <c r="AD128" s="3"/>
+      <c r="AE128" s="3"/>
+      <c r="AF128" s="3"/>
+      <c r="AG128" s="3"/>
+      <c r="AH128" s="3"/>
+      <c r="AI128" s="3"/>
+      <c r="AJ128" s="3"/>
+      <c r="AK128" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="129" spans="1:37">
+      <c r="A129" s="7">
+        <v>127</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C129" s="7">
+        <v>2025082950</v>
+      </c>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7">
+        <v>5060</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>944</v>
+      </c>
+      <c r="H129" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="I129" s="7"/>
+      <c r="J129" s="7"/>
+      <c r="K129" s="7"/>
+      <c r="L129" s="7"/>
+      <c r="M129" s="8"/>
+      <c r="N129" s="7"/>
+      <c r="O129" s="8"/>
+      <c r="P129" s="9"/>
+      <c r="Q129" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="R129" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S129" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T129" s="7">
+        <v>1</v>
+      </c>
+      <c r="U129" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V129" s="7" t="s">
+        <v>946</v>
+      </c>
+      <c r="W129" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="X129" s="7" t="s">
+        <v>947</v>
+      </c>
+      <c r="Y129" s="7"/>
+      <c r="Z129" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA129" s="7"/>
+      <c r="AB129" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC129" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD129" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE129" s="7"/>
+      <c r="AF129" s="7"/>
+      <c r="AG129" s="7"/>
+      <c r="AH129" s="7"/>
+      <c r="AI129" s="7"/>
+      <c r="AJ129" s="7"/>
+      <c r="AK129" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:37">
+      <c r="A130" s="3">
+        <v>128</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C130" s="3">
+        <v>2025082955</v>
+      </c>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3">
+        <v>5155</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="I130" s="3"/>
+      <c r="J130" s="3"/>
+      <c r="K130" s="3"/>
+      <c r="L130" s="3"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="3"/>
+      <c r="O130" s="4"/>
+      <c r="P130" s="10"/>
+      <c r="Q130" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="R130" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S130" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T130" s="3">
+        <v>1</v>
+      </c>
+      <c r="U130" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V130" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="W130" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="X130" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="Y130" s="3"/>
+      <c r="Z130" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="AA130" s="3"/>
+      <c r="AB130" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC130" s="10" t="s">
+        <v>950</v>
+      </c>
+      <c r="AD130" s="3"/>
+      <c r="AE130" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF130" s="3"/>
+      <c r="AG130" s="3"/>
+      <c r="AH130" s="3"/>
+      <c r="AI130" s="3"/>
+      <c r="AJ130" s="3"/>
+      <c r="AK130" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:37">
+      <c r="A131" s="7">
+        <v>129</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C131" s="7">
+        <v>2025082988</v>
+      </c>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="7" t="s">
+        <v>918</v>
+      </c>
+      <c r="G131" s="7" t="s">
+        <v>919</v>
+      </c>
+      <c r="H131" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I131" s="7"/>
+      <c r="J131" s="7"/>
+      <c r="K131" s="7"/>
+      <c r="L131" s="7"/>
+      <c r="M131" s="8"/>
+      <c r="N131" s="7"/>
+      <c r="O131" s="8"/>
+      <c r="P131" s="9"/>
+      <c r="Q131" s="7" t="s">
+        <v>922</v>
+      </c>
+      <c r="R131" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S131" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T131" s="7">
+        <v>1</v>
+      </c>
+      <c r="U131" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V131" s="7" t="s">
+        <v>951</v>
+      </c>
+      <c r="W131" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="X131" s="7" t="s">
+        <v>925</v>
+      </c>
+      <c r="Y131" s="7"/>
+      <c r="Z131" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA131" s="7"/>
+      <c r="AB131" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC131" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD131" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE131" s="7"/>
+      <c r="AF131" s="7"/>
+      <c r="AG131" s="7"/>
+      <c r="AH131" s="7"/>
+      <c r="AI131" s="7"/>
+      <c r="AJ131" s="7"/>
+      <c r="AK131" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="132" spans="1:37">
+      <c r="A132" s="3">
+        <v>130</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C132" s="3">
+        <v>2025082990</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3">
+        <v>2362</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I132" s="3"/>
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="3"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="3"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="R132" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S132" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T132" s="3">
+        <v>1</v>
+      </c>
+      <c r="U132" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V132" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="W132" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="X132" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="Y132" s="3"/>
+      <c r="Z132" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA132" s="3"/>
+      <c r="AB132" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC132" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD132" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE132" s="3"/>
+      <c r="AF132" s="3"/>
+      <c r="AG132" s="3"/>
+      <c r="AH132" s="3"/>
+      <c r="AI132" s="3"/>
+      <c r="AJ132" s="3"/>
+      <c r="AK132" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:37">
+      <c r="A133" s="7">
+        <v>131</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C133" s="7">
+        <v>2025082991</v>
+      </c>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7">
+        <v>5082</v>
+      </c>
+      <c r="G133" s="7" t="s">
+        <v>935</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+      <c r="L133" s="7"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="7"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="9"/>
+      <c r="Q133" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="R133" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S133" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T133" s="7">
+        <v>1</v>
+      </c>
+      <c r="U133" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V133" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="W133" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="X133" s="7" t="s">
+        <v>958</v>
+      </c>
+      <c r="Y133" s="7"/>
+      <c r="Z133" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA133" s="7"/>
+      <c r="AB133" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC133" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD133" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE133" s="7"/>
+      <c r="AF133" s="7"/>
+      <c r="AG133" s="7"/>
+      <c r="AH133" s="7"/>
+      <c r="AI133" s="7"/>
+      <c r="AJ133" s="7"/>
+      <c r="AK133" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:37">
+      <c r="A134" s="3">
+        <v>132</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C134" s="3">
+        <v>2025082995</v>
+      </c>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="3">
+        <v>4228</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I134" s="3"/>
+      <c r="J134" s="3"/>
+      <c r="K134" s="3"/>
+      <c r="L134" s="3"/>
+      <c r="M134" s="4"/>
+      <c r="N134" s="3"/>
+      <c r="O134" s="4"/>
+      <c r="P134" s="10"/>
+      <c r="Q134" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="R134" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S134" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T134" s="3">
+        <v>1</v>
+      </c>
+      <c r="U134" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V134" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="W134" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="X134" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="Y134" s="3"/>
+      <c r="Z134" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA134" s="3"/>
+      <c r="AB134" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC134" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD134" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE134" s="3"/>
+      <c r="AF134" s="3"/>
+      <c r="AG134" s="3"/>
+      <c r="AH134" s="3"/>
+      <c r="AI134" s="3"/>
+      <c r="AJ134" s="3"/>
+      <c r="AK134" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="135" spans="1:37">
+      <c r="A135" s="7">
+        <v>133</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C135" s="7">
+        <v>2025083005</v>
+      </c>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+      <c r="F135" s="7">
+        <v>4679</v>
+      </c>
+      <c r="G135" s="7" t="s">
+        <v>964</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I135" s="7"/>
+      <c r="J135" s="7"/>
+      <c r="K135" s="7"/>
+      <c r="L135" s="7"/>
+      <c r="M135" s="8"/>
+      <c r="N135" s="7"/>
+      <c r="O135" s="8"/>
+      <c r="P135" s="8"/>
+      <c r="Q135" s="7" t="s">
+        <v>965</v>
+      </c>
+      <c r="R135" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S135" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T135" s="7">
+        <v>1</v>
+      </c>
+      <c r="U135" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V135" s="7" t="s">
+        <v>966</v>
+      </c>
+      <c r="W135" s="7" t="s">
+        <v>967</v>
+      </c>
+      <c r="X135" s="7" t="s">
+        <v>968</v>
+      </c>
+      <c r="Y135" s="7"/>
+      <c r="Z135" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA135" s="7"/>
+      <c r="AB135" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC135" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="AD135" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE135" s="7"/>
+      <c r="AF135" s="7"/>
+      <c r="AG135" s="7"/>
+      <c r="AH135" s="7"/>
+      <c r="AI135" s="7"/>
+      <c r="AJ135" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK135" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08251706
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$135</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$138</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="991">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-25  )</t>
   </si>
@@ -2953,6 +2953,39 @@
     <t>印票機網路線被老鼠咬斷需請店員報修水電</t>
   </si>
   <si>
+    <t>E4210114082501</t>
+  </si>
+  <si>
+    <t>三重福華店</t>
+  </si>
+  <si>
+    <t>2025-08-25 09:31:01</t>
+  </si>
+  <si>
+    <t>鍵盤按鍵不良或無反應</t>
+  </si>
+  <si>
+    <t>門市反應sc鍵盤一個鍵帽損壞脫落....須請台芝到店協助(電腦鍵盤 鍵帽壞掉)</t>
+  </si>
+  <si>
+    <t>THILF04210</t>
+  </si>
+  <si>
+    <t>2025-08-25 09:39:23</t>
+  </si>
+  <si>
+    <t>2025-08-25 15:49:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 16:19:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 13:39:00</t>
+  </si>
+  <si>
+    <t>更換鍵盤</t>
+  </si>
+  <si>
     <t>淡水魚市店</t>
   </si>
   <si>
@@ -3026,6 +3059,39 @@
   </si>
   <si>
     <t>2025-08-25 14:20:00</t>
+  </si>
+  <si>
+    <t>新莊巷口店</t>
+  </si>
+  <si>
+    <t>THILF04762</t>
+  </si>
+  <si>
+    <t>2025-08-25 14:40:55</t>
+  </si>
+  <si>
+    <t>2025-08-25 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 14:50:00</t>
+  </si>
+  <si>
+    <t>蘆洲湧蓮店</t>
+  </si>
+  <si>
+    <t>THILF04218</t>
+  </si>
+  <si>
+    <t>2025-08-25 15:43:29</t>
+  </si>
+  <si>
+    <t>2025-08-25 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-25 15:45:00</t>
+  </si>
+  <si>
+    <t>撤機完成</t>
   </si>
 </sst>
 </file>
@@ -3439,10 +3505,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK135"/>
+  <dimension ref="A1:AK138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A135" sqref="A135"/>
+      <selection activeCell="AC135" sqref="AC135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14637,32 +14703,52 @@
         <v>127</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C129" s="7">
-        <v>2025082950</v>
-      </c>
-      <c r="D129" s="7"/>
-      <c r="E129" s="7"/>
+        <v>2025082910</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>944</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F129" s="7">
-        <v>5060</v>
+        <v>4210</v>
       </c>
       <c r="G129" s="7" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="H129" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="I129" s="7"/>
-      <c r="J129" s="7"/>
-      <c r="K129" s="7"/>
-      <c r="L129" s="7"/>
-      <c r="M129" s="8"/>
-      <c r="N129" s="7"/>
-      <c r="O129" s="8"/>
-      <c r="P129" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="I129" s="7" t="s">
+        <v>946</v>
+      </c>
+      <c r="J129" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K129" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L129" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M129" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N129" s="7">
+        <v>2402</v>
+      </c>
+      <c r="O129" s="8" t="s">
+        <v>947</v>
+      </c>
+      <c r="P129" s="9" t="s">
+        <v>948</v>
+      </c>
       <c r="Q129" s="7" t="s">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c r="R129" s="7" t="s">
         <v>51</v>
@@ -14677,28 +14763,28 @@
         <v>53</v>
       </c>
       <c r="V129" s="7" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
       <c r="W129" s="7" t="s">
-        <v>897</v>
+        <v>951</v>
       </c>
       <c r="X129" s="7" t="s">
-        <v>947</v>
-      </c>
-      <c r="Y129" s="7"/>
+        <v>952</v>
+      </c>
+      <c r="Y129" s="7" t="s">
+        <v>953</v>
+      </c>
       <c r="Z129" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA129" s="7"/>
       <c r="AB129" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC129" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD129" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>954</v>
+      </c>
+      <c r="AD129" s="7"/>
       <c r="AE129" s="7"/>
       <c r="AF129" s="7"/>
       <c r="AG129" s="7"/>
@@ -14717,15 +14803,15 @@
         <v>78</v>
       </c>
       <c r="C130" s="3">
-        <v>2025082955</v>
+        <v>2025082950</v>
       </c>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
       <c r="F130" s="3">
-        <v>5155</v>
+        <v>5060</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>928</v>
+        <v>955</v>
       </c>
       <c r="H130" s="3" t="s">
         <v>360</v>
@@ -14739,7 +14825,7 @@
       <c r="O130" s="4"/>
       <c r="P130" s="10"/>
       <c r="Q130" s="3" t="s">
-        <v>929</v>
+        <v>956</v>
       </c>
       <c r="R130" s="3" t="s">
         <v>51</v>
@@ -14754,29 +14840,29 @@
         <v>53</v>
       </c>
       <c r="V130" s="3" t="s">
-        <v>948</v>
+        <v>957</v>
       </c>
       <c r="W130" s="3" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="X130" s="3" t="s">
-        <v>949</v>
+        <v>958</v>
       </c>
       <c r="Y130" s="3"/>
       <c r="Z130" s="3">
-        <v>1.7</v>
+        <v>0.3</v>
       </c>
       <c r="AA130" s="3"/>
       <c r="AB130" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC130" s="10" t="s">
-        <v>950</v>
-      </c>
-      <c r="AD130" s="3"/>
-      <c r="AE130" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="AD130" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE130" s="3"/>
       <c r="AF130" s="3"/>
       <c r="AG130" s="3"/>
       <c r="AH130" s="3"/>
@@ -14794,18 +14880,18 @@
         <v>78</v>
       </c>
       <c r="C131" s="7">
-        <v>2025082988</v>
+        <v>2025082955</v>
       </c>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
-      <c r="F131" s="7" t="s">
-        <v>918</v>
+      <c r="F131" s="7">
+        <v>5155</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>919</v>
+        <v>928</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>206</v>
+        <v>360</v>
       </c>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
@@ -14816,13 +14902,13 @@
       <c r="O131" s="8"/>
       <c r="P131" s="9"/>
       <c r="Q131" s="7" t="s">
-        <v>922</v>
+        <v>929</v>
       </c>
       <c r="R131" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>210</v>
+        <v>52</v>
       </c>
       <c r="T131" s="7">
         <v>1</v>
@@ -14831,29 +14917,29 @@
         <v>53</v>
       </c>
       <c r="V131" s="7" t="s">
-        <v>951</v>
+        <v>959</v>
       </c>
       <c r="W131" s="7" t="s">
-        <v>924</v>
+        <v>896</v>
       </c>
       <c r="X131" s="7" t="s">
-        <v>925</v>
+        <v>960</v>
       </c>
       <c r="Y131" s="7"/>
       <c r="Z131" s="7">
-        <v>0.3</v>
+        <v>1.7</v>
       </c>
       <c r="AA131" s="7"/>
       <c r="AB131" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC131" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD131" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE131" s="7"/>
+        <v>961</v>
+      </c>
+      <c r="AD131" s="7"/>
+      <c r="AE131" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AF131" s="7"/>
       <c r="AG131" s="7"/>
       <c r="AH131" s="7"/>
@@ -14871,18 +14957,18 @@
         <v>78</v>
       </c>
       <c r="C132" s="3">
-        <v>2025082990</v>
+        <v>2025082988</v>
       </c>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
-      <c r="F132" s="3">
-        <v>2362</v>
+      <c r="F132" s="3" t="s">
+        <v>918</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>952</v>
+        <v>919</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
@@ -14893,13 +14979,13 @@
       <c r="O132" s="4"/>
       <c r="P132" s="10"/>
       <c r="Q132" s="3" t="s">
-        <v>953</v>
+        <v>922</v>
       </c>
       <c r="R132" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S132" s="3" t="s">
-        <v>72</v>
+        <v>210</v>
       </c>
       <c r="T132" s="3">
         <v>1</v>
@@ -14908,13 +14994,13 @@
         <v>53</v>
       </c>
       <c r="V132" s="3" t="s">
-        <v>954</v>
+        <v>962</v>
       </c>
       <c r="W132" s="3" t="s">
-        <v>955</v>
+        <v>924</v>
       </c>
       <c r="X132" s="3" t="s">
-        <v>956</v>
+        <v>925</v>
       </c>
       <c r="Y132" s="3"/>
       <c r="Z132" s="3">
@@ -14948,18 +15034,18 @@
         <v>78</v>
       </c>
       <c r="C133" s="7">
-        <v>2025082991</v>
+        <v>2025082990</v>
       </c>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
       <c r="F133" s="7">
-        <v>5082</v>
+        <v>2362</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>935</v>
+        <v>963</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>534</v>
+        <v>64</v>
       </c>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
@@ -14970,13 +15056,13 @@
       <c r="O133" s="8"/>
       <c r="P133" s="9"/>
       <c r="Q133" s="7" t="s">
-        <v>938</v>
+        <v>964</v>
       </c>
       <c r="R133" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S133" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T133" s="7">
         <v>1</v>
@@ -14985,17 +15071,17 @@
         <v>53</v>
       </c>
       <c r="V133" s="7" t="s">
-        <v>957</v>
+        <v>965</v>
       </c>
       <c r="W133" s="7" t="s">
-        <v>924</v>
+        <v>966</v>
       </c>
       <c r="X133" s="7" t="s">
-        <v>958</v>
+        <v>967</v>
       </c>
       <c r="Y133" s="7"/>
       <c r="Z133" s="7">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA133" s="7"/>
       <c r="AB133" s="7" t="s">
@@ -15025,18 +15111,18 @@
         <v>78</v>
       </c>
       <c r="C134" s="3">
-        <v>2025082995</v>
+        <v>2025082991</v>
       </c>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
       <c r="F134" s="3">
-        <v>4228</v>
+        <v>5082</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>959</v>
+        <v>935</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>64</v>
+        <v>534</v>
       </c>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
@@ -15047,13 +15133,13 @@
       <c r="O134" s="4"/>
       <c r="P134" s="10"/>
       <c r="Q134" s="3" t="s">
-        <v>960</v>
+        <v>938</v>
       </c>
       <c r="R134" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S134" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T134" s="3">
         <v>1</v>
@@ -15062,17 +15148,17 @@
         <v>53</v>
       </c>
       <c r="V134" s="3" t="s">
-        <v>961</v>
+        <v>968</v>
       </c>
       <c r="W134" s="3" t="s">
-        <v>962</v>
+        <v>924</v>
       </c>
       <c r="X134" s="3" t="s">
-        <v>963</v>
+        <v>969</v>
       </c>
       <c r="Y134" s="3"/>
       <c r="Z134" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA134" s="3"/>
       <c r="AB134" s="3" t="s">
@@ -15102,15 +15188,15 @@
         <v>78</v>
       </c>
       <c r="C135" s="7">
-        <v>2025083005</v>
+        <v>2025082995</v>
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
       <c r="F135" s="7">
-        <v>4679</v>
+        <v>4228</v>
       </c>
       <c r="G135" s="7" t="s">
-        <v>964</v>
+        <v>970</v>
       </c>
       <c r="H135" s="7" t="s">
         <v>64</v>
@@ -15122,9 +15208,9 @@
       <c r="M135" s="8"/>
       <c r="N135" s="7"/>
       <c r="O135" s="8"/>
-      <c r="P135" s="8"/>
+      <c r="P135" s="9"/>
       <c r="Q135" s="7" t="s">
-        <v>965</v>
+        <v>971</v>
       </c>
       <c r="R135" s="7" t="s">
         <v>51</v>
@@ -15139,13 +15225,13 @@
         <v>53</v>
       </c>
       <c r="V135" s="7" t="s">
-        <v>966</v>
+        <v>972</v>
       </c>
       <c r="W135" s="7" t="s">
-        <v>967</v>
+        <v>973</v>
       </c>
       <c r="X135" s="7" t="s">
-        <v>968</v>
+        <v>974</v>
       </c>
       <c r="Y135" s="7"/>
       <c r="Z135" s="7">
@@ -15155,8 +15241,8 @@
       <c r="AB135" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC135" s="8" t="s">
-        <v>479</v>
+      <c r="AC135" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="AD135" s="7" t="s">
         <v>60</v>
@@ -15166,10 +15252,241 @@
       <c r="AG135" s="7"/>
       <c r="AH135" s="7"/>
       <c r="AI135" s="7"/>
-      <c r="AJ135" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ135" s="7"/>
       <c r="AK135" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="136" spans="1:37">
+      <c r="A136" s="3">
+        <v>134</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C136" s="3">
+        <v>2025083005</v>
+      </c>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="3">
+        <v>4679</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>975</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I136" s="3"/>
+      <c r="J136" s="3"/>
+      <c r="K136" s="3"/>
+      <c r="L136" s="3"/>
+      <c r="M136" s="4"/>
+      <c r="N136" s="3"/>
+      <c r="O136" s="4"/>
+      <c r="P136" s="10"/>
+      <c r="Q136" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="R136" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S136" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T136" s="3">
+        <v>1</v>
+      </c>
+      <c r="U136" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V136" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="W136" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="X136" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="Y136" s="3"/>
+      <c r="Z136" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA136" s="3"/>
+      <c r="AB136" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC136" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="AD136" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE136" s="3"/>
+      <c r="AF136" s="3"/>
+      <c r="AG136" s="3"/>
+      <c r="AH136" s="3"/>
+      <c r="AI136" s="3"/>
+      <c r="AJ136" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK136" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:37">
+      <c r="A137" s="7">
+        <v>135</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C137" s="7">
+        <v>2025083011</v>
+      </c>
+      <c r="D137" s="7"/>
+      <c r="E137" s="7"/>
+      <c r="F137" s="7">
+        <v>4762</v>
+      </c>
+      <c r="G137" s="7" t="s">
+        <v>980</v>
+      </c>
+      <c r="H137" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I137" s="7"/>
+      <c r="J137" s="7"/>
+      <c r="K137" s="7"/>
+      <c r="L137" s="7"/>
+      <c r="M137" s="8"/>
+      <c r="N137" s="7"/>
+      <c r="O137" s="8"/>
+      <c r="P137" s="9"/>
+      <c r="Q137" s="7" t="s">
+        <v>981</v>
+      </c>
+      <c r="R137" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S137" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T137" s="7">
+        <v>1</v>
+      </c>
+      <c r="U137" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V137" s="7" t="s">
+        <v>982</v>
+      </c>
+      <c r="W137" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="X137" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="Y137" s="7"/>
+      <c r="Z137" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA137" s="7"/>
+      <c r="AB137" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC137" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD137" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE137" s="7"/>
+      <c r="AF137" s="7"/>
+      <c r="AG137" s="7"/>
+      <c r="AH137" s="7"/>
+      <c r="AI137" s="7"/>
+      <c r="AJ137" s="7"/>
+      <c r="AK137" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="138" spans="1:37">
+      <c r="A138" s="3">
+        <v>136</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C138" s="3">
+        <v>2025083035</v>
+      </c>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3">
+        <v>4218</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I138" s="3"/>
+      <c r="J138" s="3"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3"/>
+      <c r="M138" s="4"/>
+      <c r="N138" s="3"/>
+      <c r="O138" s="4"/>
+      <c r="P138" s="4"/>
+      <c r="Q138" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="R138" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S138" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T138" s="3">
+        <v>1</v>
+      </c>
+      <c r="U138" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V138" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="W138" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="X138" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="Y138" s="3"/>
+      <c r="Z138" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA138" s="3"/>
+      <c r="AB138" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC138" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="AD138" s="3"/>
+      <c r="AE138" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF138" s="3"/>
+      <c r="AG138" s="3"/>
+      <c r="AH138" s="3"/>
+      <c r="AI138" s="3"/>
+      <c r="AJ138" s="3"/>
+      <c r="AK138" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08261213
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$138</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$141</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="991">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-25  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1013">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-26  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3092,6 +3092,72 @@
   </si>
   <si>
     <t>撤機完成</t>
+  </si>
+  <si>
+    <t>15341114082601</t>
+  </si>
+  <si>
+    <t>蘆洲切仔麵</t>
+  </si>
+  <si>
+    <t>2025-08-26 10:50:21</t>
+  </si>
+  <si>
+    <t>HL34</t>
+  </si>
+  <si>
+    <t>HL-HUB</t>
+  </si>
+  <si>
+    <t>HUB週期維護</t>
+  </si>
+  <si>
+    <t>2025年07月份 hub調查異常:1PORT插在2PORT</t>
+  </si>
+  <si>
+    <t>THILF05341</t>
+  </si>
+  <si>
+    <t>2025-08-26 10:51:17</t>
+  </si>
+  <si>
+    <t>2025-08-26 10:27:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 10:57:00</t>
+  </si>
+  <si>
+    <t>2025-08-27 14:51:00</t>
+  </si>
+  <si>
+    <t>已將HUB網路線2PORT改接至1PORT</t>
+  </si>
+  <si>
+    <t>2025-08-26 11:02:28</t>
+  </si>
+  <si>
+    <t>2025-08-26 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 11:01:00</t>
+  </si>
+  <si>
+    <t>PMQ3+EDC+PEP安裝完成</t>
+  </si>
+  <si>
+    <t>蘆洲希望店</t>
+  </si>
+  <si>
+    <t>THILF05354</t>
+  </si>
+  <si>
+    <t>2025-08-26 11:58:59</t>
+  </si>
+  <si>
+    <t>2025-08-26 11:10:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 12:00:00</t>
   </si>
 </sst>
 </file>
@@ -3505,10 +3571,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK138"/>
+  <dimension ref="A1:AK141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC135" sqref="AC135"/>
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15441,7 +15507,7 @@
       <c r="M138" s="4"/>
       <c r="N138" s="3"/>
       <c r="O138" s="4"/>
-      <c r="P138" s="4"/>
+      <c r="P138" s="10"/>
       <c r="Q138" s="3" t="s">
         <v>986</v>
       </c>
@@ -15474,7 +15540,7 @@
       <c r="AB138" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC138" s="4" t="s">
+      <c r="AC138" s="10" t="s">
         <v>990</v>
       </c>
       <c r="AD138" s="3"/>
@@ -15487,6 +15553,261 @@
       <c r="AI138" s="3"/>
       <c r="AJ138" s="3"/>
       <c r="AK138" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="139" spans="1:37">
+      <c r="A139" s="7">
+        <v>137</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C139" s="7">
+        <v>2025083111</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>991</v>
+      </c>
+      <c r="E139" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F139" s="7">
+        <v>5341</v>
+      </c>
+      <c r="G139" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="H139" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I139" s="7" t="s">
+        <v>993</v>
+      </c>
+      <c r="J139" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="K139" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L139" s="7" t="s">
+        <v>994</v>
+      </c>
+      <c r="M139" s="8" t="s">
+        <v>995</v>
+      </c>
+      <c r="N139" s="7">
+        <v>3404</v>
+      </c>
+      <c r="O139" s="8" t="s">
+        <v>996</v>
+      </c>
+      <c r="P139" s="9" t="s">
+        <v>997</v>
+      </c>
+      <c r="Q139" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="R139" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S139" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T139" s="7">
+        <v>1</v>
+      </c>
+      <c r="U139" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V139" s="7" t="s">
+        <v>999</v>
+      </c>
+      <c r="W139" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="X139" s="7" t="s">
+        <v>1001</v>
+      </c>
+      <c r="Y139" s="7" t="s">
+        <v>1002</v>
+      </c>
+      <c r="Z139" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA139" s="7"/>
+      <c r="AB139" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC139" s="9" t="s">
+        <v>1003</v>
+      </c>
+      <c r="AD139" s="7"/>
+      <c r="AE139" s="7"/>
+      <c r="AF139" s="7"/>
+      <c r="AG139" s="7"/>
+      <c r="AH139" s="7"/>
+      <c r="AI139" s="7"/>
+      <c r="AJ139" s="7"/>
+      <c r="AK139" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140" spans="1:37">
+      <c r="A140" s="3">
+        <v>138</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C140" s="3">
+        <v>2025083115</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3">
+        <v>5341</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I140" s="3"/>
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="3"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="3"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="10"/>
+      <c r="Q140" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="R140" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S140" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T140" s="3">
+        <v>1</v>
+      </c>
+      <c r="U140" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V140" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="W140" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="X140" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="Y140" s="3"/>
+      <c r="Z140" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA140" s="3"/>
+      <c r="AB140" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC140" s="10" t="s">
+        <v>1007</v>
+      </c>
+      <c r="AD140" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE140" s="3"/>
+      <c r="AF140" s="3"/>
+      <c r="AG140" s="3"/>
+      <c r="AH140" s="3"/>
+      <c r="AI140" s="3"/>
+      <c r="AJ140" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK140" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="141" spans="1:37">
+      <c r="A141" s="7">
+        <v>139</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C141" s="7">
+        <v>2025083127</v>
+      </c>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+      <c r="F141" s="7">
+        <v>5354</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H141" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I141" s="7"/>
+      <c r="J141" s="7"/>
+      <c r="K141" s="7"/>
+      <c r="L141" s="7"/>
+      <c r="M141" s="8"/>
+      <c r="N141" s="7"/>
+      <c r="O141" s="8"/>
+      <c r="P141" s="8"/>
+      <c r="Q141" s="7" t="s">
+        <v>1009</v>
+      </c>
+      <c r="R141" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S141" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T141" s="7">
+        <v>1</v>
+      </c>
+      <c r="U141" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V141" s="7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="W141" s="7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="X141" s="7" t="s">
+        <v>1012</v>
+      </c>
+      <c r="Y141" s="7"/>
+      <c r="Z141" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA141" s="7"/>
+      <c r="AB141" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC141" s="8" t="s">
+        <v>1007</v>
+      </c>
+      <c r="AD141" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE141" s="7"/>
+      <c r="AF141" s="7"/>
+      <c r="AG141" s="7"/>
+      <c r="AH141" s="7"/>
+      <c r="AI141" s="7"/>
+      <c r="AJ141" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK141" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08261731
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$141</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$145</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1033">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-26  )</t>
   </si>
@@ -3094,6 +3094,38 @@
     <t>撤機完成</t>
   </si>
   <si>
+    <t>12399114082601</t>
+  </si>
+  <si>
+    <t>三重三陽店</t>
+  </si>
+  <si>
+    <t>2025-08-26 09:05:43</t>
+  </si>
+  <si>
+    <t>08/26 09:05 啟動緊急叫修:門市sc(SHUTTLE6S)點選訂貨3.0、hipos、e網都會出現【捷徑\'HISHOP.lnk\'參照的磁碟機或網路連線無法使用。請確定插入的磁碟正確，而且網路資源可以使用，然後重試。】，重啟SC仍異常。因開啟[訂貨3.0][HiShop][E網]出現捷徑異常訊息，請更換第二顆硬碟不備份還原，並攜帶主機隨行檢測...請台芝到店協助 
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 
+與門市確認帳務做到08/25，與通訊功評確認有收到08/25的銷售</t>
+  </si>
+  <si>
+    <t>THILF02399</t>
+  </si>
+  <si>
+    <t>2025-08-26 09:08:13</t>
+  </si>
+  <si>
+    <t>2025-08-26 12:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 14:15:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 15:08:00</t>
+  </si>
+  <si>
+    <t>更換第二顆硬碟不備份還原，更換STAT線*1</t>
+  </si>
+  <si>
     <t>15341114082601</t>
   </si>
   <si>
@@ -3158,6 +3190,36 @@
   </si>
   <si>
     <t>2025-08-26 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 14:18:53</t>
+  </si>
+  <si>
+    <t>2025-08-26 14:17:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 15:03:45</t>
+  </si>
+  <si>
+    <t>2025-08-26 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 15:03:00</t>
+  </si>
+  <si>
+    <t>撤機裝潢完成</t>
+  </si>
+  <si>
+    <t>2025-08-26 15:04:17</t>
+  </si>
+  <si>
+    <t>2025-08-26 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-26 15:10:00</t>
+  </si>
+  <si>
+    <t>撤店</t>
   </si>
 </sst>
 </file>
@@ -3571,10 +3633,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK141"/>
+  <dimension ref="A1:AK145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A141" sqref="A141"/>
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15564,22 +15626,22 @@
         <v>38</v>
       </c>
       <c r="C139" s="7">
-        <v>2025083111</v>
+        <v>2025083088</v>
       </c>
       <c r="D139" s="7" t="s">
         <v>991</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>40</v>
+        <v>382</v>
       </c>
       <c r="F139" s="7">
-        <v>5341</v>
+        <v>2399</v>
       </c>
       <c r="G139" s="7" t="s">
         <v>992</v>
       </c>
       <c r="H139" s="7" t="s">
-        <v>534</v>
+        <v>42</v>
       </c>
       <c r="I139" s="7" t="s">
         <v>993</v>
@@ -15591,22 +15653,22 @@
         <v>45</v>
       </c>
       <c r="L139" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M139" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N139" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O139" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="P139" s="9" t="s">
         <v>994</v>
       </c>
-      <c r="M139" s="8" t="s">
+      <c r="Q139" s="7" t="s">
         <v>995</v>
-      </c>
-      <c r="N139" s="7">
-        <v>3404</v>
-      </c>
-      <c r="O139" s="8" t="s">
-        <v>996</v>
-      </c>
-      <c r="P139" s="9" t="s">
-        <v>997</v>
-      </c>
-      <c r="Q139" s="7" t="s">
-        <v>998</v>
       </c>
       <c r="R139" s="7" t="s">
         <v>51</v>
@@ -15621,26 +15683,26 @@
         <v>53</v>
       </c>
       <c r="V139" s="7" t="s">
+        <v>996</v>
+      </c>
+      <c r="W139" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="X139" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="Y139" s="7" t="s">
         <v>999</v>
       </c>
-      <c r="W139" s="7" t="s">
-        <v>1000</v>
-      </c>
-      <c r="X139" s="7" t="s">
-        <v>1001</v>
-      </c>
-      <c r="Y139" s="7" t="s">
-        <v>1002</v>
-      </c>
       <c r="Z139" s="7">
-        <v>0.5</v>
+        <v>1.8</v>
       </c>
       <c r="AA139" s="7"/>
       <c r="AB139" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC139" s="9" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="AD139" s="7"/>
       <c r="AE139" s="7"/>
@@ -15658,32 +15720,52 @@
         <v>138</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C140" s="3">
-        <v>2025083115</v>
-      </c>
-      <c r="D140" s="3"/>
-      <c r="E140" s="3"/>
+        <v>2025083111</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F140" s="3">
         <v>5341</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>992</v>
+        <v>1002</v>
       </c>
       <c r="H140" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="I140" s="3"/>
-      <c r="J140" s="3"/>
-      <c r="K140" s="3"/>
-      <c r="L140" s="3"/>
-      <c r="M140" s="4"/>
-      <c r="N140" s="3"/>
-      <c r="O140" s="4"/>
-      <c r="P140" s="10"/>
+      <c r="I140" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J140" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="K140" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L140" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="M140" s="4" t="s">
+        <v>1005</v>
+      </c>
+      <c r="N140" s="3">
+        <v>3404</v>
+      </c>
+      <c r="O140" s="4" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P140" s="10" t="s">
+        <v>1007</v>
+      </c>
       <c r="Q140" s="3" t="s">
-        <v>998</v>
+        <v>1008</v>
       </c>
       <c r="R140" s="3" t="s">
         <v>51</v>
@@ -15698,36 +15780,34 @@
         <v>53</v>
       </c>
       <c r="V140" s="3" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="W140" s="3" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="X140" s="3" t="s">
-        <v>1006</v>
-      </c>
-      <c r="Y140" s="3"/>
+        <v>1011</v>
+      </c>
+      <c r="Y140" s="3" t="s">
+        <v>1012</v>
+      </c>
       <c r="Z140" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AA140" s="3"/>
       <c r="AB140" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC140" s="10" t="s">
-        <v>1007</v>
-      </c>
-      <c r="AD140" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>1013</v>
+      </c>
+      <c r="AD140" s="3"/>
       <c r="AE140" s="3"/>
       <c r="AF140" s="3"/>
       <c r="AG140" s="3"/>
       <c r="AH140" s="3"/>
       <c r="AI140" s="3"/>
-      <c r="AJ140" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ140" s="3"/>
       <c r="AK140" s="3" t="s">
         <v>60</v>
       </c>
@@ -15740,15 +15820,15 @@
         <v>78</v>
       </c>
       <c r="C141" s="7">
-        <v>2025083127</v>
+        <v>2025083115</v>
       </c>
       <c r="D141" s="7"/>
       <c r="E141" s="7"/>
       <c r="F141" s="7">
-        <v>5354</v>
+        <v>5341</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="H141" s="7" t="s">
         <v>534</v>
@@ -15760,9 +15840,9 @@
       <c r="M141" s="8"/>
       <c r="N141" s="7"/>
       <c r="O141" s="8"/>
-      <c r="P141" s="8"/>
+      <c r="P141" s="9"/>
       <c r="Q141" s="7" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="R141" s="7" t="s">
         <v>51</v>
@@ -15777,24 +15857,24 @@
         <v>53</v>
       </c>
       <c r="V141" s="7" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="W141" s="7" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="X141" s="7" t="s">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="Y141" s="7"/>
       <c r="Z141" s="7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AA141" s="7"/>
       <c r="AB141" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC141" s="8" t="s">
-        <v>1007</v>
+      <c r="AC141" s="9" t="s">
+        <v>1017</v>
       </c>
       <c r="AD141" s="7" t="s">
         <v>60</v>
@@ -15808,6 +15888,316 @@
         <v>60</v>
       </c>
       <c r="AK141" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="142" spans="1:37">
+      <c r="A142" s="3">
+        <v>140</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C142" s="3">
+        <v>2025083127</v>
+      </c>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3">
+        <v>5354</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I142" s="3"/>
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="3"/>
+      <c r="O142" s="4"/>
+      <c r="P142" s="10"/>
+      <c r="Q142" s="3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="R142" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S142" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T142" s="3">
+        <v>1</v>
+      </c>
+      <c r="U142" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V142" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="W142" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="X142" s="3" t="s">
+        <v>1022</v>
+      </c>
+      <c r="Y142" s="3"/>
+      <c r="Z142" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA142" s="3"/>
+      <c r="AB142" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC142" s="10" t="s">
+        <v>1017</v>
+      </c>
+      <c r="AD142" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE142" s="3"/>
+      <c r="AF142" s="3"/>
+      <c r="AG142" s="3"/>
+      <c r="AH142" s="3"/>
+      <c r="AI142" s="3"/>
+      <c r="AJ142" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK142" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="143" spans="1:37">
+      <c r="A143" s="7">
+        <v>141</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C143" s="7">
+        <v>2025083142</v>
+      </c>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
+      <c r="F143" s="7">
+        <v>2399</v>
+      </c>
+      <c r="G143" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="H143" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I143" s="7"/>
+      <c r="J143" s="7"/>
+      <c r="K143" s="7"/>
+      <c r="L143" s="7"/>
+      <c r="M143" s="8"/>
+      <c r="N143" s="7"/>
+      <c r="O143" s="8"/>
+      <c r="P143" s="9"/>
+      <c r="Q143" s="7" t="s">
+        <v>995</v>
+      </c>
+      <c r="R143" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S143" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T143" s="7">
+        <v>1</v>
+      </c>
+      <c r="U143" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V143" s="7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="W143" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="X143" s="7" t="s">
+        <v>1024</v>
+      </c>
+      <c r="Y143" s="7"/>
+      <c r="Z143" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="AA143" s="7"/>
+      <c r="AB143" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC143" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD143" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE143" s="7"/>
+      <c r="AF143" s="7"/>
+      <c r="AG143" s="7"/>
+      <c r="AH143" s="7"/>
+      <c r="AI143" s="7"/>
+      <c r="AJ143" s="7"/>
+      <c r="AK143" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:37">
+      <c r="A144" s="3">
+        <v>142</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C144" s="3">
+        <v>2025083159</v>
+      </c>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3">
+        <v>3929</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="10"/>
+      <c r="Q144" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="R144" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S144" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T144" s="3">
+        <v>1</v>
+      </c>
+      <c r="U144" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V144" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="W144" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="X144" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="Y144" s="3"/>
+      <c r="Z144" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA144" s="3"/>
+      <c r="AB144" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC144" s="10" t="s">
+        <v>1028</v>
+      </c>
+      <c r="AD144" s="3"/>
+      <c r="AE144" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF144" s="3"/>
+      <c r="AG144" s="3"/>
+      <c r="AH144" s="3"/>
+      <c r="AI144" s="3"/>
+      <c r="AJ144" s="3"/>
+      <c r="AK144" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="145" spans="1:37">
+      <c r="A145" s="7">
+        <v>143</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C145" s="7">
+        <v>2025083160</v>
+      </c>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="7">
+        <v>3929</v>
+      </c>
+      <c r="G145" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="H145" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I145" s="7"/>
+      <c r="J145" s="7"/>
+      <c r="K145" s="7"/>
+      <c r="L145" s="7"/>
+      <c r="M145" s="8"/>
+      <c r="N145" s="7"/>
+      <c r="O145" s="8"/>
+      <c r="P145" s="8"/>
+      <c r="Q145" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="R145" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S145" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T145" s="7">
+        <v>1</v>
+      </c>
+      <c r="U145" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V145" s="7" t="s">
+        <v>1029</v>
+      </c>
+      <c r="W145" s="7" t="s">
+        <v>1030</v>
+      </c>
+      <c r="X145" s="7" t="s">
+        <v>1031</v>
+      </c>
+      <c r="Y145" s="7"/>
+      <c r="Z145" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AA145" s="7"/>
+      <c r="AB145" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC145" s="8" t="s">
+        <v>1032</v>
+      </c>
+      <c r="AD145" s="7"/>
+      <c r="AE145" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF145" s="7"/>
+      <c r="AG145" s="7"/>
+      <c r="AH145" s="7"/>
+      <c r="AI145" s="7"/>
+      <c r="AJ145" s="7"/>
+      <c r="AK145" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08271340
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$145</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$148</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1033">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-26  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1058">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-27  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3094,6 +3094,40 @@
     <t>撤機完成</t>
   </si>
   <si>
+    <t>E4406114082601</t>
+  </si>
+  <si>
+    <t>板橋稚暉店</t>
+  </si>
+  <si>
+    <t>2025-08-26 08:21:42</t>
+  </si>
+  <si>
+    <t>無電源反應、無法開機</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應LIFEET印票機L90無電源反應無亮燈，已有按壓電源鍵也無法開機，門市告知因繁忙無法協助重新拔插線路...請台芝到店協助(票卷機沒訂位紙印不出來)
+</t>
+  </si>
+  <si>
+    <t>THILF04406</t>
+  </si>
+  <si>
+    <t>2025-08-26 09:03:01</t>
+  </si>
+  <si>
+    <t>2025-08-27 11:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-27 12:25:00</t>
+  </si>
+  <si>
+    <t>2025-08-27 13:03:00</t>
+  </si>
+  <si>
+    <t>電源線鬆脫，重插後正常</t>
+  </si>
+  <si>
     <t>12399114082601</t>
   </si>
   <si>
@@ -3177,6 +3211,43 @@
     <t>PMQ3+EDC+PEP安裝完成</t>
   </si>
   <si>
+    <t>15080114082601</t>
+  </si>
+  <si>
+    <t>三芝楓愛林</t>
+  </si>
+  <si>
+    <t>新北市三芝區</t>
+  </si>
+  <si>
+    <t>2025-08-26 11:54:19</t>
+  </si>
+  <si>
+    <t>錢匣損壞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應tm1收銀機(TCX800)(抽屜顏色:白色、鑰匙孔位子(右)、鎖頭編號:726)夾紙鈔彈簧斷掉...請台芝到店協助
+</t>
+  </si>
+  <si>
+    <t>THILF05080</t>
+  </si>
+  <si>
+    <t>2025-08-26 11:56:49</t>
+  </si>
+  <si>
+    <t>2025-08-27 11:44:00</t>
+  </si>
+  <si>
+    <t>2025-08-27 12:14:00</t>
+  </si>
+  <si>
+    <t>2025-08-27 15:56:00</t>
+  </si>
+  <si>
+    <t>更換紙鈔夾</t>
+  </si>
+  <si>
     <t>蘆洲希望店</t>
   </si>
   <si>
@@ -3220,6 +3291,12 @@
   </si>
   <si>
     <t>撤店</t>
+  </si>
+  <si>
+    <t>2025-08-27 12:30:02</t>
+  </si>
+  <si>
+    <t>2025-08-27 12:10:00</t>
   </si>
 </sst>
 </file>
@@ -3633,10 +3710,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK145"/>
+  <dimension ref="A1:AK148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A145" sqref="A145"/>
+      <selection activeCell="AC145" sqref="AC145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15626,22 +15703,22 @@
         <v>38</v>
       </c>
       <c r="C139" s="7">
-        <v>2025083088</v>
+        <v>2025083086</v>
       </c>
       <c r="D139" s="7" t="s">
         <v>991</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>382</v>
+        <v>40</v>
       </c>
       <c r="F139" s="7">
-        <v>2399</v>
+        <v>4406</v>
       </c>
       <c r="G139" s="7" t="s">
         <v>992</v>
       </c>
       <c r="H139" s="7" t="s">
-        <v>42</v>
+        <v>206</v>
       </c>
       <c r="I139" s="7" t="s">
         <v>993</v>
@@ -15653,28 +15730,28 @@
         <v>45</v>
       </c>
       <c r="L139" s="7" t="s">
-        <v>67</v>
+        <v>276</v>
       </c>
       <c r="M139" s="8" t="s">
-        <v>68</v>
+        <v>277</v>
       </c>
       <c r="N139" s="7">
-        <v>2405</v>
+        <v>6004</v>
       </c>
       <c r="O139" s="8" t="s">
-        <v>386</v>
+        <v>994</v>
       </c>
       <c r="P139" s="9" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="Q139" s="7" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="R139" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S139" s="7" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="T139" s="7">
         <v>1</v>
@@ -15683,26 +15760,26 @@
         <v>53</v>
       </c>
       <c r="V139" s="7" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="W139" s="7" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="X139" s="7" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="Y139" s="7" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="Z139" s="7">
-        <v>1.8</v>
+        <v>0.6</v>
       </c>
       <c r="AA139" s="7"/>
       <c r="AB139" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC139" s="9" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="AD139" s="7"/>
       <c r="AE139" s="7"/>
@@ -15723,25 +15800,25 @@
         <v>38</v>
       </c>
       <c r="C140" s="3">
-        <v>2025083111</v>
+        <v>2025083088</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>40</v>
+        <v>382</v>
       </c>
       <c r="F140" s="3">
-        <v>5341</v>
+        <v>2399</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>534</v>
+        <v>42</v>
       </c>
       <c r="I140" s="3" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="J140" s="3" t="s">
         <v>230</v>
@@ -15750,22 +15827,22 @@
         <v>45</v>
       </c>
       <c r="L140" s="3" t="s">
-        <v>1004</v>
+        <v>67</v>
       </c>
       <c r="M140" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N140" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O140" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="P140" s="10" t="s">
         <v>1005</v>
       </c>
-      <c r="N140" s="3">
-        <v>3404</v>
-      </c>
-      <c r="O140" s="4" t="s">
+      <c r="Q140" s="3" t="s">
         <v>1006</v>
-      </c>
-      <c r="P140" s="10" t="s">
-        <v>1007</v>
-      </c>
-      <c r="Q140" s="3" t="s">
-        <v>1008</v>
       </c>
       <c r="R140" s="3" t="s">
         <v>51</v>
@@ -15780,26 +15857,26 @@
         <v>53</v>
       </c>
       <c r="V140" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="W140" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="X140" s="3" t="s">
         <v>1009</v>
       </c>
-      <c r="W140" s="3" t="s">
+      <c r="Y140" s="3" t="s">
         <v>1010</v>
       </c>
-      <c r="X140" s="3" t="s">
-        <v>1011</v>
-      </c>
-      <c r="Y140" s="3" t="s">
-        <v>1012</v>
-      </c>
       <c r="Z140" s="3">
-        <v>0.5</v>
+        <v>1.8</v>
       </c>
       <c r="AA140" s="3"/>
       <c r="AB140" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC140" s="10" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="AD140" s="3"/>
       <c r="AE140" s="3"/>
@@ -15817,32 +15894,52 @@
         <v>139</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C141" s="7">
-        <v>2025083115</v>
-      </c>
-      <c r="D141" s="7"/>
-      <c r="E141" s="7"/>
+        <v>2025083111</v>
+      </c>
+      <c r="D141" s="7" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E141" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F141" s="7">
         <v>5341</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>1002</v>
+        <v>1013</v>
       </c>
       <c r="H141" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="I141" s="7"/>
-      <c r="J141" s="7"/>
-      <c r="K141" s="7"/>
-      <c r="L141" s="7"/>
-      <c r="M141" s="8"/>
-      <c r="N141" s="7"/>
-      <c r="O141" s="8"/>
-      <c r="P141" s="9"/>
+      <c r="I141" s="7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J141" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="K141" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L141" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="M141" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="N141" s="7">
+        <v>3404</v>
+      </c>
+      <c r="O141" s="8" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P141" s="9" t="s">
+        <v>1018</v>
+      </c>
       <c r="Q141" s="7" t="s">
-        <v>1008</v>
+        <v>1019</v>
       </c>
       <c r="R141" s="7" t="s">
         <v>51</v>
@@ -15857,36 +15954,34 @@
         <v>53</v>
       </c>
       <c r="V141" s="7" t="s">
-        <v>1014</v>
+        <v>1020</v>
       </c>
       <c r="W141" s="7" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="X141" s="7" t="s">
-        <v>1016</v>
-      </c>
-      <c r="Y141" s="7"/>
+        <v>1022</v>
+      </c>
+      <c r="Y141" s="7" t="s">
+        <v>1023</v>
+      </c>
       <c r="Z141" s="7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AA141" s="7"/>
       <c r="AB141" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC141" s="9" t="s">
-        <v>1017</v>
-      </c>
-      <c r="AD141" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>1024</v>
+      </c>
+      <c r="AD141" s="7"/>
       <c r="AE141" s="7"/>
       <c r="AF141" s="7"/>
       <c r="AG141" s="7"/>
       <c r="AH141" s="7"/>
       <c r="AI141" s="7"/>
-      <c r="AJ141" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ141" s="7"/>
       <c r="AK141" s="7" t="s">
         <v>60</v>
       </c>
@@ -15899,15 +15994,15 @@
         <v>78</v>
       </c>
       <c r="C142" s="3">
-        <v>2025083127</v>
+        <v>2025083115</v>
       </c>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
       <c r="F142" s="3">
-        <v>5354</v>
+        <v>5341</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>1018</v>
+        <v>1013</v>
       </c>
       <c r="H142" s="3" t="s">
         <v>534</v>
@@ -15936,24 +16031,24 @@
         <v>53</v>
       </c>
       <c r="V142" s="3" t="s">
-        <v>1020</v>
+        <v>1025</v>
       </c>
       <c r="W142" s="3" t="s">
-        <v>1021</v>
+        <v>1026</v>
       </c>
       <c r="X142" s="3" t="s">
-        <v>1022</v>
+        <v>1027</v>
       </c>
       <c r="Y142" s="3"/>
       <c r="Z142" s="3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AA142" s="3"/>
       <c r="AB142" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC142" s="10" t="s">
-        <v>1017</v>
+        <v>1028</v>
       </c>
       <c r="AD142" s="3" t="s">
         <v>60</v>
@@ -15975,32 +16070,52 @@
         <v>141</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C143" s="7">
-        <v>2025083142</v>
-      </c>
-      <c r="D143" s="7"/>
-      <c r="E143" s="7"/>
+        <v>2025083126</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F143" s="7">
-        <v>2399</v>
+        <v>5080</v>
       </c>
       <c r="G143" s="7" t="s">
-        <v>992</v>
+        <v>1030</v>
       </c>
       <c r="H143" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I143" s="7"/>
-      <c r="J143" s="7"/>
-      <c r="K143" s="7"/>
-      <c r="L143" s="7"/>
-      <c r="M143" s="8"/>
-      <c r="N143" s="7"/>
-      <c r="O143" s="8"/>
-      <c r="P143" s="9"/>
+        <v>1031</v>
+      </c>
+      <c r="I143" s="7" t="s">
+        <v>1032</v>
+      </c>
+      <c r="J143" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="K143" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L143" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M143" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N143" s="7">
+        <v>2304</v>
+      </c>
+      <c r="O143" s="8" t="s">
+        <v>1033</v>
+      </c>
+      <c r="P143" s="9" t="s">
+        <v>1034</v>
+      </c>
       <c r="Q143" s="7" t="s">
-        <v>995</v>
+        <v>1035</v>
       </c>
       <c r="R143" s="7" t="s">
         <v>51</v>
@@ -16015,28 +16130,28 @@
         <v>53</v>
       </c>
       <c r="V143" s="7" t="s">
-        <v>1023</v>
+        <v>1036</v>
       </c>
       <c r="W143" s="7" t="s">
-        <v>997</v>
+        <v>1037</v>
       </c>
       <c r="X143" s="7" t="s">
-        <v>1024</v>
-      </c>
-      <c r="Y143" s="7"/>
+        <v>1038</v>
+      </c>
+      <c r="Y143" s="7" t="s">
+        <v>1039</v>
+      </c>
       <c r="Z143" s="7">
-        <v>1.8</v>
+        <v>0.5</v>
       </c>
       <c r="AA143" s="7"/>
       <c r="AB143" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC143" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD143" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>1040</v>
+      </c>
+      <c r="AD143" s="7"/>
       <c r="AE143" s="7"/>
       <c r="AF143" s="7"/>
       <c r="AG143" s="7"/>
@@ -16055,15 +16170,15 @@
         <v>78</v>
       </c>
       <c r="C144" s="3">
-        <v>2025083159</v>
+        <v>2025083127</v>
       </c>
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
       <c r="F144" s="3">
-        <v>3929</v>
+        <v>5354</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>662</v>
+        <v>1041</v>
       </c>
       <c r="H144" s="3" t="s">
         <v>534</v>
@@ -16077,7 +16192,7 @@
       <c r="O144" s="4"/>
       <c r="P144" s="10"/>
       <c r="Q144" s="3" t="s">
-        <v>665</v>
+        <v>1042</v>
       </c>
       <c r="R144" s="3" t="s">
         <v>51</v>
@@ -16092,17 +16207,17 @@
         <v>53</v>
       </c>
       <c r="V144" s="3" t="s">
-        <v>1025</v>
+        <v>1043</v>
       </c>
       <c r="W144" s="3" t="s">
-        <v>1026</v>
+        <v>1044</v>
       </c>
       <c r="X144" s="3" t="s">
-        <v>1027</v>
+        <v>1045</v>
       </c>
       <c r="Y144" s="3"/>
       <c r="Z144" s="3">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="AA144" s="3"/>
       <c r="AB144" s="3" t="s">
@@ -16111,15 +16226,17 @@
       <c r="AC144" s="10" t="s">
         <v>1028</v>
       </c>
-      <c r="AD144" s="3"/>
-      <c r="AE144" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AD144" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE144" s="3"/>
       <c r="AF144" s="3"/>
       <c r="AG144" s="3"/>
       <c r="AH144" s="3"/>
       <c r="AI144" s="3"/>
-      <c r="AJ144" s="3"/>
+      <c r="AJ144" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AK144" s="3" t="s">
         <v>60</v>
       </c>
@@ -16132,18 +16249,18 @@
         <v>78</v>
       </c>
       <c r="C145" s="7">
-        <v>2025083160</v>
+        <v>2025083142</v>
       </c>
       <c r="D145" s="7"/>
       <c r="E145" s="7"/>
       <c r="F145" s="7">
-        <v>3929</v>
+        <v>2399</v>
       </c>
       <c r="G145" s="7" t="s">
-        <v>662</v>
+        <v>1003</v>
       </c>
       <c r="H145" s="7" t="s">
-        <v>534</v>
+        <v>42</v>
       </c>
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
@@ -16152,15 +16269,15 @@
       <c r="M145" s="8"/>
       <c r="N145" s="7"/>
       <c r="O145" s="8"/>
-      <c r="P145" s="8"/>
+      <c r="P145" s="9"/>
       <c r="Q145" s="7" t="s">
-        <v>665</v>
+        <v>1006</v>
       </c>
       <c r="R145" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S145" s="7" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T145" s="7">
         <v>1</v>
@@ -16169,29 +16286,29 @@
         <v>53</v>
       </c>
       <c r="V145" s="7" t="s">
-        <v>1029</v>
+        <v>1046</v>
       </c>
       <c r="W145" s="7" t="s">
-        <v>1030</v>
+        <v>1008</v>
       </c>
       <c r="X145" s="7" t="s">
-        <v>1031</v>
+        <v>1047</v>
       </c>
       <c r="Y145" s="7"/>
       <c r="Z145" s="7">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="AA145" s="7"/>
       <c r="AB145" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC145" s="8" t="s">
-        <v>1032</v>
-      </c>
-      <c r="AD145" s="7"/>
-      <c r="AE145" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC145" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD145" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE145" s="7"/>
       <c r="AF145" s="7"/>
       <c r="AG145" s="7"/>
       <c r="AH145" s="7"/>
@@ -16200,6 +16317,235 @@
       <c r="AK145" s="7" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="146" spans="1:37">
+      <c r="A146" s="3">
+        <v>144</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C146" s="3">
+        <v>2025083159</v>
+      </c>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3">
+        <v>3929</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I146" s="3"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="3"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="10"/>
+      <c r="Q146" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="R146" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S146" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T146" s="3">
+        <v>1</v>
+      </c>
+      <c r="U146" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V146" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="W146" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="X146" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="Y146" s="3"/>
+      <c r="Z146" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA146" s="3"/>
+      <c r="AB146" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC146" s="10" t="s">
+        <v>1051</v>
+      </c>
+      <c r="AD146" s="3"/>
+      <c r="AE146" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF146" s="3"/>
+      <c r="AG146" s="3"/>
+      <c r="AH146" s="3"/>
+      <c r="AI146" s="3"/>
+      <c r="AJ146" s="3"/>
+      <c r="AK146" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="147" spans="1:37">
+      <c r="A147" s="7">
+        <v>145</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C147" s="7">
+        <v>2025083160</v>
+      </c>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="7">
+        <v>3929</v>
+      </c>
+      <c r="G147" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="H147" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I147" s="7"/>
+      <c r="J147" s="7"/>
+      <c r="K147" s="7"/>
+      <c r="L147" s="7"/>
+      <c r="M147" s="8"/>
+      <c r="N147" s="7"/>
+      <c r="O147" s="8"/>
+      <c r="P147" s="9"/>
+      <c r="Q147" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="R147" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S147" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T147" s="7">
+        <v>1</v>
+      </c>
+      <c r="U147" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V147" s="7" t="s">
+        <v>1052</v>
+      </c>
+      <c r="W147" s="7" t="s">
+        <v>1053</v>
+      </c>
+      <c r="X147" s="7" t="s">
+        <v>1054</v>
+      </c>
+      <c r="Y147" s="7"/>
+      <c r="Z147" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AA147" s="7"/>
+      <c r="AB147" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC147" s="9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="AD147" s="7"/>
+      <c r="AE147" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF147" s="7"/>
+      <c r="AG147" s="7"/>
+      <c r="AH147" s="7"/>
+      <c r="AI147" s="7"/>
+      <c r="AJ147" s="7"/>
+      <c r="AK147" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="148" spans="1:37">
+      <c r="A148" s="3">
+        <v>146</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C148" s="3">
+        <v>2025083311</v>
+      </c>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3">
+        <v>4406</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="4"/>
+      <c r="N148" s="3"/>
+      <c r="O148" s="4"/>
+      <c r="P148" s="4"/>
+      <c r="Q148" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="R148" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S148" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="T148" s="3">
+        <v>1</v>
+      </c>
+      <c r="U148" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V148" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="W148" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="X148" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="Y148" s="3"/>
+      <c r="Z148" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA148" s="3"/>
+      <c r="AB148" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC148" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD148" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE148" s="3"/>
+      <c r="AF148" s="3"/>
+      <c r="AG148" s="3"/>
+      <c r="AH148" s="3"/>
+      <c r="AI148" s="3"/>
+      <c r="AJ148" s="3"/>
+      <c r="AK148" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Auto commit - 08271723
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$148</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$150</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1066">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-27  )</t>
   </si>
@@ -3297,6 +3297,30 @@
   </si>
   <si>
     <t>2025-08-27 12:10:00</t>
+  </si>
+  <si>
+    <t>金山銀山店</t>
+  </si>
+  <si>
+    <t>THILF04906</t>
+  </si>
+  <si>
+    <t>2025-08-27 15:39:41</t>
+  </si>
+  <si>
+    <t>2025-08-27 15:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-27 15:40:00</t>
+  </si>
+  <si>
+    <t>2025-08-27 16:00:14</t>
+  </si>
+  <si>
+    <t>2025-08-27 15:44:00</t>
+  </si>
+  <si>
+    <t>2025-08-27 16:05:00</t>
   </si>
 </sst>
 </file>
@@ -3710,10 +3734,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK148"/>
+  <dimension ref="A1:AK150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC145" sqref="AC145"/>
+      <selection activeCell="AC147" sqref="AC147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16500,7 +16524,7 @@
       <c r="M148" s="4"/>
       <c r="N148" s="3"/>
       <c r="O148" s="4"/>
-      <c r="P148" s="4"/>
+      <c r="P148" s="10"/>
       <c r="Q148" s="3" t="s">
         <v>996</v>
       </c>
@@ -16533,7 +16557,7 @@
       <c r="AB148" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC148" s="4" t="s">
+      <c r="AC148" s="10" t="s">
         <v>84</v>
       </c>
       <c r="AD148" s="3" t="s">
@@ -16546,6 +16570,160 @@
       <c r="AI148" s="3"/>
       <c r="AJ148" s="3"/>
       <c r="AK148" s="3"/>
+    </row>
+    <row r="149" spans="1:37">
+      <c r="A149" s="7">
+        <v>147</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C149" s="7">
+        <v>2025083336</v>
+      </c>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7">
+        <v>4906</v>
+      </c>
+      <c r="G149" s="7" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H149" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="I149" s="7"/>
+      <c r="J149" s="7"/>
+      <c r="K149" s="7"/>
+      <c r="L149" s="7"/>
+      <c r="M149" s="8"/>
+      <c r="N149" s="7"/>
+      <c r="O149" s="8"/>
+      <c r="P149" s="9"/>
+      <c r="Q149" s="7" t="s">
+        <v>1059</v>
+      </c>
+      <c r="R149" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S149" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T149" s="7">
+        <v>1</v>
+      </c>
+      <c r="U149" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V149" s="7" t="s">
+        <v>1060</v>
+      </c>
+      <c r="W149" s="7" t="s">
+        <v>1061</v>
+      </c>
+      <c r="X149" s="7" t="s">
+        <v>1062</v>
+      </c>
+      <c r="Y149" s="7"/>
+      <c r="Z149" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA149" s="7"/>
+      <c r="AB149" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC149" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD149" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE149" s="7"/>
+      <c r="AF149" s="7"/>
+      <c r="AG149" s="7"/>
+      <c r="AH149" s="7"/>
+      <c r="AI149" s="7"/>
+      <c r="AJ149" s="7"/>
+      <c r="AK149" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="150" spans="1:37">
+      <c r="A150" s="3">
+        <v>148</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C150" s="3">
+        <v>2025083342</v>
+      </c>
+      <c r="D150" s="3"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3">
+        <v>2267</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="I150" s="3"/>
+      <c r="J150" s="3"/>
+      <c r="K150" s="3"/>
+      <c r="L150" s="3"/>
+      <c r="M150" s="4"/>
+      <c r="N150" s="3"/>
+      <c r="O150" s="4"/>
+      <c r="P150" s="4"/>
+      <c r="Q150" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="R150" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S150" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T150" s="3">
+        <v>1</v>
+      </c>
+      <c r="U150" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V150" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="W150" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="X150" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="Y150" s="3"/>
+      <c r="Z150" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA150" s="3"/>
+      <c r="AB150" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC150" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD150" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE150" s="3"/>
+      <c r="AF150" s="3"/>
+      <c r="AG150" s="3"/>
+      <c r="AH150" s="3"/>
+      <c r="AI150" s="3"/>
+      <c r="AJ150" s="3"/>
+      <c r="AK150" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Auto commit - 08281246
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$150</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$155</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1066">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-27  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1115">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-28  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3293,12 +3293,85 @@
     <t>撤店</t>
   </si>
   <si>
+    <t>E3796114082701</t>
+  </si>
+  <si>
+    <t>2025-08-27 12:16:23</t>
+  </si>
+  <si>
+    <t>HLL5</t>
+  </si>
+  <si>
+    <t>HL-多卡機TS2000</t>
+  </si>
+  <si>
+    <t>L502</t>
+  </si>
+  <si>
+    <t>無法讀卡</t>
+  </si>
+  <si>
+    <t>門市反應MMK四代機多卡機TS2000無法讀卡，已遠端重啟MMK並測試讀卡仍異常...須請台芝到店協助(無法讀取感應悠遊卡區)</t>
+  </si>
+  <si>
+    <t>2025-08-27 12:22:08</t>
+  </si>
+  <si>
+    <t>2025-08-28 10:02:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 10:32:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 16:22:00</t>
+  </si>
+  <si>
+    <t>更換TS2000多卡機
+換下8184000606
+換上8184001645</t>
+  </si>
+  <si>
     <t>2025-08-27 12:30:02</t>
   </si>
   <si>
     <t>2025-08-27 12:10:00</t>
   </si>
   <si>
+    <t>E4652114082701</t>
+  </si>
+  <si>
+    <t>三重商工店</t>
+  </si>
+  <si>
+    <t>2025-08-27 13:42:00</t>
+  </si>
+  <si>
+    <t>無電源反應、無紅光</t>
+  </si>
+  <si>
+    <t>門市反S應SC CCD掃描器(CLab1070)無電源反應無亮紅光，已有重新拔插線路仍異常...請台芝到店協助(沒有感應無紅光)</t>
+  </si>
+  <si>
+    <t>THILF04652</t>
+  </si>
+  <si>
+    <t>2025-08-27 13:52:55</t>
+  </si>
+  <si>
+    <t>2025-08-28 12:04:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 12:34:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 17:52:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119009822
+換上8119013106</t>
+  </si>
+  <si>
     <t>金山銀山店</t>
   </si>
   <si>
@@ -3321,6 +3394,87 @@
   </si>
   <si>
     <t>2025-08-27 16:05:00</t>
+  </si>
+  <si>
+    <t>14144114082702</t>
+  </si>
+  <si>
+    <t>2025-08-27 18:56:44</t>
+  </si>
+  <si>
+    <t>門市反應LIFE ET熱感機(T70II)無反應，欲更換紙捲時發現出小白單的小門螺絲轉不動無法打開，需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-27 19:00:48</t>
+  </si>
+  <si>
+    <t>2025-08-28 09:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 10:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 23:00:00</t>
+  </si>
+  <si>
+    <t>調整T70小門螺絲 更換紙卷</t>
+  </si>
+  <si>
+    <t>14241114082801</t>
+  </si>
+  <si>
+    <t>2025-08-28 09:04:40</t>
+  </si>
+  <si>
+    <t>門市反應昨日TM2結帳菸品時僅印出空白發票，TM無跳出任何訊息，發票機設備燈號正常，門市發票機為二代(BSC10II)，未操作任何基本排除後續門市點餐紙正常，經HIPOS查看Eventlog無異常，發票檔內有此張發票，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。門市今日08/28又來電反應昨晚仍未列印出發票...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-28 09:07:13</t>
+  </si>
+  <si>
+    <t>2025-08-28 11:04:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 11:34:00</t>
+  </si>
+  <si>
+    <t>2025-08-29 13:07:00</t>
+  </si>
+  <si>
+    <t>檢查測試發票機正常無異狀
+更換發票機
+換下8155004157
+換上8155006318</t>
+  </si>
+  <si>
+    <t>E4341114082801</t>
+  </si>
+  <si>
+    <t>新莊莊美店</t>
+  </si>
+  <si>
+    <t>2025-08-28 08:05:04</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)無法開機，電源燈無亮，已有重新拔插線路仍異常，改換白色插座測試有過電仍無法開機，PING81不通無法VNC...請台芝到店協助 已與門市確認入帳日08/28有交易PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)(TM 無法開機  優游刷卡機無做動)</t>
+  </si>
+  <si>
+    <t>THILF04341</t>
+  </si>
+  <si>
+    <t>2025-08-28 09:12:20</t>
+  </si>
+  <si>
+    <t>2025-08-28 09:22:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 09:52:00</t>
+  </si>
+  <si>
+    <t>2025-08-29 13:12:00</t>
+  </si>
+  <si>
+    <t>變壓器脫落 重接排線</t>
   </si>
 </sst>
 </file>
@@ -3734,10 +3888,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK150"/>
+  <dimension ref="A1:AK155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC147" sqref="AC147"/>
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16501,38 +16655,58 @@
         <v>146</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C148" s="3">
-        <v>2025083311</v>
-      </c>
-      <c r="D148" s="3"/>
-      <c r="E148" s="3"/>
+        <v>2025083309</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F148" s="3">
-        <v>4406</v>
+        <v>3796</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>992</v>
+        <v>469</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="I148" s="3"/>
-      <c r="J148" s="3"/>
-      <c r="K148" s="3"/>
-      <c r="L148" s="3"/>
-      <c r="M148" s="4"/>
-      <c r="N148" s="3"/>
-      <c r="O148" s="4"/>
-      <c r="P148" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L148" s="3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="M148" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="N148" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="O148" s="4" t="s">
+        <v>1061</v>
+      </c>
+      <c r="P148" s="10" t="s">
+        <v>1062</v>
+      </c>
       <c r="Q148" s="3" t="s">
-        <v>996</v>
+        <v>470</v>
       </c>
       <c r="R148" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S148" s="3" t="s">
-        <v>210</v>
+        <v>52</v>
       </c>
       <c r="T148" s="3">
         <v>1</v>
@@ -16541,35 +16715,37 @@
         <v>53</v>
       </c>
       <c r="V148" s="3" t="s">
-        <v>1056</v>
+        <v>1063</v>
       </c>
       <c r="W148" s="3" t="s">
-        <v>1057</v>
+        <v>1064</v>
       </c>
       <c r="X148" s="3" t="s">
-        <v>999</v>
-      </c>
-      <c r="Y148" s="3"/>
+        <v>1065</v>
+      </c>
+      <c r="Y148" s="3" t="s">
+        <v>1066</v>
+      </c>
       <c r="Z148" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA148" s="3"/>
       <c r="AB148" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC148" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD148" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>1067</v>
+      </c>
+      <c r="AD148" s="3"/>
       <c r="AE148" s="3"/>
       <c r="AF148" s="3"/>
       <c r="AG148" s="3"/>
       <c r="AH148" s="3"/>
       <c r="AI148" s="3"/>
       <c r="AJ148" s="3"/>
-      <c r="AK148" s="3"/>
+      <c r="AK148" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="149" spans="1:37">
       <c r="A149" s="7">
@@ -16579,18 +16755,18 @@
         <v>78</v>
       </c>
       <c r="C149" s="7">
-        <v>2025083336</v>
+        <v>2025083311</v>
       </c>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
       <c r="F149" s="7">
-        <v>4906</v>
+        <v>4406</v>
       </c>
       <c r="G149" s="7" t="s">
-        <v>1058</v>
+        <v>992</v>
       </c>
       <c r="H149" s="7" t="s">
-        <v>426</v>
+        <v>206</v>
       </c>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
@@ -16601,13 +16777,13 @@
       <c r="O149" s="8"/>
       <c r="P149" s="9"/>
       <c r="Q149" s="7" t="s">
-        <v>1059</v>
+        <v>996</v>
       </c>
       <c r="R149" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S149" s="7" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="T149" s="7">
         <v>1</v>
@@ -16616,13 +16792,13 @@
         <v>53</v>
       </c>
       <c r="V149" s="7" t="s">
-        <v>1060</v>
+        <v>1068</v>
       </c>
       <c r="W149" s="7" t="s">
-        <v>1061</v>
+        <v>1069</v>
       </c>
       <c r="X149" s="7" t="s">
-        <v>1062</v>
+        <v>999</v>
       </c>
       <c r="Y149" s="7"/>
       <c r="Z149" s="7">
@@ -16644,41 +16820,59 @@
       <c r="AH149" s="7"/>
       <c r="AI149" s="7"/>
       <c r="AJ149" s="7"/>
-      <c r="AK149" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AK149" s="7"/>
     </row>
     <row r="150" spans="1:37">
       <c r="A150" s="3">
         <v>148</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C150" s="3">
-        <v>2025083342</v>
-      </c>
-      <c r="D150" s="3"/>
-      <c r="E150" s="3"/>
+        <v>2025083318</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F150" s="3">
-        <v>2267</v>
+        <v>4652</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>425</v>
+        <v>1071</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="I150" s="3"/>
-      <c r="J150" s="3"/>
-      <c r="K150" s="3"/>
-      <c r="L150" s="3"/>
-      <c r="M150" s="4"/>
-      <c r="N150" s="3"/>
-      <c r="O150" s="4"/>
-      <c r="P150" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L150" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="M150" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="N150" s="3">
+        <v>2902</v>
+      </c>
+      <c r="O150" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="P150" s="10" t="s">
+        <v>1074</v>
+      </c>
       <c r="Q150" s="3" t="s">
-        <v>429</v>
+        <v>1075</v>
       </c>
       <c r="R150" s="3" t="s">
         <v>51</v>
@@ -16693,28 +16887,28 @@
         <v>53</v>
       </c>
       <c r="V150" s="3" t="s">
-        <v>1063</v>
+        <v>1076</v>
       </c>
       <c r="W150" s="3" t="s">
-        <v>1064</v>
+        <v>1077</v>
       </c>
       <c r="X150" s="3" t="s">
-        <v>1065</v>
-      </c>
-      <c r="Y150" s="3"/>
+        <v>1078</v>
+      </c>
+      <c r="Y150" s="3" t="s">
+        <v>1079</v>
+      </c>
       <c r="Z150" s="3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AA150" s="3"/>
       <c r="AB150" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC150" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD150" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC150" s="10" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD150" s="3"/>
       <c r="AE150" s="3"/>
       <c r="AF150" s="3"/>
       <c r="AG150" s="3"/>
@@ -16722,6 +16916,451 @@
       <c r="AI150" s="3"/>
       <c r="AJ150" s="3"/>
       <c r="AK150" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="151" spans="1:37">
+      <c r="A151" s="7">
+        <v>149</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C151" s="7">
+        <v>2025083336</v>
+      </c>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7">
+        <v>4906</v>
+      </c>
+      <c r="G151" s="7" t="s">
+        <v>1081</v>
+      </c>
+      <c r="H151" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="I151" s="7"/>
+      <c r="J151" s="7"/>
+      <c r="K151" s="7"/>
+      <c r="L151" s="7"/>
+      <c r="M151" s="8"/>
+      <c r="N151" s="7"/>
+      <c r="O151" s="8"/>
+      <c r="P151" s="9"/>
+      <c r="Q151" s="7" t="s">
+        <v>1082</v>
+      </c>
+      <c r="R151" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S151" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T151" s="7">
+        <v>1</v>
+      </c>
+      <c r="U151" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V151" s="7" t="s">
+        <v>1083</v>
+      </c>
+      <c r="W151" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="X151" s="7" t="s">
+        <v>1085</v>
+      </c>
+      <c r="Y151" s="7"/>
+      <c r="Z151" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA151" s="7"/>
+      <c r="AB151" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC151" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD151" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE151" s="7"/>
+      <c r="AF151" s="7"/>
+      <c r="AG151" s="7"/>
+      <c r="AH151" s="7"/>
+      <c r="AI151" s="7"/>
+      <c r="AJ151" s="7"/>
+      <c r="AK151" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="152" spans="1:37">
+      <c r="A152" s="3">
+        <v>150</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C152" s="3">
+        <v>2025083342</v>
+      </c>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3">
+        <v>2267</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="I152" s="3"/>
+      <c r="J152" s="3"/>
+      <c r="K152" s="3"/>
+      <c r="L152" s="3"/>
+      <c r="M152" s="4"/>
+      <c r="N152" s="3"/>
+      <c r="O152" s="4"/>
+      <c r="P152" s="10"/>
+      <c r="Q152" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="R152" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S152" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T152" s="3">
+        <v>1</v>
+      </c>
+      <c r="U152" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V152" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="W152" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="X152" s="3" t="s">
+        <v>1088</v>
+      </c>
+      <c r="Y152" s="3"/>
+      <c r="Z152" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA152" s="3"/>
+      <c r="AB152" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC152" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD152" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE152" s="3"/>
+      <c r="AF152" s="3"/>
+      <c r="AG152" s="3"/>
+      <c r="AH152" s="3"/>
+      <c r="AI152" s="3"/>
+      <c r="AJ152" s="3"/>
+      <c r="AK152" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="153" spans="1:37">
+      <c r="A153" s="7">
+        <v>151</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C153" s="7">
+        <v>2025083399</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F153" s="7">
+        <v>4144</v>
+      </c>
+      <c r="G153" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="H153" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I153" s="7" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J153" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="K153" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="L153" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M153" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N153" s="7">
+        <v>5903</v>
+      </c>
+      <c r="O153" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P153" s="9" t="s">
+        <v>1091</v>
+      </c>
+      <c r="Q153" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="R153" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S153" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T153" s="7">
+        <v>1</v>
+      </c>
+      <c r="U153" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V153" s="7" t="s">
+        <v>1092</v>
+      </c>
+      <c r="W153" s="7" t="s">
+        <v>1093</v>
+      </c>
+      <c r="X153" s="7" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Y153" s="7" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Z153" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA153" s="7"/>
+      <c r="AB153" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC153" s="9" t="s">
+        <v>1096</v>
+      </c>
+      <c r="AD153" s="7"/>
+      <c r="AE153" s="7"/>
+      <c r="AF153" s="7"/>
+      <c r="AG153" s="7"/>
+      <c r="AH153" s="7"/>
+      <c r="AI153" s="7"/>
+      <c r="AJ153" s="7"/>
+      <c r="AK153" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="154" spans="1:37">
+      <c r="A154" s="3">
+        <v>152</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C154" s="3">
+        <v>2025083412</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F154" s="3">
+        <v>4241</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>1098</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L154" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M154" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N154" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O154" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="P154" s="10" t="s">
+        <v>1099</v>
+      </c>
+      <c r="Q154" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="R154" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S154" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T154" s="3">
+        <v>1</v>
+      </c>
+      <c r="U154" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V154" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="W154" s="3" t="s">
+        <v>1101</v>
+      </c>
+      <c r="X154" s="3" t="s">
+        <v>1102</v>
+      </c>
+      <c r="Y154" s="3" t="s">
+        <v>1103</v>
+      </c>
+      <c r="Z154" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA154" s="3"/>
+      <c r="AB154" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC154" s="10" t="s">
+        <v>1104</v>
+      </c>
+      <c r="AD154" s="3"/>
+      <c r="AE154" s="3"/>
+      <c r="AF154" s="3"/>
+      <c r="AG154" s="3"/>
+      <c r="AH154" s="3"/>
+      <c r="AI154" s="3"/>
+      <c r="AJ154" s="3"/>
+      <c r="AK154" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155" spans="1:37">
+      <c r="A155" s="7">
+        <v>153</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C155" s="7">
+        <v>2025083418</v>
+      </c>
+      <c r="D155" s="7" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F155" s="7">
+        <v>4341</v>
+      </c>
+      <c r="G155" s="7" t="s">
+        <v>1106</v>
+      </c>
+      <c r="H155" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I155" s="7" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J155" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K155" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L155" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M155" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N155" s="7">
+        <v>2306</v>
+      </c>
+      <c r="O155" s="8" t="s">
+        <v>994</v>
+      </c>
+      <c r="P155" s="8" t="s">
+        <v>1108</v>
+      </c>
+      <c r="Q155" s="7" t="s">
+        <v>1109</v>
+      </c>
+      <c r="R155" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S155" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T155" s="7">
+        <v>1</v>
+      </c>
+      <c r="U155" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V155" s="7" t="s">
+        <v>1110</v>
+      </c>
+      <c r="W155" s="7" t="s">
+        <v>1111</v>
+      </c>
+      <c r="X155" s="7" t="s">
+        <v>1112</v>
+      </c>
+      <c r="Y155" s="7" t="s">
+        <v>1113</v>
+      </c>
+      <c r="Z155" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA155" s="7"/>
+      <c r="AB155" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC155" s="8" t="s">
+        <v>1114</v>
+      </c>
+      <c r="AD155" s="7"/>
+      <c r="AE155" s="7"/>
+      <c r="AF155" s="7"/>
+      <c r="AG155" s="7"/>
+      <c r="AH155" s="7"/>
+      <c r="AI155" s="7"/>
+      <c r="AJ155" s="7"/>
+      <c r="AK155" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08281700
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$155</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$157</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1131">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-28  )</t>
   </si>
@@ -3475,6 +3475,57 @@
   </si>
   <si>
     <t>變壓器脫落 重接排線</t>
+  </si>
+  <si>
+    <t>12109114082802</t>
+  </si>
+  <si>
+    <t>新莊瓊林南</t>
+  </si>
+  <si>
+    <t>2025-08-28 14:17:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應近期TM2熱感發票機(BSC10II)頻繁發生第一筆交易未出發票的異狀，TM無跳出任何訊息，設備燈號正常，未操作任何基本排除後續交易重結打發票出紙正常，hipos查看Eventlog無異常，發票檔內有此張發票，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。
+</t>
+  </si>
+  <si>
+    <t>THILF02109</t>
+  </si>
+  <si>
+    <t>2025-08-28 14:21:14</t>
+  </si>
+  <si>
+    <t>2025-08-28 15:50:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 16:20:00</t>
+  </si>
+  <si>
+    <t>2025-08-29 18:21:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換上8155005388
+換下8155005469</t>
+  </si>
+  <si>
+    <t>三重大榮店</t>
+  </si>
+  <si>
+    <t>THILF02619</t>
+  </si>
+  <si>
+    <t>2025-08-28 15:21:30</t>
+  </si>
+  <si>
+    <t>2025-08-28 14:45:00</t>
+  </si>
+  <si>
+    <t>2025-08-28 15:20:00</t>
+  </si>
+  <si>
+    <t>閉店撤機完成</t>
   </si>
 </sst>
 </file>
@@ -3888,10 +3939,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK155"/>
+  <dimension ref="A1:AK157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A155" sqref="A155"/>
+      <selection activeCell="A157" sqref="A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17313,7 +17364,7 @@
       <c r="O155" s="8" t="s">
         <v>994</v>
       </c>
-      <c r="P155" s="8" t="s">
+      <c r="P155" s="9" t="s">
         <v>1108</v>
       </c>
       <c r="Q155" s="7" t="s">
@@ -17350,7 +17401,7 @@
       <c r="AB155" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC155" s="8" t="s">
+      <c r="AC155" s="9" t="s">
         <v>1114</v>
       </c>
       <c r="AD155" s="7"/>
@@ -17361,6 +17412,180 @@
       <c r="AI155" s="7"/>
       <c r="AJ155" s="7"/>
       <c r="AK155" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="156" spans="1:37">
+      <c r="A156" s="3">
+        <v>154</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C156" s="3">
+        <v>2025083485</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F156" s="3">
+        <v>2109</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="H156" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J156" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K156" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L156" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M156" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N156" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="O156" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P156" s="10" t="s">
+        <v>1118</v>
+      </c>
+      <c r="Q156" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="R156" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S156" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T156" s="3">
+        <v>1</v>
+      </c>
+      <c r="U156" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V156" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="W156" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="X156" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="Y156" s="3" t="s">
+        <v>1123</v>
+      </c>
+      <c r="Z156" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA156" s="3"/>
+      <c r="AB156" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC156" s="10" t="s">
+        <v>1124</v>
+      </c>
+      <c r="AD156" s="3"/>
+      <c r="AE156" s="3"/>
+      <c r="AF156" s="3"/>
+      <c r="AG156" s="3"/>
+      <c r="AH156" s="3"/>
+      <c r="AI156" s="3"/>
+      <c r="AJ156" s="3"/>
+      <c r="AK156" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="157" spans="1:37">
+      <c r="A157" s="7">
+        <v>155</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C157" s="7">
+        <v>2025083500</v>
+      </c>
+      <c r="D157" s="7"/>
+      <c r="E157" s="7"/>
+      <c r="F157" s="7">
+        <v>2619</v>
+      </c>
+      <c r="G157" s="7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="H157" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I157" s="7"/>
+      <c r="J157" s="7"/>
+      <c r="K157" s="7"/>
+      <c r="L157" s="7"/>
+      <c r="M157" s="8"/>
+      <c r="N157" s="7"/>
+      <c r="O157" s="8"/>
+      <c r="P157" s="8"/>
+      <c r="Q157" s="7" t="s">
+        <v>1126</v>
+      </c>
+      <c r="R157" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S157" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T157" s="7">
+        <v>1</v>
+      </c>
+      <c r="U157" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V157" s="7" t="s">
+        <v>1127</v>
+      </c>
+      <c r="W157" s="7" t="s">
+        <v>1128</v>
+      </c>
+      <c r="X157" s="7" t="s">
+        <v>1129</v>
+      </c>
+      <c r="Y157" s="7"/>
+      <c r="Z157" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA157" s="7"/>
+      <c r="AB157" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC157" s="8" t="s">
+        <v>1130</v>
+      </c>
+      <c r="AD157" s="7"/>
+      <c r="AE157" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF157" s="7"/>
+      <c r="AG157" s="7"/>
+      <c r="AH157" s="7"/>
+      <c r="AI157" s="7"/>
+      <c r="AJ157" s="7"/>
+      <c r="AK157" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08291713
</commit_message>
<xml_diff>
--- a/IM/202508_HL_Maintain_Report.xlsx
+++ b/IM/202508_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$157</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$159</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1131">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-28  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1145">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202508   (  製表日期:2025-08-29  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3526,6 +3526,53 @@
   </si>
   <si>
     <t>閉店撤機完成</t>
+  </si>
+  <si>
+    <t>13890114082901</t>
+  </si>
+  <si>
+    <t>2025-08-29 09:07:24</t>
+  </si>
+  <si>
+    <t>門市反應tm1(TCX800)觸控異常鼠標會不斷飄移亂點，vnc查看鼠標飄移閃爍嚴重無法操作觸控校正重啟，門市自行重啟仍異常，台芝於2025-08-21 10:56:00.000將主機電源插座換孔位比且重新矯正螢幕....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-29 09:10:03</t>
+  </si>
+  <si>
+    <t>2025-08-29 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-29 12:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 13:10:00</t>
+  </si>
+  <si>
+    <t>轉為緊急叫修
+更換主機，無更換硬碟
+換下8185000714
+換上8185000630</t>
+  </si>
+  <si>
+    <t>13890114082902</t>
+  </si>
+  <si>
+    <t>2025-08-29 09:19:55</t>
+  </si>
+  <si>
+    <t>08/29 09:19 總公司郁仁來電啟動緊急叫修:門市反應tm1(TCX800)觸控異常鼠標會不斷飄移亂點，vnc查看鼠標飄移閃爍嚴重無法操作觸控校正重啟，門市自行重啟仍異常，台芝於2025-08-21 10:56:00.000將主機電源插座換孔位比且重新矯正螢幕....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-08-29 09:21:50</t>
+  </si>
+  <si>
+    <t>2025-08-29 15:21:00</t>
+  </si>
+  <si>
+    <t>更換主機，無更換硬碟
+換下8185000714
+換上8185000630</t>
   </si>
 </sst>
 </file>
@@ -3939,10 +3986,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK157"/>
+  <dimension ref="A1:AK159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A157" sqref="A157"/>
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17540,7 +17587,7 @@
       <c r="M157" s="8"/>
       <c r="N157" s="7"/>
       <c r="O157" s="8"/>
-      <c r="P157" s="8"/>
+      <c r="P157" s="9"/>
       <c r="Q157" s="7" t="s">
         <v>1126</v>
       </c>
@@ -17573,7 +17620,7 @@
       <c r="AB157" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC157" s="8" t="s">
+      <c r="AC157" s="9" t="s">
         <v>1130</v>
       </c>
       <c r="AD157" s="7"/>
@@ -17586,6 +17633,200 @@
       <c r="AI157" s="7"/>
       <c r="AJ157" s="7"/>
       <c r="AK157" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="158" spans="1:37">
+      <c r="A158" s="3">
+        <v>156</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C158" s="3">
+        <v>2025083584</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F158" s="3">
+        <v>3890</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="H158" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="J158" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K158" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L158" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M158" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="N158" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O158" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="P158" s="10" t="s">
+        <v>1133</v>
+      </c>
+      <c r="Q158" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="R158" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S158" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T158" s="3">
+        <v>1</v>
+      </c>
+      <c r="U158" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V158" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="W158" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="X158" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Y158" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="Z158" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA158" s="3"/>
+      <c r="AB158" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC158" s="10" t="s">
+        <v>1138</v>
+      </c>
+      <c r="AD158" s="3"/>
+      <c r="AE158" s="3"/>
+      <c r="AF158" s="3"/>
+      <c r="AG158" s="3"/>
+      <c r="AH158" s="3"/>
+      <c r="AI158" s="3"/>
+      <c r="AJ158" s="3"/>
+      <c r="AK158" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="159" spans="1:37">
+      <c r="A159" s="7">
+        <v>157</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C159" s="7">
+        <v>2025083585</v>
+      </c>
+      <c r="D159" s="7" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E159" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="F159" s="7">
+        <v>3890</v>
+      </c>
+      <c r="G159" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="H159" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I159" s="7" t="s">
+        <v>1140</v>
+      </c>
+      <c r="J159" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K159" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L159" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M159" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N159" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O159" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="P159" s="8" t="s">
+        <v>1141</v>
+      </c>
+      <c r="Q159" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="R159" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S159" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T159" s="7">
+        <v>1</v>
+      </c>
+      <c r="U159" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V159" s="7" t="s">
+        <v>1142</v>
+      </c>
+      <c r="W159" s="7" t="s">
+        <v>1135</v>
+      </c>
+      <c r="X159" s="7" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Y159" s="7" t="s">
+        <v>1143</v>
+      </c>
+      <c r="Z159" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA159" s="7"/>
+      <c r="AB159" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC159" s="8" t="s">
+        <v>1144</v>
+      </c>
+      <c r="AD159" s="7"/>
+      <c r="AE159" s="7"/>
+      <c r="AF159" s="7"/>
+      <c r="AG159" s="7"/>
+      <c r="AH159" s="7"/>
+      <c r="AI159" s="7"/>
+      <c r="AJ159" s="7"/>
+      <c r="AK159" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>